<commit_message>
update producao and balde - base 03/12/2025
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2025-12.xlsx
+++ b/first-atlas/producao_2025-12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A27899-F3D1-422C-9CFB-9DE3151E872F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A79F91F-1BEE-4C21-9BB2-435F0EFBD8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="377">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -119,9 +119,6 @@
     <t>DISCADOR</t>
   </si>
   <si>
-    <t>PENDÊNCIA DOC</t>
-  </si>
-  <si>
     <t>Jessica Lorenzetto Leme</t>
   </si>
   <si>
@@ -218,54 +215,24 @@
     <t>ANTIMULTAS ZERO PONTO LTDA</t>
   </si>
   <si>
-    <t>73631491000142</t>
-  </si>
-  <si>
-    <t>CRYSLU REPRESENTACOES COMERCIAIS LTDA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Contrato social da empresa GV EMERGENCIAS MEDICAS LTDA, atualizado e registrado no orgao competente, com a devida clausula de administracao. </t>
   </si>
   <si>
     <t>ANÁLISE</t>
   </si>
   <si>
-    <t>62749331000186</t>
-  </si>
-  <si>
-    <t>JULIANA ARISTINA EDUCACAO E DESENVOLVIMENTO INFANTIL LTDA</t>
-  </si>
-  <si>
     <t>21725568000140</t>
   </si>
   <si>
     <t>INFOSERV INFORMATICA E TECNOLOGIA LTDA</t>
   </si>
   <si>
-    <t>62954851000120</t>
-  </si>
-  <si>
-    <t>CSH MARQUEVISKI USINAGEM LTDA</t>
-  </si>
-  <si>
     <t>43813367000137</t>
   </si>
   <si>
     <t>ACTION CRIACAO DIGITAL LTDA</t>
   </si>
   <si>
-    <t>62908692000128</t>
-  </si>
-  <si>
-    <t>EDUARDO EMPREENDIMENTOS LTDA</t>
-  </si>
-  <si>
-    <t>63571942000140</t>
-  </si>
-  <si>
-    <t>F M DE OLIVEIRA METAIS LTDA</t>
-  </si>
-  <si>
     <t>63810792000180</t>
   </si>
   <si>
@@ -278,24 +245,12 @@
     <t>BERGA'S WINE VINHOS E ESPUMANTES LTDA</t>
   </si>
   <si>
-    <t>39580054000109</t>
-  </si>
-  <si>
-    <t>MAURO ROSSIGNOLLI SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
-  </si>
-  <si>
     <t>22579931000129</t>
   </si>
   <si>
     <t>ADRIANO APARECIDO CARLOS 35313802810</t>
   </si>
   <si>
-    <t>22409819000140</t>
-  </si>
-  <si>
-    <t>ELIOMAR RODRIGUES CAIRES DA SILVA</t>
-  </si>
-  <si>
     <t>17220741000180</t>
   </si>
   <si>
@@ -618,6 +573,603 @@
   </si>
   <si>
     <t>BRENO AUGUSTO ARANTES MARANGONI</t>
+  </si>
+  <si>
+    <t>Ainda nao iniciou a abertura de conta</t>
+  </si>
+  <si>
+    <t>62308365000135</t>
+  </si>
+  <si>
+    <t>RESTAURANTE OLIVEIRAS LTDA</t>
+  </si>
+  <si>
+    <t>EL CENTER</t>
+  </si>
+  <si>
+    <t>38715409000248</t>
+  </si>
+  <si>
+    <t>EMBALPLASTI COMERCIO DE DESCARTAVEIS LTDA</t>
+  </si>
+  <si>
+    <t>62342475000113</t>
+  </si>
+  <si>
+    <t>ZAKO ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>39238430000181</t>
+  </si>
+  <si>
+    <t>NORDICA ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>62986727000147</t>
+  </si>
+  <si>
+    <t>JOAO VICTOR SIOTANI PEDROSO</t>
+  </si>
+  <si>
+    <t>Andrey de Souza Batista Bizao</t>
+  </si>
+  <si>
+    <t>BACKOFFICE</t>
+  </si>
+  <si>
+    <t>63553071000131</t>
+  </si>
+  <si>
+    <t>INSTITUTO DE SAUDE ODONTOLOGICA CASSIS LTDA</t>
+  </si>
+  <si>
+    <t>58912816000171</t>
+  </si>
+  <si>
+    <t>Moreira Nery Engenharia LTDA</t>
+  </si>
+  <si>
+    <t>41835655000167</t>
+  </si>
+  <si>
+    <t>ART &amp; MEDIDA MARCENARIA LTDA</t>
+  </si>
+  <si>
+    <t>35396021000152</t>
+  </si>
+  <si>
+    <t>V8 BEER CONVENIENCIA LTDA</t>
+  </si>
+  <si>
+    <t>63802705000142</t>
+  </si>
+  <si>
+    <t>GABRIEL SABINO DE CARVALHO SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>61617157000155</t>
+  </si>
+  <si>
+    <t>RR EMPLACADORA</t>
+  </si>
+  <si>
+    <t>47228236000143</t>
+  </si>
+  <si>
+    <t>MERCADO BUENO COMERCIO DE SECOS E MOLHADOS LTDA</t>
+  </si>
+  <si>
+    <t>17433187000110</t>
+  </si>
+  <si>
+    <t>AGROTILE COMERCIAL LTDA</t>
+  </si>
+  <si>
+    <t>30426419000170</t>
+  </si>
+  <si>
+    <t>ALUMIFER ALUMINIOS LTDA</t>
+  </si>
+  <si>
+    <t>28946269000184</t>
+  </si>
+  <si>
+    <t>ABJ SEMI JOIAS LTDA</t>
+  </si>
+  <si>
+    <t>27305245000183</t>
+  </si>
+  <si>
+    <t>AUDILIEIA STUDIO HAIR LTDA</t>
+  </si>
+  <si>
+    <t>26907715000116</t>
+  </si>
+  <si>
+    <t>ARMANDO SOARES DO AMARAL JUNIOR</t>
+  </si>
+  <si>
+    <t>29264438000169</t>
+  </si>
+  <si>
+    <t>29.264.438 CLAUDIA CRISTINA FRANCELINO</t>
+  </si>
+  <si>
+    <t>27580590000125</t>
+  </si>
+  <si>
+    <t>CLAUDINEY PERPETUO GOMES LACERDA</t>
+  </si>
+  <si>
+    <t>21942534000107</t>
+  </si>
+  <si>
+    <t>GISNELLI BATAGLIA MINCACHE</t>
+  </si>
+  <si>
+    <t>28941420000191</t>
+  </si>
+  <si>
+    <t>A DE SOUZA RABELO</t>
+  </si>
+  <si>
+    <t>27977442000149</t>
+  </si>
+  <si>
+    <t>F F F DA COSTA</t>
+  </si>
+  <si>
+    <t>27869477000164</t>
+  </si>
+  <si>
+    <t>ENTRETONIC LOCACAO E MANUTENCAO ELETRONICA</t>
+  </si>
+  <si>
+    <t>27550116000150</t>
+  </si>
+  <si>
+    <t>27.550.116 DANIELLA SALES RODRIGUES SILVA</t>
+  </si>
+  <si>
+    <t>62777342000170</t>
+  </si>
+  <si>
+    <t>BARRETO ADMINISTRACAO ALVO LTDA</t>
+  </si>
+  <si>
+    <t>28514145000120</t>
+  </si>
+  <si>
+    <t>JOAO BATISTA G J LTDA</t>
+  </si>
+  <si>
+    <t>07062737000188</t>
+  </si>
+  <si>
+    <t>DIGITAL CITY SOLUCOES &amp; INOVACOES CORPORATIVAS LTDA</t>
+  </si>
+  <si>
+    <t>28426910000150</t>
+  </si>
+  <si>
+    <t>GUILHERME ALVES JABOUR</t>
+  </si>
+  <si>
+    <t>63605086000104</t>
+  </si>
+  <si>
+    <t>NEILMA LIMA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>26957390000186</t>
+  </si>
+  <si>
+    <t>GEYLSON B. TAVARES CORRETORA DE SEGUROS</t>
+  </si>
+  <si>
+    <t>54194322000148</t>
+  </si>
+  <si>
+    <t>BOKA DE ALCOOL DISTRIBUIDORA DE BEBIDAS LTDA</t>
+  </si>
+  <si>
+    <t>29227314000103</t>
+  </si>
+  <si>
+    <t>MARCILIO BENICIO COSTA</t>
+  </si>
+  <si>
+    <t>27813272000167</t>
+  </si>
+  <si>
+    <t>ORIENTE DISTRIBUIDORA DE MATERIAIS ELETRICOS LTDA</t>
+  </si>
+  <si>
+    <t>27863097000112</t>
+  </si>
+  <si>
+    <t>ERIC ROBERTO ALEXANDRE DOS REIS</t>
+  </si>
+  <si>
+    <t>29326770000100</t>
+  </si>
+  <si>
+    <t>R&amp;F MANUTENCOES E INSTALACOES ELETRICAS E HIDRAULICAS LTDA</t>
+  </si>
+  <si>
+    <t>27230881000193</t>
+  </si>
+  <si>
+    <t>RODA BRASIL LOCACOES LTDA</t>
+  </si>
+  <si>
+    <t>12012438000179</t>
+  </si>
+  <si>
+    <t>JONAS STEINHAUSER LTDA</t>
+  </si>
+  <si>
+    <t>26936080000185</t>
+  </si>
+  <si>
+    <t>TALITA DOS SANTOS ROCHA</t>
+  </si>
+  <si>
+    <t>27800013000100</t>
+  </si>
+  <si>
+    <t>TALITA EVARISTO DO NASCIMENTO</t>
+  </si>
+  <si>
+    <t>28846385000121</t>
+  </si>
+  <si>
+    <t>28.846.385 PAULO ROBERTO ALVES PORTELA</t>
+  </si>
+  <si>
+    <t>28457220000168</t>
+  </si>
+  <si>
+    <t>28.457.220 UBIRAJARA JOSE TRAVASSOS</t>
+  </si>
+  <si>
+    <t>29749580000104</t>
+  </si>
+  <si>
+    <t>ANEYDE MACIEIRA COSTA</t>
+  </si>
+  <si>
+    <t>29861764000153</t>
+  </si>
+  <si>
+    <t>ADAILTON LIMA DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>30651633000120</t>
+  </si>
+  <si>
+    <t>30.651.633 ANGELITA BRIAN MELO DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>32243005000131</t>
+  </si>
+  <si>
+    <t>ANTONIA LEILIANE FERREIRA DA SILVA</t>
+  </si>
+  <si>
+    <t>31498653000176</t>
+  </si>
+  <si>
+    <t>31.498.653 BRUNA MURIELLY DE GODOI PRAXEDES</t>
+  </si>
+  <si>
+    <t>30937194000117</t>
+  </si>
+  <si>
+    <t>CAMILA MENEZES NERVO</t>
+  </si>
+  <si>
+    <t>30746954000109</t>
+  </si>
+  <si>
+    <t>DEBORAH KAROLINE CABRAL ISIDRO ARAUJO</t>
+  </si>
+  <si>
+    <t>54443402000190</t>
+  </si>
+  <si>
+    <t>CONDOMINIO RESIDENCIAL MONALISA III</t>
+  </si>
+  <si>
+    <t>28214977000120</t>
+  </si>
+  <si>
+    <t>JONATA AVELINO ALCARACA</t>
+  </si>
+  <si>
+    <t>63164433000100</t>
+  </si>
+  <si>
+    <t>ED COMERCIO COSMETICOS LTDA</t>
+  </si>
+  <si>
+    <t>28764259000128</t>
+  </si>
+  <si>
+    <t>28.764.259 CLEITON MICHEL COSTA ALMEIDA</t>
+  </si>
+  <si>
+    <t>30634137000169</t>
+  </si>
+  <si>
+    <t>FERNANDA DIAS DA ROSA MACHADO</t>
+  </si>
+  <si>
+    <t>30003918000155</t>
+  </si>
+  <si>
+    <t>ERLEANE NEVES DA SILVA LTDA</t>
+  </si>
+  <si>
+    <t>63871770000120</t>
+  </si>
+  <si>
+    <t>WB SERVICOS ADIMINISTRATIVOS LTDA</t>
+  </si>
+  <si>
+    <t>Gabrieli Regina Ferreira Lima</t>
+  </si>
+  <si>
+    <t>55134552000184</t>
+  </si>
+  <si>
+    <t>3K STANDS E CENOGRAFIA LTDA</t>
+  </si>
+  <si>
+    <t>27646378000113</t>
+  </si>
+  <si>
+    <t>FRANCISMAR GOMES BARRADAS COMERCIO DE VEICULOS</t>
+  </si>
+  <si>
+    <t>37642166000111</t>
+  </si>
+  <si>
+    <t>FENSTER BURGER LTDA</t>
+  </si>
+  <si>
+    <t>63825932000193</t>
+  </si>
+  <si>
+    <t>MM PROMOCOES DE VENDAS LTDA</t>
+  </si>
+  <si>
+    <t>63720572000165</t>
+  </si>
+  <si>
+    <t>RC FILHO VEICULOS 2026 MULTIMARCAS LTDA</t>
+  </si>
+  <si>
+    <t>30971579000109</t>
+  </si>
+  <si>
+    <t>JOSE WASHINGTON DOS SANTOS JUNIOR</t>
+  </si>
+  <si>
+    <t>63523913000102</t>
+  </si>
+  <si>
+    <t>CASTRO REPRESENTACOES E CONSULTORIA LTDA</t>
+  </si>
+  <si>
+    <t>26836922000127</t>
+  </si>
+  <si>
+    <t>SUATS VIGILANCIA E SEGURANCA LTDA</t>
+  </si>
+  <si>
+    <t>31954483000197</t>
+  </si>
+  <si>
+    <t>NATIELLE MACHADO CORREA</t>
+  </si>
+  <si>
+    <t>59830704000134</t>
+  </si>
+  <si>
+    <t>PEDRO BECKER CORREIA LTDA</t>
+  </si>
+  <si>
+    <t>30789340000104</t>
+  </si>
+  <si>
+    <t>MARCELO DA SILVA COSTA</t>
+  </si>
+  <si>
+    <t>28338110000187</t>
+  </si>
+  <si>
+    <t>NR - COLOMBARI REPRESENTACOES COMERCIAIS LTDA</t>
+  </si>
+  <si>
+    <t>29035039000126</t>
+  </si>
+  <si>
+    <t>BAR PETISCARIA E LANCHONETE ZERO GRAU LTDA</t>
+  </si>
+  <si>
+    <t>63539931000182</t>
+  </si>
+  <si>
+    <t>CAIO COIMBRA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>28656654000197</t>
+  </si>
+  <si>
+    <t>28.656.654 MICHELLE LIMA DA SILVA</t>
+  </si>
+  <si>
+    <t>29096756000168</t>
+  </si>
+  <si>
+    <t>RAISSA BASSANI</t>
+  </si>
+  <si>
+    <t>63377107000173</t>
+  </si>
+  <si>
+    <t>NAPEDRA PIZZARIA LTDA</t>
+  </si>
+  <si>
+    <t>10943668000126</t>
+  </si>
+  <si>
+    <t>LPC MULTI SPORTE BIKE LTDA</t>
+  </si>
+  <si>
+    <t>27546694000113</t>
+  </si>
+  <si>
+    <t>VANDERLEI PROCOPIO</t>
+  </si>
+  <si>
+    <t>60141395000174</t>
+  </si>
+  <si>
+    <t>S E CONSTRUCOES EM GERAL LTDA</t>
+  </si>
+  <si>
+    <t>Felipe Silva</t>
+  </si>
+  <si>
+    <t>28056823000158</t>
+  </si>
+  <si>
+    <t>EDINAVAL C. DA S. SANTOS JUNIOR - LANCHONETE JUNIOR</t>
+  </si>
+  <si>
+    <t>30283213000139</t>
+  </si>
+  <si>
+    <t>R.F. FILHO MOVEIS PERSONALIZADOS</t>
+  </si>
+  <si>
+    <t>27562276000110</t>
+  </si>
+  <si>
+    <t>27.562.276 CARLOS EURIPEDES ROSA JUNIOR</t>
+  </si>
+  <si>
+    <t>60184682000161</t>
+  </si>
+  <si>
+    <t>ALBA TERCEIRIZACOES LTDA</t>
+  </si>
+  <si>
+    <t>29933519000104</t>
+  </si>
+  <si>
+    <t>ALESSANDRO SILVA DE MELO</t>
+  </si>
+  <si>
+    <t>28362825000175</t>
+  </si>
+  <si>
+    <t>JOSE EDUARDO FLORENCIANO INSTALACAO DE MAQUINAS</t>
+  </si>
+  <si>
+    <t>31073254000163</t>
+  </si>
+  <si>
+    <t>EC DE ALMEIDA CARDOSO</t>
+  </si>
+  <si>
+    <t>29003788000171</t>
+  </si>
+  <si>
+    <t>29.003.788 CLOVIS HENRIQUE DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>61189563000164</t>
+  </si>
+  <si>
+    <t>PANIFICADORA GREEN PARK</t>
+  </si>
+  <si>
+    <t>61363098000136</t>
+  </si>
+  <si>
+    <t>RESTAURANTE BAR E LANCHONETE FALCAO LTDA</t>
+  </si>
+  <si>
+    <t>26017859000105</t>
+  </si>
+  <si>
+    <t>J. DE LIMA SEGURANCA E ELETRONICA</t>
+  </si>
+  <si>
+    <t>32199217000169</t>
+  </si>
+  <si>
+    <t>GABRIEL DE OLIVEIRA MELO RANGEL</t>
+  </si>
+  <si>
+    <t>30453410000159</t>
+  </si>
+  <si>
+    <t>WILLIAM ALVES DE SOUZA</t>
+  </si>
+  <si>
+    <t>54975725000124</t>
+  </si>
+  <si>
+    <t>MARIA APARECIDA DA SILVA</t>
+  </si>
+  <si>
+    <t>63761475000110</t>
+  </si>
+  <si>
+    <t>VALE MADEIRAS LTDA</t>
+  </si>
+  <si>
+    <t>22655977000180</t>
+  </si>
+  <si>
+    <t>E A RODRIGUES</t>
+  </si>
+  <si>
+    <t>63634157000199</t>
+  </si>
+  <si>
+    <t>MC MARKET LTDA</t>
+  </si>
+  <si>
+    <t>28264348000105</t>
+  </si>
+  <si>
+    <t>PIPOQUINHA KIDS LTDA</t>
+  </si>
+  <si>
+    <t>63467505000180</t>
+  </si>
+  <si>
+    <t>MAQPATOS LTDA</t>
+  </si>
+  <si>
+    <t>21947763000114</t>
+  </si>
+  <si>
+    <t>TERRITORIO TATICO  CENTRO DE FORMACAO E SERVICOS MECANICOS LTDA</t>
+  </si>
+  <si>
+    <t>63542643000187</t>
+  </si>
+  <si>
+    <t>LARA CONDE PSICOLOGIA LTDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procuracao com poderes para abrir e movimentar contas, pois identificamos que a representacao da sua empresa deve ser em conjunto pelos socios,  A procuracao deve ser assinada digitalmente pelos socios pela plataforma "GOV." e estar em formato PDF.&lt;br&gt;&lt;br&gt;Para garantir a seguranca e a validade do processo, Pedimos gentilmente que envie uma nova selfie, conforme as orientacoes </t>
   </si>
 </sst>
 </file>
@@ -989,10 +1541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCD3CE2-DBA2-4F4F-B6A3-11EE884EA727}">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,7 +1573,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1029,10 +1581,10 @@
         <v>45992</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -1052,10 +1604,10 @@
         <v>45992</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1064,10 +1616,10 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1075,10 +1627,10 @@
         <v>45992</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -1098,10 +1650,10 @@
         <v>45992</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
         <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -1110,10 +1662,10 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1121,19 +1673,19 @@
         <v>45992</v>
       </c>
       <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1144,10 +1696,10 @@
         <v>45992</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
         <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -1156,7 +1708,7 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1167,10 +1719,10 @@
         <v>45992</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1179,7 +1731,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1190,10 +1742,10 @@
         <v>45992</v>
       </c>
       <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1202,7 +1754,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1213,22 +1765,22 @@
         <v>45992</v>
       </c>
       <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
-        <v>56</v>
-      </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="G10" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1236,10 +1788,10 @@
         <v>45992</v>
       </c>
       <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
         <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>58</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -1248,7 +1800,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1259,19 +1811,19 @@
         <v>45992</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1282,19 +1834,19 @@
         <v>45992</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1305,19 +1857,19 @@
         <v>45992</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1328,19 +1880,19 @@
         <v>45992</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1351,19 +1903,19 @@
         <v>45992</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1374,19 +1926,19 @@
         <v>45992</v>
       </c>
       <c r="B17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
-        <v>70</v>
-      </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1397,13 +1949,13 @@
         <v>45992</v>
       </c>
       <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
         <v>71</v>
       </c>
-      <c r="C18" t="s">
-        <v>72</v>
-      </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -1420,13 +1972,13 @@
         <v>45992</v>
       </c>
       <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
         <v>73</v>
       </c>
-      <c r="C19" t="s">
-        <v>74</v>
-      </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -1443,19 +1995,19 @@
         <v>45992</v>
       </c>
       <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
         <v>75</v>
       </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1466,16 +2018,16 @@
         <v>45992</v>
       </c>
       <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
         <v>77</v>
       </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
@@ -1489,19 +2041,19 @@
         <v>45992</v>
       </c>
       <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
         <v>79</v>
       </c>
-      <c r="C22" t="s">
-        <v>80</v>
-      </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1512,10 +2064,10 @@
         <v>45992</v>
       </c>
       <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
         <v>81</v>
-      </c>
-      <c r="C23" t="s">
-        <v>82</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -1524,7 +2076,7 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1535,16 +2087,16 @@
         <v>45992</v>
       </c>
       <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
@@ -1558,13 +2110,13 @@
         <v>45992</v>
       </c>
       <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
         <v>85</v>
       </c>
-      <c r="C25" t="s">
-        <v>86</v>
-      </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E25" t="s">
         <v>7</v>
@@ -1581,13 +2133,13 @@
         <v>45992</v>
       </c>
       <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
         <v>87</v>
       </c>
-      <c r="C26" t="s">
-        <v>88</v>
-      </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -1604,19 +2156,19 @@
         <v>45992</v>
       </c>
       <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
         <v>89</v>
       </c>
-      <c r="C27" t="s">
-        <v>90</v>
-      </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1627,19 +2179,19 @@
         <v>45992</v>
       </c>
       <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" t="s">
         <v>91</v>
       </c>
-      <c r="C28" t="s">
-        <v>92</v>
-      </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E28" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1650,19 +2202,19 @@
         <v>45992</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1673,19 +2225,19 @@
         <v>45992</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1696,19 +2248,19 @@
         <v>45992</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E31" t="s">
         <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1719,13 +2271,13 @@
         <v>45992</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
@@ -1742,10 +2294,10 @@
         <v>45992</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -1765,19 +2317,19 @@
         <v>45992</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1788,19 +2340,19 @@
         <v>45992</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -1811,16 +2363,16 @@
         <v>45992</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
         <v>22</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -1834,16 +2386,16 @@
         <v>45992</v>
       </c>
       <c r="B37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
         <v>107</v>
       </c>
-      <c r="C37" t="s">
-        <v>108</v>
-      </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -1857,19 +2409,19 @@
         <v>45992</v>
       </c>
       <c r="B38" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" t="s">
         <v>109</v>
       </c>
-      <c r="C38" t="s">
-        <v>110</v>
-      </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1880,13 +2432,13 @@
         <v>45992</v>
       </c>
       <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s">
         <v>111</v>
       </c>
-      <c r="C39" t="s">
-        <v>112</v>
-      </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
         <v>7</v>
@@ -1903,19 +2455,19 @@
         <v>45992</v>
       </c>
       <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" t="s">
         <v>113</v>
       </c>
-      <c r="C40" t="s">
-        <v>114</v>
-      </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E40" t="s">
         <v>7</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -1926,13 +2478,13 @@
         <v>45992</v>
       </c>
       <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
         <v>115</v>
       </c>
-      <c r="C41" t="s">
-        <v>116</v>
-      </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
         <v>7</v>
@@ -1949,13 +2501,13 @@
         <v>45992</v>
       </c>
       <c r="B42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" t="s">
         <v>117</v>
       </c>
-      <c r="C42" t="s">
-        <v>118</v>
-      </c>
       <c r="D42" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E42" t="s">
         <v>7</v>
@@ -1972,16 +2524,16 @@
         <v>45992</v>
       </c>
       <c r="B43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" t="s">
         <v>119</v>
       </c>
-      <c r="C43" t="s">
-        <v>120</v>
-      </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
@@ -1995,16 +2547,16 @@
         <v>45992</v>
       </c>
       <c r="B44" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" t="s">
         <v>121</v>
       </c>
-      <c r="C44" t="s">
-        <v>122</v>
-      </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F44" t="s">
         <v>15</v>
@@ -2018,16 +2570,16 @@
         <v>45992</v>
       </c>
       <c r="B45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" t="s">
         <v>123</v>
       </c>
-      <c r="C45" t="s">
-        <v>124</v>
-      </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F45" t="s">
         <v>15</v>
@@ -2041,16 +2593,16 @@
         <v>45992</v>
       </c>
       <c r="B46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" t="s">
         <v>125</v>
       </c>
-      <c r="C46" t="s">
-        <v>126</v>
-      </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F46" t="s">
         <v>15</v>
@@ -2064,19 +2616,19 @@
         <v>45992</v>
       </c>
       <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" t="s">
         <v>127</v>
       </c>
-      <c r="C47" t="s">
-        <v>128</v>
-      </c>
       <c r="D47" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E47" t="s">
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2087,19 +2639,19 @@
         <v>45992</v>
       </c>
       <c r="B48" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" t="s">
         <v>129</v>
       </c>
-      <c r="C48" t="s">
-        <v>130</v>
-      </c>
       <c r="D48" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2110,10 +2662,10 @@
         <v>45992</v>
       </c>
       <c r="B49" t="s">
+        <v>130</v>
+      </c>
+      <c r="C49" t="s">
         <v>131</v>
-      </c>
-      <c r="C49" t="s">
-        <v>132</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
@@ -2122,7 +2674,7 @@
         <v>7</v>
       </c>
       <c r="F49" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2133,13 +2685,13 @@
         <v>45992</v>
       </c>
       <c r="B50" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" t="s">
         <v>133</v>
       </c>
-      <c r="C50" t="s">
-        <v>134</v>
-      </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E50" t="s">
         <v>7</v>
@@ -2156,16 +2708,16 @@
         <v>45992</v>
       </c>
       <c r="B51" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" t="s">
         <v>135</v>
       </c>
-      <c r="C51" t="s">
-        <v>136</v>
-      </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E51" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F51" t="s">
         <v>15</v>
@@ -2179,16 +2731,16 @@
         <v>45992</v>
       </c>
       <c r="B52" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" t="s">
         <v>137</v>
       </c>
-      <c r="C52" t="s">
-        <v>138</v>
-      </c>
       <c r="D52" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F52" t="s">
         <v>15</v>
@@ -2202,22 +2754,22 @@
         <v>45992</v>
       </c>
       <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
         <v>139</v>
       </c>
-      <c r="C53" t="s">
-        <v>140</v>
-      </c>
       <c r="D53" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E53" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F53" t="s">
-        <v>15</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="G53" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2225,10 +2777,10 @@
         <v>45992</v>
       </c>
       <c r="B54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" t="s">
         <v>141</v>
-      </c>
-      <c r="C54" t="s">
-        <v>142</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -2248,10 +2800,10 @@
         <v>45992</v>
       </c>
       <c r="B55" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" t="s">
         <v>143</v>
-      </c>
-      <c r="C55" t="s">
-        <v>144</v>
       </c>
       <c r="D55" t="s">
         <v>13</v>
@@ -2260,7 +2812,7 @@
         <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>62</v>
+        <v>178</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2271,19 +2823,19 @@
         <v>45992</v>
       </c>
       <c r="B56" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" t="s">
         <v>145</v>
       </c>
-      <c r="C56" t="s">
-        <v>146</v>
-      </c>
       <c r="D56" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E56" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F56" t="s">
-        <v>8</v>
+        <v>178</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2294,16 +2846,16 @@
         <v>45992</v>
       </c>
       <c r="B57" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" t="s">
         <v>147</v>
       </c>
-      <c r="C57" t="s">
-        <v>148</v>
-      </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F57" t="s">
         <v>15</v>
@@ -2317,16 +2869,16 @@
         <v>45992</v>
       </c>
       <c r="B58" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" t="s">
         <v>149</v>
       </c>
-      <c r="C58" t="s">
-        <v>150</v>
-      </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E58" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F58" t="s">
         <v>15</v>
@@ -2340,19 +2892,19 @@
         <v>45992</v>
       </c>
       <c r="B59" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" t="s">
         <v>151</v>
       </c>
-      <c r="C59" t="s">
-        <v>152</v>
-      </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E59" t="s">
         <v>14</v>
       </c>
       <c r="F59" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2363,10 +2915,10 @@
         <v>45992</v>
       </c>
       <c r="B60" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" t="s">
         <v>153</v>
-      </c>
-      <c r="C60" t="s">
-        <v>154</v>
       </c>
       <c r="D60" t="s">
         <v>19</v>
@@ -2375,10 +2927,10 @@
         <v>7</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
-      </c>
-      <c r="G60" t="s">
-        <v>35</v>
+        <v>59</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2386,10 +2938,10 @@
         <v>45992</v>
       </c>
       <c r="B61" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" t="s">
         <v>155</v>
-      </c>
-      <c r="C61" t="s">
-        <v>156</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -2409,19 +2961,19 @@
         <v>45992</v>
       </c>
       <c r="B62" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" t="s">
         <v>157</v>
       </c>
-      <c r="C62" t="s">
-        <v>158</v>
-      </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F62" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2432,19 +2984,19 @@
         <v>45992</v>
       </c>
       <c r="B63" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" t="s">
         <v>159</v>
       </c>
-      <c r="C63" t="s">
-        <v>160</v>
-      </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F63" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2455,19 +3007,19 @@
         <v>45992</v>
       </c>
       <c r="B64" t="s">
+        <v>160</v>
+      </c>
+      <c r="C64" t="s">
         <v>161</v>
-      </c>
-      <c r="C64" t="s">
-        <v>162</v>
       </c>
       <c r="D64" t="s">
         <v>27</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F64" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -2478,13 +3030,13 @@
         <v>45992</v>
       </c>
       <c r="B65" t="s">
+        <v>162</v>
+      </c>
+      <c r="C65" t="s">
         <v>163</v>
       </c>
-      <c r="C65" t="s">
-        <v>164</v>
-      </c>
       <c r="D65" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E65" t="s">
         <v>7</v>
@@ -2501,19 +3053,19 @@
         <v>45992</v>
       </c>
       <c r="B66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" t="s">
         <v>165</v>
       </c>
-      <c r="C66" t="s">
-        <v>166</v>
-      </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F66" t="s">
-        <v>62</v>
+        <v>178</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2524,19 +3076,19 @@
         <v>45992</v>
       </c>
       <c r="B67" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" t="s">
         <v>167</v>
       </c>
-      <c r="C67" t="s">
-        <v>168</v>
-      </c>
       <c r="D67" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F67" t="s">
-        <v>62</v>
+        <v>178</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -2547,13 +3099,13 @@
         <v>45992</v>
       </c>
       <c r="B68" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" t="s">
         <v>169</v>
       </c>
-      <c r="C68" t="s">
-        <v>170</v>
-      </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E68" t="s">
         <v>7</v>
@@ -2570,13 +3122,13 @@
         <v>45992</v>
       </c>
       <c r="B69" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" t="s">
         <v>171</v>
       </c>
-      <c r="C69" t="s">
-        <v>172</v>
-      </c>
       <c r="D69" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E69" t="s">
         <v>7</v>
@@ -2593,19 +3145,19 @@
         <v>45992</v>
       </c>
       <c r="B70" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" t="s">
         <v>173</v>
       </c>
-      <c r="C70" t="s">
-        <v>174</v>
-      </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E70" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F70" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2616,16 +3168,16 @@
         <v>45992</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>43</v>
       </c>
       <c r="C71" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="D71" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E71" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F71" t="s">
         <v>15</v>
@@ -2639,13 +3191,13 @@
         <v>45992</v>
       </c>
       <c r="B72" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C72" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D72" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
@@ -2662,19 +3214,19 @@
         <v>45992</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C73" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D73" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
       </c>
       <c r="F73" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -2685,19 +3237,19 @@
         <v>45992</v>
       </c>
       <c r="B74" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" t="s">
         <v>181</v>
-      </c>
-      <c r="C74" t="s">
-        <v>182</v>
-      </c>
-      <c r="D74" t="s">
-        <v>23</v>
       </c>
       <c r="E74" t="s">
         <v>25</v>
       </c>
       <c r="F74" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -2708,16 +3260,16 @@
         <v>45992</v>
       </c>
       <c r="B75" t="s">
+        <v>182</v>
+      </c>
+      <c r="C75" t="s">
         <v>183</v>
       </c>
-      <c r="C75" t="s">
-        <v>184</v>
-      </c>
       <c r="D75" t="s">
-        <v>19</v>
+        <v>181</v>
       </c>
       <c r="E75" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F75" t="s">
         <v>15</v>
@@ -2731,16 +3283,16 @@
         <v>45992</v>
       </c>
       <c r="B76" t="s">
+        <v>184</v>
+      </c>
+      <c r="C76" t="s">
         <v>185</v>
       </c>
-      <c r="C76" t="s">
-        <v>186</v>
-      </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>181</v>
       </c>
       <c r="E76" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F76" t="s">
         <v>15</v>
@@ -2754,16 +3306,16 @@
         <v>45992</v>
       </c>
       <c r="B77" t="s">
+        <v>186</v>
+      </c>
+      <c r="C77" t="s">
         <v>187</v>
       </c>
-      <c r="C77" t="s">
-        <v>188</v>
-      </c>
       <c r="D77" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="E77" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F77" t="s">
         <v>15</v>
@@ -2774,19 +3326,19 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="B78" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="C78" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="D78" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="E78" t="s">
-        <v>7</v>
+        <v>191</v>
       </c>
       <c r="F78" t="s">
         <v>15</v>
@@ -2797,19 +3349,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="B79" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C79" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D79" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E79" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F79" t="s">
         <v>15</v>
@@ -2820,24 +3372,2071 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>45992</v>
+        <v>45993</v>
       </c>
       <c r="B80" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="C80" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D80" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" t="s">
+        <v>15</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B81" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" t="s">
+        <v>197</v>
+      </c>
+      <c r="D81" t="s">
+        <v>20</v>
+      </c>
+      <c r="E81" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B82" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" t="s">
+        <v>199</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82" t="s">
+        <v>15</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B83" t="s">
+        <v>200</v>
+      </c>
+      <c r="C83" t="s">
+        <v>201</v>
+      </c>
+      <c r="D83" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" t="s">
+        <v>15</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B84" t="s">
+        <v>202</v>
+      </c>
+      <c r="C84" t="s">
+        <v>203</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B85" t="s">
+        <v>204</v>
+      </c>
+      <c r="C85" t="s">
+        <v>205</v>
+      </c>
+      <c r="D85" t="s">
+        <v>10</v>
+      </c>
+      <c r="E85" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" t="s">
+        <v>59</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B86" t="s">
+        <v>206</v>
+      </c>
+      <c r="C86" t="s">
+        <v>207</v>
+      </c>
+      <c r="D86" t="s">
+        <v>23</v>
+      </c>
+      <c r="E86" t="s">
+        <v>7</v>
+      </c>
+      <c r="F86" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B87" t="s">
+        <v>208</v>
+      </c>
+      <c r="C87" t="s">
+        <v>209</v>
+      </c>
+      <c r="D87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87" t="s">
+        <v>15</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B88" t="s">
+        <v>210</v>
+      </c>
+      <c r="C88" t="s">
+        <v>211</v>
+      </c>
+      <c r="D88" t="s">
+        <v>20</v>
+      </c>
+      <c r="E88" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88" t="s">
+        <v>15</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B89" t="s">
+        <v>212</v>
+      </c>
+      <c r="C89" t="s">
+        <v>213</v>
+      </c>
+      <c r="D89" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89" t="s">
+        <v>59</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B90" t="s">
+        <v>214</v>
+      </c>
+      <c r="C90" t="s">
+        <v>215</v>
+      </c>
+      <c r="D90" t="s">
+        <v>19</v>
+      </c>
+      <c r="E90" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90" t="s">
+        <v>15</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B91" t="s">
+        <v>216</v>
+      </c>
+      <c r="C91" t="s">
+        <v>217</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91" t="s">
+        <v>15</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C92" t="s">
+        <v>219</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92" t="s">
+        <v>15</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B93" t="s">
+        <v>220</v>
+      </c>
+      <c r="C93" t="s">
+        <v>221</v>
+      </c>
+      <c r="D93" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93" t="s">
+        <v>15</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B94" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" t="s">
+        <v>223</v>
+      </c>
+      <c r="D94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B95" t="s">
+        <v>224</v>
+      </c>
+      <c r="C95" t="s">
+        <v>225</v>
+      </c>
+      <c r="D95" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" t="s">
+        <v>7</v>
+      </c>
+      <c r="F95" t="s">
+        <v>15</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B96" t="s">
+        <v>226</v>
+      </c>
+      <c r="C96" t="s">
+        <v>227</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" t="s">
+        <v>7</v>
+      </c>
+      <c r="F96" t="s">
+        <v>15</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B97" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" t="s">
+        <v>229</v>
+      </c>
+      <c r="D97" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" t="s">
+        <v>7</v>
+      </c>
+      <c r="F97" t="s">
+        <v>15</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B98" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" t="s">
+        <v>231</v>
+      </c>
+      <c r="D98" t="s">
+        <v>27</v>
+      </c>
+      <c r="E98" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" t="s">
+        <v>15</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B99" t="s">
+        <v>232</v>
+      </c>
+      <c r="C99" t="s">
+        <v>233</v>
+      </c>
+      <c r="D99" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" t="s">
+        <v>15</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B100" t="s">
+        <v>234</v>
+      </c>
+      <c r="C100" t="s">
+        <v>235</v>
+      </c>
+      <c r="D100" t="s">
+        <v>20</v>
+      </c>
+      <c r="E100" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100" t="s">
+        <v>15</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B101" t="s">
+        <v>236</v>
+      </c>
+      <c r="C101" t="s">
+        <v>237</v>
+      </c>
+      <c r="D101" t="s">
+        <v>20</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101" t="s">
+        <v>15</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B102" t="s">
+        <v>238</v>
+      </c>
+      <c r="C102" t="s">
+        <v>239</v>
+      </c>
+      <c r="D102" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" t="s">
+        <v>25</v>
+      </c>
+      <c r="F102" t="s">
+        <v>59</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B103" t="s">
+        <v>240</v>
+      </c>
+      <c r="C103" t="s">
+        <v>241</v>
+      </c>
+      <c r="D103" t="s">
+        <v>17</v>
+      </c>
+      <c r="E103" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103" t="s">
+        <v>15</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B104" t="s">
+        <v>242</v>
+      </c>
+      <c r="C104" t="s">
+        <v>243</v>
+      </c>
+      <c r="D104" t="s">
+        <v>19</v>
+      </c>
+      <c r="E104" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" t="s">
+        <v>15</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B105" t="s">
+        <v>244</v>
+      </c>
+      <c r="C105" t="s">
+        <v>245</v>
+      </c>
+      <c r="D105" t="s">
+        <v>23</v>
+      </c>
+      <c r="E105" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105" t="s">
+        <v>8</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B106" t="s">
+        <v>246</v>
+      </c>
+      <c r="C106" t="s">
+        <v>247</v>
+      </c>
+      <c r="D106" t="s">
+        <v>27</v>
+      </c>
+      <c r="E106" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" t="s">
+        <v>15</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B107" t="s">
+        <v>248</v>
+      </c>
+      <c r="C107" t="s">
+        <v>249</v>
+      </c>
+      <c r="D107" t="s">
+        <v>22</v>
+      </c>
+      <c r="E107" t="s">
+        <v>7</v>
+      </c>
+      <c r="F107" t="s">
+        <v>15</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B108" t="s">
+        <v>250</v>
+      </c>
+      <c r="C108" t="s">
+        <v>251</v>
+      </c>
+      <c r="D108" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" t="s">
+        <v>7</v>
+      </c>
+      <c r="F108" t="s">
+        <v>8</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B109" t="s">
+        <v>252</v>
+      </c>
+      <c r="C109" t="s">
+        <v>253</v>
+      </c>
+      <c r="D109" t="s">
+        <v>20</v>
+      </c>
+      <c r="E109" t="s">
+        <v>7</v>
+      </c>
+      <c r="F109" t="s">
+        <v>15</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B110" t="s">
+        <v>254</v>
+      </c>
+      <c r="C110" t="s">
+        <v>255</v>
+      </c>
+      <c r="D110" t="s">
         <v>13</v>
       </c>
-      <c r="E80" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" t="s">
-        <v>15</v>
-      </c>
-      <c r="G80">
+      <c r="E110" t="s">
+        <v>7</v>
+      </c>
+      <c r="F110" t="s">
+        <v>8</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B111" t="s">
+        <v>256</v>
+      </c>
+      <c r="C111" t="s">
+        <v>257</v>
+      </c>
+      <c r="D111" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" t="s">
+        <v>7</v>
+      </c>
+      <c r="F111" t="s">
+        <v>15</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B112" t="s">
+        <v>258</v>
+      </c>
+      <c r="C112" t="s">
+        <v>259</v>
+      </c>
+      <c r="D112" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112" t="s">
+        <v>7</v>
+      </c>
+      <c r="F112" t="s">
+        <v>8</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B113" t="s">
+        <v>260</v>
+      </c>
+      <c r="C113" t="s">
+        <v>261</v>
+      </c>
+      <c r="D113" t="s">
+        <v>10</v>
+      </c>
+      <c r="E113" t="s">
+        <v>7</v>
+      </c>
+      <c r="F113" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B114" t="s">
+        <v>262</v>
+      </c>
+      <c r="C114" t="s">
+        <v>263</v>
+      </c>
+      <c r="D114" t="s">
+        <v>22</v>
+      </c>
+      <c r="E114" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114" t="s">
+        <v>8</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B115" t="s">
+        <v>264</v>
+      </c>
+      <c r="C115" t="s">
+        <v>265</v>
+      </c>
+      <c r="D115" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115" t="s">
+        <v>15</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B116" t="s">
+        <v>266</v>
+      </c>
+      <c r="C116" t="s">
+        <v>267</v>
+      </c>
+      <c r="D116" t="s">
+        <v>17</v>
+      </c>
+      <c r="E116" t="s">
+        <v>7</v>
+      </c>
+      <c r="F116" t="s">
+        <v>15</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B117" t="s">
+        <v>268</v>
+      </c>
+      <c r="C117" t="s">
+        <v>269</v>
+      </c>
+      <c r="D117" t="s">
+        <v>10</v>
+      </c>
+      <c r="E117" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117" t="s">
+        <v>15</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B118" t="s">
+        <v>270</v>
+      </c>
+      <c r="C118" t="s">
+        <v>271</v>
+      </c>
+      <c r="D118" t="s">
+        <v>19</v>
+      </c>
+      <c r="E118" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" t="s">
+        <v>15</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B119" t="s">
+        <v>272</v>
+      </c>
+      <c r="C119" t="s">
+        <v>273</v>
+      </c>
+      <c r="D119" t="s">
+        <v>27</v>
+      </c>
+      <c r="E119" t="s">
+        <v>7</v>
+      </c>
+      <c r="F119" t="s">
+        <v>15</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B120" t="s">
+        <v>274</v>
+      </c>
+      <c r="C120" t="s">
+        <v>275</v>
+      </c>
+      <c r="D120" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" t="s">
+        <v>7</v>
+      </c>
+      <c r="F120" t="s">
+        <v>8</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B121" t="s">
+        <v>276</v>
+      </c>
+      <c r="C121" t="s">
+        <v>277</v>
+      </c>
+      <c r="D121" t="s">
+        <v>17</v>
+      </c>
+      <c r="E121" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121" t="s">
+        <v>15</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B122" t="s">
+        <v>278</v>
+      </c>
+      <c r="C122" t="s">
+        <v>279</v>
+      </c>
+      <c r="D122" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122" t="s">
+        <v>7</v>
+      </c>
+      <c r="F122" t="s">
+        <v>59</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B123" t="s">
+        <v>280</v>
+      </c>
+      <c r="C123" t="s">
+        <v>281</v>
+      </c>
+      <c r="D123" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" t="s">
+        <v>7</v>
+      </c>
+      <c r="F123" t="s">
+        <v>15</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B124" t="s">
+        <v>282</v>
+      </c>
+      <c r="C124" t="s">
+        <v>283</v>
+      </c>
+      <c r="D124" t="s">
+        <v>22</v>
+      </c>
+      <c r="E124" t="s">
+        <v>7</v>
+      </c>
+      <c r="F124" t="s">
+        <v>59</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B125" t="s">
+        <v>284</v>
+      </c>
+      <c r="C125" t="s">
+        <v>285</v>
+      </c>
+      <c r="D125" t="s">
+        <v>19</v>
+      </c>
+      <c r="E125" t="s">
+        <v>7</v>
+      </c>
+      <c r="F125" t="s">
+        <v>15</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B126" t="s">
+        <v>286</v>
+      </c>
+      <c r="C126" t="s">
+        <v>287</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" t="s">
+        <v>7</v>
+      </c>
+      <c r="F126" t="s">
+        <v>15</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B127" t="s">
+        <v>288</v>
+      </c>
+      <c r="C127" t="s">
+        <v>289</v>
+      </c>
+      <c r="D127" t="s">
+        <v>19</v>
+      </c>
+      <c r="E127" t="s">
+        <v>7</v>
+      </c>
+      <c r="F127" t="s">
+        <v>8</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B128" t="s">
+        <v>290</v>
+      </c>
+      <c r="C128" t="s">
+        <v>291</v>
+      </c>
+      <c r="D128" t="s">
+        <v>292</v>
+      </c>
+      <c r="E128" t="s">
+        <v>25</v>
+      </c>
+      <c r="F128" t="s">
+        <v>15</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B129" t="s">
+        <v>293</v>
+      </c>
+      <c r="C129" t="s">
+        <v>294</v>
+      </c>
+      <c r="D129" t="s">
+        <v>16</v>
+      </c>
+      <c r="E129" t="s">
+        <v>7</v>
+      </c>
+      <c r="F129" t="s">
+        <v>15</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B130" t="s">
+        <v>295</v>
+      </c>
+      <c r="C130" t="s">
+        <v>296</v>
+      </c>
+      <c r="D130" t="s">
+        <v>23</v>
+      </c>
+      <c r="E130" t="s">
+        <v>7</v>
+      </c>
+      <c r="F130" t="s">
+        <v>8</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B131" t="s">
+        <v>297</v>
+      </c>
+      <c r="C131" t="s">
+        <v>298</v>
+      </c>
+      <c r="D131" t="s">
+        <v>16</v>
+      </c>
+      <c r="E131" t="s">
+        <v>7</v>
+      </c>
+      <c r="F131" t="s">
+        <v>15</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B132" t="s">
+        <v>299</v>
+      </c>
+      <c r="C132" t="s">
+        <v>300</v>
+      </c>
+      <c r="D132" t="s">
+        <v>292</v>
+      </c>
+      <c r="E132" t="s">
+        <v>25</v>
+      </c>
+      <c r="F132" t="s">
+        <v>8</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B133" t="s">
+        <v>301</v>
+      </c>
+      <c r="C133" t="s">
+        <v>302</v>
+      </c>
+      <c r="D133" t="s">
+        <v>11</v>
+      </c>
+      <c r="E133" t="s">
+        <v>25</v>
+      </c>
+      <c r="F133" t="s">
+        <v>15</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B134" t="s">
+        <v>303</v>
+      </c>
+      <c r="C134" t="s">
+        <v>304</v>
+      </c>
+      <c r="D134" t="s">
+        <v>23</v>
+      </c>
+      <c r="E134" t="s">
+        <v>7</v>
+      </c>
+      <c r="F134" t="s">
+        <v>15</v>
+      </c>
+      <c r="G134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B135" t="s">
+        <v>305</v>
+      </c>
+      <c r="C135" t="s">
+        <v>306</v>
+      </c>
+      <c r="D135" t="s">
+        <v>292</v>
+      </c>
+      <c r="E135" t="s">
+        <v>25</v>
+      </c>
+      <c r="F135" t="s">
+        <v>15</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B136" t="s">
+        <v>307</v>
+      </c>
+      <c r="C136" t="s">
+        <v>308</v>
+      </c>
+      <c r="D136" t="s">
+        <v>6</v>
+      </c>
+      <c r="E136" t="s">
+        <v>7</v>
+      </c>
+      <c r="F136" t="s">
+        <v>15</v>
+      </c>
+      <c r="G136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B137" t="s">
+        <v>309</v>
+      </c>
+      <c r="C137" t="s">
+        <v>310</v>
+      </c>
+      <c r="D137" t="s">
+        <v>10</v>
+      </c>
+      <c r="E137" t="s">
+        <v>7</v>
+      </c>
+      <c r="F137" t="s">
+        <v>8</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B138" t="s">
+        <v>311</v>
+      </c>
+      <c r="C138" t="s">
+        <v>312</v>
+      </c>
+      <c r="D138" t="s">
+        <v>22</v>
+      </c>
+      <c r="E138" t="s">
+        <v>7</v>
+      </c>
+      <c r="F138" t="s">
+        <v>15</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B139" t="s">
+        <v>313</v>
+      </c>
+      <c r="C139" t="s">
+        <v>314</v>
+      </c>
+      <c r="D139" t="s">
+        <v>23</v>
+      </c>
+      <c r="E139" t="s">
+        <v>7</v>
+      </c>
+      <c r="F139" t="s">
+        <v>15</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B140" t="s">
+        <v>315</v>
+      </c>
+      <c r="C140" t="s">
+        <v>316</v>
+      </c>
+      <c r="D140" t="s">
+        <v>16</v>
+      </c>
+      <c r="E140" t="s">
+        <v>7</v>
+      </c>
+      <c r="F140" t="s">
+        <v>15</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B141" t="s">
+        <v>317</v>
+      </c>
+      <c r="C141" t="s">
+        <v>318</v>
+      </c>
+      <c r="D141" t="s">
+        <v>17</v>
+      </c>
+      <c r="E141" t="s">
+        <v>7</v>
+      </c>
+      <c r="F141" t="s">
+        <v>59</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B142" t="s">
+        <v>319</v>
+      </c>
+      <c r="C142" t="s">
+        <v>320</v>
+      </c>
+      <c r="D142" t="s">
+        <v>292</v>
+      </c>
+      <c r="E142" t="s">
+        <v>25</v>
+      </c>
+      <c r="F142" t="s">
+        <v>15</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B143" t="s">
+        <v>321</v>
+      </c>
+      <c r="C143" t="s">
+        <v>322</v>
+      </c>
+      <c r="D143" t="s">
+        <v>23</v>
+      </c>
+      <c r="E143" t="s">
+        <v>7</v>
+      </c>
+      <c r="F143" t="s">
+        <v>15</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B144" t="s">
+        <v>323</v>
+      </c>
+      <c r="C144" t="s">
+        <v>324</v>
+      </c>
+      <c r="D144" t="s">
+        <v>19</v>
+      </c>
+      <c r="E144" t="s">
+        <v>7</v>
+      </c>
+      <c r="F144" t="s">
+        <v>15</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B145" t="s">
+        <v>325</v>
+      </c>
+      <c r="C145" t="s">
+        <v>326</v>
+      </c>
+      <c r="D145" t="s">
+        <v>17</v>
+      </c>
+      <c r="E145" t="s">
+        <v>7</v>
+      </c>
+      <c r="F145" t="s">
+        <v>15</v>
+      </c>
+      <c r="G145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B146" t="s">
+        <v>327</v>
+      </c>
+      <c r="C146" t="s">
+        <v>328</v>
+      </c>
+      <c r="D146" t="s">
+        <v>26</v>
+      </c>
+      <c r="E146" t="s">
+        <v>7</v>
+      </c>
+      <c r="F146" t="s">
+        <v>59</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B147" t="s">
+        <v>329</v>
+      </c>
+      <c r="C147" t="s">
+        <v>330</v>
+      </c>
+      <c r="D147" t="s">
+        <v>22</v>
+      </c>
+      <c r="E147" t="s">
+        <v>7</v>
+      </c>
+      <c r="F147" t="s">
+        <v>15</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B148" t="s">
+        <v>331</v>
+      </c>
+      <c r="C148" t="s">
+        <v>332</v>
+      </c>
+      <c r="D148" t="s">
+        <v>333</v>
+      </c>
+      <c r="E148" t="s">
+        <v>7</v>
+      </c>
+      <c r="F148" t="s">
+        <v>59</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B149" t="s">
+        <v>334</v>
+      </c>
+      <c r="C149" t="s">
+        <v>335</v>
+      </c>
+      <c r="D149" t="s">
+        <v>17</v>
+      </c>
+      <c r="E149" t="s">
+        <v>7</v>
+      </c>
+      <c r="F149" t="s">
+        <v>15</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B150" t="s">
+        <v>336</v>
+      </c>
+      <c r="C150" t="s">
+        <v>337</v>
+      </c>
+      <c r="D150" t="s">
+        <v>18</v>
+      </c>
+      <c r="E150" t="s">
+        <v>7</v>
+      </c>
+      <c r="F150" t="s">
+        <v>15</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B151" t="s">
+        <v>338</v>
+      </c>
+      <c r="C151" t="s">
+        <v>339</v>
+      </c>
+      <c r="D151" t="s">
+        <v>16</v>
+      </c>
+      <c r="E151" t="s">
+        <v>7</v>
+      </c>
+      <c r="F151" t="s">
+        <v>15</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B152" t="s">
+        <v>340</v>
+      </c>
+      <c r="C152" t="s">
+        <v>341</v>
+      </c>
+      <c r="D152" t="s">
+        <v>17</v>
+      </c>
+      <c r="E152" t="s">
+        <v>7</v>
+      </c>
+      <c r="F152" t="s">
+        <v>15</v>
+      </c>
+      <c r="G152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B153" t="s">
+        <v>342</v>
+      </c>
+      <c r="C153" t="s">
+        <v>343</v>
+      </c>
+      <c r="D153" t="s">
+        <v>22</v>
+      </c>
+      <c r="E153" t="s">
+        <v>7</v>
+      </c>
+      <c r="F153" t="s">
+        <v>15</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B154" t="s">
+        <v>344</v>
+      </c>
+      <c r="C154" t="s">
+        <v>345</v>
+      </c>
+      <c r="D154" t="s">
+        <v>13</v>
+      </c>
+      <c r="E154" t="s">
+        <v>7</v>
+      </c>
+      <c r="F154" t="s">
+        <v>8</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B155" t="s">
+        <v>346</v>
+      </c>
+      <c r="C155" t="s">
+        <v>347</v>
+      </c>
+      <c r="D155" t="s">
+        <v>22</v>
+      </c>
+      <c r="E155" t="s">
+        <v>7</v>
+      </c>
+      <c r="F155" t="s">
+        <v>15</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B156" t="s">
+        <v>348</v>
+      </c>
+      <c r="C156" t="s">
+        <v>349</v>
+      </c>
+      <c r="D156" t="s">
+        <v>333</v>
+      </c>
+      <c r="E156" t="s">
+        <v>7</v>
+      </c>
+      <c r="F156" t="s">
+        <v>15</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B157" t="s">
+        <v>350</v>
+      </c>
+      <c r="C157" t="s">
+        <v>351</v>
+      </c>
+      <c r="D157" t="s">
+        <v>9</v>
+      </c>
+      <c r="E157" t="s">
+        <v>7</v>
+      </c>
+      <c r="F157" t="s">
+        <v>15</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B158" t="s">
+        <v>352</v>
+      </c>
+      <c r="C158" t="s">
+        <v>353</v>
+      </c>
+      <c r="D158" t="s">
+        <v>13</v>
+      </c>
+      <c r="E158" t="s">
+        <v>7</v>
+      </c>
+      <c r="F158" t="s">
+        <v>8</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B159" t="s">
+        <v>354</v>
+      </c>
+      <c r="C159" t="s">
+        <v>355</v>
+      </c>
+      <c r="D159" t="s">
+        <v>22</v>
+      </c>
+      <c r="E159" t="s">
+        <v>7</v>
+      </c>
+      <c r="F159" t="s">
+        <v>15</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B160" t="s">
+        <v>356</v>
+      </c>
+      <c r="C160" t="s">
+        <v>357</v>
+      </c>
+      <c r="D160" t="s">
+        <v>23</v>
+      </c>
+      <c r="E160" t="s">
+        <v>7</v>
+      </c>
+      <c r="F160" t="s">
+        <v>15</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B161" t="s">
+        <v>358</v>
+      </c>
+      <c r="C161" t="s">
+        <v>359</v>
+      </c>
+      <c r="D161" t="s">
+        <v>23</v>
+      </c>
+      <c r="E161" t="s">
+        <v>7</v>
+      </c>
+      <c r="F161" t="s">
+        <v>15</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>45993</v>
+      </c>
+      <c r="B162" t="s">
+        <v>360</v>
+      </c>
+      <c r="C162" t="s">
+        <v>361</v>
+      </c>
+      <c r="D162" t="s">
+        <v>19</v>
+      </c>
+      <c r="E162" t="s">
+        <v>7</v>
+      </c>
+      <c r="F162" t="s">
+        <v>15</v>
+      </c>
+      <c r="G162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>45994</v>
+      </c>
+      <c r="B163" t="s">
+        <v>362</v>
+      </c>
+      <c r="C163" t="s">
+        <v>363</v>
+      </c>
+      <c r="D163" t="s">
+        <v>18</v>
+      </c>
+      <c r="E163" t="s">
+        <v>25</v>
+      </c>
+      <c r="F163" t="s">
+        <v>15</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>45994</v>
+      </c>
+      <c r="B164" t="s">
+        <v>364</v>
+      </c>
+      <c r="C164" t="s">
+        <v>365</v>
+      </c>
+      <c r="D164" t="s">
+        <v>22</v>
+      </c>
+      <c r="E164" t="s">
+        <v>7</v>
+      </c>
+      <c r="F164" t="s">
+        <v>15</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>45994</v>
+      </c>
+      <c r="B165" t="s">
+        <v>366</v>
+      </c>
+      <c r="C165" t="s">
+        <v>367</v>
+      </c>
+      <c r="D165" t="s">
+        <v>13</v>
+      </c>
+      <c r="E165" t="s">
+        <v>7</v>
+      </c>
+      <c r="F165" t="s">
+        <v>15</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>45994</v>
+      </c>
+      <c r="B166" t="s">
+        <v>368</v>
+      </c>
+      <c r="C166" t="s">
+        <v>369</v>
+      </c>
+      <c r="D166" t="s">
+        <v>13</v>
+      </c>
+      <c r="E166" t="s">
+        <v>7</v>
+      </c>
+      <c r="F166" t="s">
+        <v>15</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>45994</v>
+      </c>
+      <c r="B167" t="s">
+        <v>370</v>
+      </c>
+      <c r="C167" t="s">
+        <v>371</v>
+      </c>
+      <c r="D167" t="s">
+        <v>13</v>
+      </c>
+      <c r="E167" t="s">
+        <v>7</v>
+      </c>
+      <c r="F167" t="s">
+        <v>15</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>45994</v>
+      </c>
+      <c r="B168" t="s">
+        <v>372</v>
+      </c>
+      <c r="C168" t="s">
+        <v>373</v>
+      </c>
+      <c r="D168" t="s">
+        <v>10</v>
+      </c>
+      <c r="E168" t="s">
+        <v>7</v>
+      </c>
+      <c r="F168" t="s">
+        <v>15</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>45994</v>
+      </c>
+      <c r="B169" t="s">
+        <v>374</v>
+      </c>
+      <c r="C169" t="s">
+        <v>375</v>
+      </c>
+      <c r="D169" t="s">
+        <v>11</v>
+      </c>
+      <c r="E169" t="s">
+        <v>25</v>
+      </c>
+      <c r="F169" t="s">
+        <v>15</v>
+      </c>
+      <c r="G169">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated producao and balde - base 05/12/2025
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2025-12.xlsx
+++ b/first-atlas/producao_2025-12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29603"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96807290-9C6B-47A8-A6AB-F99CAFCD7CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B05717-E6B5-4C3A-907D-F357D70BF7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="684">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -1160,12 +1160,6 @@
     <t>LARA CONDE PSICOLOGIA LTDA</t>
   </si>
   <si>
-    <t xml:space="preserve">Procuracao com poderes para abrir e movimentar contas, pois identificamos que a representacao da sua empresa deve ser em conjunto pelos socios,  A procuracao deve ser assinada digitalmente pelos socios pela plataforma "GOV." e estar em formato PDF.&lt;br&gt;&lt;br&gt;Para garantir a seguranca e a validade do processo, Pedimos gentilmente que envie uma nova selfie, conforme as orientacoes </t>
-  </si>
-  <si>
-    <t>PENDENTE DOC</t>
-  </si>
-  <si>
     <t>46200500000178</t>
   </si>
   <si>
@@ -1665,6 +1659,438 @@
   </si>
   <si>
     <t>Procuracao com poderes de abrir e movimentar conta corrente junto a instituicoes financeiras com mandato vigente e devidamente assinada&lt;br&gt;&lt;br&gt;Contrato social atualizado e registrado no orgao competente</t>
+  </si>
+  <si>
+    <t>PENDÊNCIA DOC</t>
+  </si>
+  <si>
+    <t>63496917000149</t>
+  </si>
+  <si>
+    <t>ANA LUISA DE TORRES VALENTIM ANA LUISA DE TORRES VALENTIM</t>
+  </si>
+  <si>
+    <t>46427424000138</t>
+  </si>
+  <si>
+    <t>JOEL MARTINS RIBEIRO JOEL MARTINS RIBEIRO</t>
+  </si>
+  <si>
+    <t>27459913000127</t>
+  </si>
+  <si>
+    <t>PROSERV MAO DE OBRAS LTDA</t>
+  </si>
+  <si>
+    <t>30784571000125</t>
+  </si>
+  <si>
+    <t>LUIZ ANTONIO DOS SANTOS</t>
+  </si>
+  <si>
+    <t>63275494000137</t>
+  </si>
+  <si>
+    <t>TIAGO ANDRADE TELLES FIGHT TEAM</t>
+  </si>
+  <si>
+    <t>CARIMBADA</t>
+  </si>
+  <si>
+    <t>33230166000153</t>
+  </si>
+  <si>
+    <t>CONSTRUROCHA MANUTENCAO E REFORMAS LTDA</t>
+  </si>
+  <si>
+    <t>63911681000160</t>
+  </si>
+  <si>
+    <t>RS SERVICOS DE ALIMENTACAO LTDA</t>
+  </si>
+  <si>
+    <t>41457172000176</t>
+  </si>
+  <si>
+    <t>M V COMERCIO E LOCACOES DE MAQUINAS E EQUIPAMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>63606277000182</t>
+  </si>
+  <si>
+    <t>MANA MINERACAO IMPORTACAO E EXPORTACAO LTDA</t>
+  </si>
+  <si>
+    <t>98525850000108</t>
+  </si>
+  <si>
+    <t>NEIDE MARIA CITON GIEQUELIN</t>
+  </si>
+  <si>
+    <t>10777416000174</t>
+  </si>
+  <si>
+    <t>ASSOCIACAO PROJETO SEGREDO DA VITORIA</t>
+  </si>
+  <si>
+    <t>21562513000166</t>
+  </si>
+  <si>
+    <t>MILA SANTOS SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>20373055000154</t>
+  </si>
+  <si>
+    <t>JULIO MATHEUS DE SOUSA SOARES LTDA</t>
+  </si>
+  <si>
+    <t>21043217000159</t>
+  </si>
+  <si>
+    <t>21.043.217 LEONARDO CORADO PEREIRA</t>
+  </si>
+  <si>
+    <t>18831722000153</t>
+  </si>
+  <si>
+    <t>ANDRE GILBERTO SILVA DE OLIVEIRA REGO</t>
+  </si>
+  <si>
+    <t>20514000000117</t>
+  </si>
+  <si>
+    <t>SICKORRA TRANSPORTES E SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>27266049000147</t>
+  </si>
+  <si>
+    <t>IMPERIO CLINICA ODONTOLOGICA E CUIDADOS COM A SAUDE LTDA</t>
+  </si>
+  <si>
+    <t>32210038000185</t>
+  </si>
+  <si>
+    <t>ANA CRISTINA COSTA DOS SANTOS</t>
+  </si>
+  <si>
+    <t>36932253000140</t>
+  </si>
+  <si>
+    <t>T4G CONSULTORIA LTDA</t>
+  </si>
+  <si>
+    <t>31577186000170</t>
+  </si>
+  <si>
+    <t>31.577.186 AYANA SILVA DE LIMA</t>
+  </si>
+  <si>
+    <t>51543873000181</t>
+  </si>
+  <si>
+    <t>FABIOLA STEFANE DE SOUZA PEREIRA LTDA</t>
+  </si>
+  <si>
+    <t>19734140000111</t>
+  </si>
+  <si>
+    <t>ANA PAULA BARBOSA MAGALHAES</t>
+  </si>
+  <si>
+    <t>19809026000103</t>
+  </si>
+  <si>
+    <t>CIRCO KARTOON LTDA</t>
+  </si>
+  <si>
+    <t>63204435000178</t>
+  </si>
+  <si>
+    <t>SS ENGENHARIA E SERVICOS INDUSTRIAIS LTDA</t>
+  </si>
+  <si>
+    <t>63414556000144</t>
+  </si>
+  <si>
+    <t>RAMOS HUB LTDA</t>
+  </si>
+  <si>
+    <t>21414898000114</t>
+  </si>
+  <si>
+    <t>THIAGO PEREIRA DE LIMA ODONTOLOGIA</t>
+  </si>
+  <si>
+    <t>30131369000102</t>
+  </si>
+  <si>
+    <t>HEBACH SERVICOS ODONTOLOGICOS LTDA</t>
+  </si>
+  <si>
+    <t>22964010000180</t>
+  </si>
+  <si>
+    <t>A L DOS SANTOS AUTO PECAS</t>
+  </si>
+  <si>
+    <t>30113072000106</t>
+  </si>
+  <si>
+    <t>GT PILATES E TREINAMENTO FUNCIONAL LTDA</t>
+  </si>
+  <si>
+    <t>19876743000158</t>
+  </si>
+  <si>
+    <t>SBS SOLUCOES FINANCEIRAS LTDA</t>
+  </si>
+  <si>
+    <t>21020831000103</t>
+  </si>
+  <si>
+    <t>LORENA OLIVEIRA DOURADO</t>
+  </si>
+  <si>
+    <t>20747058000100</t>
+  </si>
+  <si>
+    <t>SUPRIMED DISTRIBUICAO LTDA</t>
+  </si>
+  <si>
+    <t>20250264000100</t>
+  </si>
+  <si>
+    <t>CAUE ZADRA BERTOLI</t>
+  </si>
+  <si>
+    <t>21197400000109</t>
+  </si>
+  <si>
+    <t>D'MARKS FACILITIES LTDA</t>
+  </si>
+  <si>
+    <t>31133621000177</t>
+  </si>
+  <si>
+    <t>JTR AGRICOLA LTDA</t>
+  </si>
+  <si>
+    <t>30824667000170</t>
+  </si>
+  <si>
+    <t>ARLINSON EDUARDO LOPES COELHO</t>
+  </si>
+  <si>
+    <t>Jose Guilherme de Abreu Mattos</t>
+  </si>
+  <si>
+    <t>15338842000125</t>
+  </si>
+  <si>
+    <t>MAGNIFFICA CONFECCOES LTDA</t>
+  </si>
+  <si>
+    <t>20456657000175</t>
+  </si>
+  <si>
+    <t>20.456.657 RICARDO NEREU CAPOVILLA</t>
+  </si>
+  <si>
+    <t>30051412000111</t>
+  </si>
+  <si>
+    <t>G M DA SILVA MAQUINAS AGRICOLAS</t>
+  </si>
+  <si>
+    <t>24831649000112</t>
+  </si>
+  <si>
+    <t>MEC MARINS SERVICOS E REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>24046477000176</t>
+  </si>
+  <si>
+    <t>MFT ACABAMENTOS CERAMICA E GRANITOS LTDA</t>
+  </si>
+  <si>
+    <t>62536474000100</t>
+  </si>
+  <si>
+    <t>VALE FORTE SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>26733908000106</t>
+  </si>
+  <si>
+    <t>26.733.908 MAICON PEREIRA ALVES</t>
+  </si>
+  <si>
+    <t>26569130000133</t>
+  </si>
+  <si>
+    <t>RAQUEL ALVES SOARES</t>
+  </si>
+  <si>
+    <t>19722494000146</t>
+  </si>
+  <si>
+    <t>E3 SERVICOS DE ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>22124611000265</t>
+  </si>
+  <si>
+    <t>LUCIANO CARLOS DE MELO</t>
+  </si>
+  <si>
+    <t>63905481000102</t>
+  </si>
+  <si>
+    <t>DABUL TOSIN SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>31337051000137</t>
+  </si>
+  <si>
+    <t>31.337.051 LUIS GUSTAVO ROCHA</t>
+  </si>
+  <si>
+    <t>23978450000159</t>
+  </si>
+  <si>
+    <t>ARAUJO &amp; SERPA LTDA</t>
+  </si>
+  <si>
+    <t>24326042000185</t>
+  </si>
+  <si>
+    <t>ADEMIR ALVES DE SOUZA</t>
+  </si>
+  <si>
+    <t>63497793000116</t>
+  </si>
+  <si>
+    <t>A R NUNES COMERCIO E SERVICOS DE ELETROELETRONICOS</t>
+  </si>
+  <si>
+    <t>24908106000156</t>
+  </si>
+  <si>
+    <t>JOAO PAULO GOMES OLIVEIRA</t>
+  </si>
+  <si>
+    <t>20242710000135</t>
+  </si>
+  <si>
+    <t>THIAGO LUIZ PENIDO</t>
+  </si>
+  <si>
+    <t>31483422000199</t>
+  </si>
+  <si>
+    <t>SILMARA THAISE SANTOS RODRIGUES ASSUNCAO</t>
+  </si>
+  <si>
+    <t>37931978000187</t>
+  </si>
+  <si>
+    <t>BRAGA MADEIRAS E TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>62046796000170</t>
+  </si>
+  <si>
+    <t>AZEVEDO HOLDING LTDA</t>
+  </si>
+  <si>
+    <t>Luana Duarte Paulo</t>
+  </si>
+  <si>
+    <t>31970917000142</t>
+  </si>
+  <si>
+    <t>SAMUEL SOUSA TRINDADE</t>
+  </si>
+  <si>
+    <t>27750607000145</t>
+  </si>
+  <si>
+    <t>LEE PETTERSON DA SILVA ALMEIDA</t>
+  </si>
+  <si>
+    <t>24964923000121</t>
+  </si>
+  <si>
+    <t>24.964.923 DIEGO ALBERTO NASCIMENTO DE MORAIS</t>
+  </si>
+  <si>
+    <t>27728255000121</t>
+  </si>
+  <si>
+    <t>MAGALHAES TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>25279741000184</t>
+  </si>
+  <si>
+    <t>F B FERREIRA SOLUCOES DIGITAIS</t>
+  </si>
+  <si>
+    <t>21536179000176</t>
+  </si>
+  <si>
+    <t>DMS DE OLIVEIRA DESENVOLVIMENTO DE PRODUTOS</t>
+  </si>
+  <si>
+    <t>28029773000110</t>
+  </si>
+  <si>
+    <t>28.029.773 LUIZ FELLIPE FRANCO FIALHO</t>
+  </si>
+  <si>
+    <t>62649051000104</t>
+  </si>
+  <si>
+    <t>AMG SERVICOS LTDA</t>
+  </si>
+  <si>
+    <t>48904351000153</t>
+  </si>
+  <si>
+    <t>SEABRA ASSESSORIA E CONSULTORIA EMPRESARIAL LTDA</t>
+  </si>
+  <si>
+    <t>63717239000105</t>
+  </si>
+  <si>
+    <t>JONNY MOTOS CG LTDA</t>
+  </si>
+  <si>
+    <t>26067761000154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLAUCIA REIS MENEZES PAIVA </t>
+  </si>
+  <si>
+    <t>26424954000115</t>
+  </si>
+  <si>
+    <t>CAROLINE CHAGAS PAIVA RESTAURANTE E MINIMERCADO</t>
+  </si>
+  <si>
+    <t>19825741000130</t>
+  </si>
+  <si>
+    <t>SCHWARZENEGGER CAMPOS DOS SANTOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Convencao de condominio atualizada e devidamente registrada em orgao competente.</t>
+  </si>
+  <si>
+    <t>Contrato Social da empresa TRANSPORTADORA JUNIOR E JULIANO LTDA, devidamente atualizado e registrado no orgao competente&lt;br&gt;&lt;br&gt;Ã‰ necessario o envio do Ato Constitutivo para validacao das informacoes.</t>
   </si>
 </sst>
 </file>
@@ -2036,10 +2462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCD3CE2-DBA2-4F4F-B6A3-11EE884EA727}">
-  <dimension ref="A1:G249"/>
+  <dimension ref="A1:G319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,7 +2537,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>374</v>
+        <v>540</v>
       </c>
       <c r="G3" t="s">
         <v>57</v>
@@ -2272,10 +2698,10 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>374</v>
-      </c>
-      <c r="G10" t="s">
-        <v>373</v>
+        <v>177</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2295,7 +2721,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -2318,7 +2744,7 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3263,8 +3689,8 @@
       <c r="F53" t="s">
         <v>15</v>
       </c>
-      <c r="G53" t="e">
-        <v>#N/A</v>
+      <c r="G53">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3422,10 +3848,10 @@
         <v>7</v>
       </c>
       <c r="F60" t="s">
-        <v>374</v>
+        <v>58</v>
       </c>
       <c r="G60" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3491,7 +3917,7 @@
         <v>25</v>
       </c>
       <c r="F63" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -4825,10 +5251,10 @@
         <v>7</v>
       </c>
       <c r="F121" t="s">
-        <v>58</v>
-      </c>
-      <c r="G121">
-        <v>0</v>
+        <v>540</v>
+      </c>
+      <c r="G121" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -4871,7 +5297,7 @@
         <v>7</v>
       </c>
       <c r="F123" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -5917,10 +6343,10 @@
         <v>45994</v>
       </c>
       <c r="B169" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C169" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D169" t="s">
         <v>187</v>
@@ -5940,10 +6366,10 @@
         <v>45994</v>
       </c>
       <c r="B170" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C170" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D170" t="s">
         <v>187</v>
@@ -5963,10 +6389,10 @@
         <v>45994</v>
       </c>
       <c r="B171" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C171" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D171" t="s">
         <v>18</v>
@@ -5986,10 +6412,10 @@
         <v>45994</v>
       </c>
       <c r="B172" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C172" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D172" t="s">
         <v>6</v>
@@ -6009,10 +6435,10 @@
         <v>45994</v>
       </c>
       <c r="B173" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C173" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D173" t="s">
         <v>6</v>
@@ -6032,16 +6458,16 @@
         <v>45994</v>
       </c>
       <c r="B174" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C174" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D174" t="s">
         <v>11</v>
       </c>
       <c r="E174" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F174" t="s">
         <v>15</v>
@@ -6055,10 +6481,10 @@
         <v>45994</v>
       </c>
       <c r="B175" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C175" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D175" t="s">
         <v>17</v>
@@ -6078,10 +6504,10 @@
         <v>45994</v>
       </c>
       <c r="B176" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C176" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D176" t="s">
         <v>9</v>
@@ -6101,10 +6527,10 @@
         <v>45994</v>
       </c>
       <c r="B177" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C177" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D177" t="s">
         <v>22</v>
@@ -6124,10 +6550,10 @@
         <v>45994</v>
       </c>
       <c r="B178" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C178" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D178" t="s">
         <v>6</v>
@@ -6147,10 +6573,10 @@
         <v>45994</v>
       </c>
       <c r="B179" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C179" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D179" t="s">
         <v>23</v>
@@ -6170,10 +6596,10 @@
         <v>45994</v>
       </c>
       <c r="B180" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C180" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D180" t="s">
         <v>27</v>
@@ -6193,10 +6619,10 @@
         <v>45994</v>
       </c>
       <c r="B181" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C181" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D181" t="s">
         <v>17</v>
@@ -6216,10 +6642,10 @@
         <v>45994</v>
       </c>
       <c r="B182" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C182" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D182" t="s">
         <v>13</v>
@@ -6239,10 +6665,10 @@
         <v>45994</v>
       </c>
       <c r="B183" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C183" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D183" t="s">
         <v>13</v>
@@ -6262,10 +6688,10 @@
         <v>45994</v>
       </c>
       <c r="B184" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C184" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D184" t="s">
         <v>17</v>
@@ -6285,10 +6711,10 @@
         <v>45994</v>
       </c>
       <c r="B185" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C185" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D185" t="s">
         <v>17</v>
@@ -6308,10 +6734,10 @@
         <v>45994</v>
       </c>
       <c r="B186" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C186" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D186" t="s">
         <v>6</v>
@@ -6331,10 +6757,10 @@
         <v>45994</v>
       </c>
       <c r="B187" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C187" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D187" t="s">
         <v>17</v>
@@ -6354,10 +6780,10 @@
         <v>45994</v>
       </c>
       <c r="B188" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C188" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D188" t="s">
         <v>16</v>
@@ -6366,7 +6792,7 @@
         <v>7</v>
       </c>
       <c r="F188" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G188">
         <v>0</v>
@@ -6377,10 +6803,10 @@
         <v>45994</v>
       </c>
       <c r="B189" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C189" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D189" t="s">
         <v>23</v>
@@ -6400,10 +6826,10 @@
         <v>45994</v>
       </c>
       <c r="B190" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C190" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D190" t="s">
         <v>13</v>
@@ -6423,10 +6849,10 @@
         <v>45994</v>
       </c>
       <c r="B191" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C191" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D191" t="s">
         <v>11</v>
@@ -6446,10 +6872,10 @@
         <v>45994</v>
       </c>
       <c r="B192" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C192" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D192" t="s">
         <v>16</v>
@@ -6469,10 +6895,10 @@
         <v>45994</v>
       </c>
       <c r="B193" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C193" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D193" t="s">
         <v>19</v>
@@ -6492,10 +6918,10 @@
         <v>45994</v>
       </c>
       <c r="B194" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C194" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D194" t="s">
         <v>13</v>
@@ -6515,10 +6941,10 @@
         <v>45994</v>
       </c>
       <c r="B195" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C195" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D195" t="s">
         <v>23</v>
@@ -6538,10 +6964,10 @@
         <v>45994</v>
       </c>
       <c r="B196" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C196" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D196" t="s">
         <v>18</v>
@@ -6550,7 +6976,7 @@
         <v>7</v>
       </c>
       <c r="F196" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G196">
         <v>0</v>
@@ -6561,10 +6987,10 @@
         <v>45994</v>
       </c>
       <c r="B197" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C197" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D197" t="s">
         <v>17</v>
@@ -6584,10 +7010,10 @@
         <v>45994</v>
       </c>
       <c r="B198" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C198" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D198" t="s">
         <v>13</v>
@@ -6607,10 +7033,10 @@
         <v>45994</v>
       </c>
       <c r="B199" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C199" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D199" t="s">
         <v>22</v>
@@ -6630,10 +7056,10 @@
         <v>45994</v>
       </c>
       <c r="B200" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C200" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D200" t="s">
         <v>13</v>
@@ -6653,10 +7079,10 @@
         <v>45994</v>
       </c>
       <c r="B201" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C201" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D201" t="s">
         <v>22</v>
@@ -6676,10 +7102,10 @@
         <v>45994</v>
       </c>
       <c r="B202" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C202" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D202" t="s">
         <v>17</v>
@@ -6699,10 +7125,10 @@
         <v>45994</v>
       </c>
       <c r="B203" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C203" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D203" t="s">
         <v>10</v>
@@ -6722,10 +7148,10 @@
         <v>45994</v>
       </c>
       <c r="B204" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C204" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D204" t="s">
         <v>19</v>
@@ -6745,10 +7171,10 @@
         <v>45994</v>
       </c>
       <c r="B205" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C205" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D205" t="s">
         <v>11</v>
@@ -6768,10 +7194,10 @@
         <v>45994</v>
       </c>
       <c r="B206" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C206" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D206" t="s">
         <v>9</v>
@@ -6791,10 +7217,10 @@
         <v>45994</v>
       </c>
       <c r="B207" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C207" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D207" t="s">
         <v>19</v>
@@ -6814,10 +7240,10 @@
         <v>45994</v>
       </c>
       <c r="B208" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C208" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D208" t="s">
         <v>17</v>
@@ -6837,10 +7263,10 @@
         <v>45994</v>
       </c>
       <c r="B209" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C209" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D209" t="s">
         <v>13</v>
@@ -6860,16 +7286,16 @@
         <v>45994</v>
       </c>
       <c r="B210" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C210" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D210" t="s">
         <v>10</v>
       </c>
       <c r="E210" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F210" t="s">
         <v>15</v>
@@ -6883,16 +7309,16 @@
         <v>45994</v>
       </c>
       <c r="B211" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C211" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D211" t="s">
         <v>23</v>
       </c>
       <c r="E211" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F211" t="s">
         <v>15</v>
@@ -6906,10 +7332,10 @@
         <v>45994</v>
       </c>
       <c r="B212" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C212" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D212" t="s">
         <v>26</v>
@@ -6918,7 +7344,7 @@
         <v>7</v>
       </c>
       <c r="F212" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G212">
         <v>0</v>
@@ -6929,16 +7355,16 @@
         <v>45994</v>
       </c>
       <c r="B213" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C213" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D213" t="s">
         <v>9</v>
       </c>
       <c r="E213" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F213" t="s">
         <v>15</v>
@@ -6952,10 +7378,10 @@
         <v>45994</v>
       </c>
       <c r="B214" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C214" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D214" t="s">
         <v>9</v>
@@ -6975,10 +7401,10 @@
         <v>45994</v>
       </c>
       <c r="B215" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C215" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D215" t="s">
         <v>10</v>
@@ -6990,7 +7416,7 @@
         <v>58</v>
       </c>
       <c r="G215" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -6998,10 +7424,10 @@
         <v>45994</v>
       </c>
       <c r="B216" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C216" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D216" t="s">
         <v>27</v>
@@ -7021,10 +7447,10 @@
         <v>45994</v>
       </c>
       <c r="B217" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C217" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D217" t="s">
         <v>9</v>
@@ -7044,10 +7470,10 @@
         <v>45994</v>
       </c>
       <c r="B218" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C218" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D218" t="s">
         <v>27</v>
@@ -7067,10 +7493,10 @@
         <v>45994</v>
       </c>
       <c r="B219" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C219" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D219" t="s">
         <v>23</v>
@@ -7090,10 +7516,10 @@
         <v>45994</v>
       </c>
       <c r="B220" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C220" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D220" t="s">
         <v>23</v>
@@ -7113,10 +7539,10 @@
         <v>45994</v>
       </c>
       <c r="B221" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C221" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D221" t="s">
         <v>19</v>
@@ -7136,10 +7562,10 @@
         <v>45994</v>
       </c>
       <c r="B222" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C222" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D222" t="s">
         <v>23</v>
@@ -7159,10 +7585,10 @@
         <v>45994</v>
       </c>
       <c r="B223" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C223" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D223" t="s">
         <v>6</v>
@@ -7182,10 +7608,10 @@
         <v>45994</v>
       </c>
       <c r="B224" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C224" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D224" t="s">
         <v>20</v>
@@ -7205,10 +7631,10 @@
         <v>45994</v>
       </c>
       <c r="B225" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C225" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D225" t="s">
         <v>11</v>
@@ -7217,7 +7643,7 @@
         <v>14</v>
       </c>
       <c r="F225" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G225">
         <v>0</v>
@@ -7228,10 +7654,10 @@
         <v>45994</v>
       </c>
       <c r="B226" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C226" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D226" t="s">
         <v>10</v>
@@ -7251,10 +7677,10 @@
         <v>45994</v>
       </c>
       <c r="B227" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C227" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D227" t="s">
         <v>17</v>
@@ -7274,19 +7700,19 @@
         <v>45994</v>
       </c>
       <c r="B228" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C228" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D228" t="s">
         <v>16</v>
       </c>
       <c r="E228" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F228" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G228">
         <v>0</v>
@@ -7297,10 +7723,10 @@
         <v>45994</v>
       </c>
       <c r="B229" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C229" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D229" t="s">
         <v>17</v>
@@ -7309,7 +7735,7 @@
         <v>7</v>
       </c>
       <c r="F229" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G229">
         <v>0</v>
@@ -7320,10 +7746,10 @@
         <v>45994</v>
       </c>
       <c r="B230" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C230" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D230" t="s">
         <v>23</v>
@@ -7343,10 +7769,10 @@
         <v>45994</v>
       </c>
       <c r="B231" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C231" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D231" t="s">
         <v>17</v>
@@ -7366,10 +7792,10 @@
         <v>45994</v>
       </c>
       <c r="B232" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C232" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D232" t="s">
         <v>17</v>
@@ -7378,7 +7804,7 @@
         <v>7</v>
       </c>
       <c r="F232" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G232">
         <v>0</v>
@@ -7389,10 +7815,10 @@
         <v>45994</v>
       </c>
       <c r="B233" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C233" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D233" t="s">
         <v>9</v>
@@ -7412,10 +7838,10 @@
         <v>45994</v>
       </c>
       <c r="B234" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C234" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D234" t="s">
         <v>17</v>
@@ -7424,7 +7850,7 @@
         <v>7</v>
       </c>
       <c r="F234" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G234">
         <v>0</v>
@@ -7435,10 +7861,10 @@
         <v>45994</v>
       </c>
       <c r="B235" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C235" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D235" t="s">
         <v>17</v>
@@ -7447,7 +7873,7 @@
         <v>7</v>
       </c>
       <c r="F235" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G235">
         <v>0</v>
@@ -7458,10 +7884,10 @@
         <v>45994</v>
       </c>
       <c r="B236" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C236" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D236" t="s">
         <v>19</v>
@@ -7481,10 +7907,10 @@
         <v>45994</v>
       </c>
       <c r="B237" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C237" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D237" t="s">
         <v>22</v>
@@ -7493,7 +7919,7 @@
         <v>7</v>
       </c>
       <c r="F237" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G237">
         <v>0</v>
@@ -7504,10 +7930,10 @@
         <v>45994</v>
       </c>
       <c r="B238" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C238" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D238" t="s">
         <v>13</v>
@@ -7516,10 +7942,10 @@
         <v>14</v>
       </c>
       <c r="F238" t="s">
-        <v>58</v>
-      </c>
-      <c r="G238">
-        <v>0</v>
+        <v>540</v>
+      </c>
+      <c r="G238" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -7527,10 +7953,10 @@
         <v>45994</v>
       </c>
       <c r="B239" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C239" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D239" t="s">
         <v>13</v>
@@ -7550,10 +7976,10 @@
         <v>45994</v>
       </c>
       <c r="B240" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C240" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D240" t="s">
         <v>17</v>
@@ -7562,7 +7988,7 @@
         <v>14</v>
       </c>
       <c r="F240" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G240">
         <v>0</v>
@@ -7573,10 +7999,10 @@
         <v>45994</v>
       </c>
       <c r="B241" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C241" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D241" t="s">
         <v>17</v>
@@ -7585,7 +8011,7 @@
         <v>7</v>
       </c>
       <c r="F241" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G241">
         <v>0</v>
@@ -7596,10 +8022,10 @@
         <v>45994</v>
       </c>
       <c r="B242" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C242" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D242" t="s">
         <v>23</v>
@@ -7619,10 +8045,10 @@
         <v>45994</v>
       </c>
       <c r="B243" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C243" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D243" t="s">
         <v>19</v>
@@ -7642,10 +8068,10 @@
         <v>45994</v>
       </c>
       <c r="B244" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C244" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D244" t="s">
         <v>23</v>
@@ -7665,10 +8091,10 @@
         <v>45994</v>
       </c>
       <c r="B245" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C245" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D245" t="s">
         <v>17</v>
@@ -7677,7 +8103,7 @@
         <v>7</v>
       </c>
       <c r="F245" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="G245">
         <v>0</v>
@@ -7688,10 +8114,10 @@
         <v>45994</v>
       </c>
       <c r="B246" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C246" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D246" t="s">
         <v>17</v>
@@ -7711,10 +8137,10 @@
         <v>45994</v>
       </c>
       <c r="B247" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C247" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D247" t="s">
         <v>9</v>
@@ -7734,10 +8160,10 @@
         <v>45994</v>
       </c>
       <c r="B248" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C248" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D248" t="s">
         <v>22</v>
@@ -7757,10 +8183,10 @@
         <v>45995</v>
       </c>
       <c r="B249" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C249" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D249" t="s">
         <v>9</v>
@@ -7772,6 +8198,1613 @@
         <v>15</v>
       </c>
       <c r="G249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B250" t="s">
+        <v>541</v>
+      </c>
+      <c r="C250" t="s">
+        <v>542</v>
+      </c>
+      <c r="D250" t="s">
+        <v>11</v>
+      </c>
+      <c r="E250" t="s">
+        <v>188</v>
+      </c>
+      <c r="F250" t="s">
+        <v>15</v>
+      </c>
+      <c r="G250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B251" t="s">
+        <v>543</v>
+      </c>
+      <c r="C251" t="s">
+        <v>544</v>
+      </c>
+      <c r="D251" t="s">
+        <v>187</v>
+      </c>
+      <c r="E251" t="s">
+        <v>188</v>
+      </c>
+      <c r="F251" t="s">
+        <v>15</v>
+      </c>
+      <c r="G251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B252" t="s">
+        <v>545</v>
+      </c>
+      <c r="C252" t="s">
+        <v>546</v>
+      </c>
+      <c r="D252" t="s">
+        <v>10</v>
+      </c>
+      <c r="E252" t="s">
+        <v>7</v>
+      </c>
+      <c r="F252" t="s">
+        <v>8</v>
+      </c>
+      <c r="G252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B253" t="s">
+        <v>547</v>
+      </c>
+      <c r="C253" t="s">
+        <v>548</v>
+      </c>
+      <c r="D253" t="s">
+        <v>10</v>
+      </c>
+      <c r="E253" t="s">
+        <v>7</v>
+      </c>
+      <c r="F253" t="s">
+        <v>15</v>
+      </c>
+      <c r="G253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B254" t="s">
+        <v>549</v>
+      </c>
+      <c r="C254" t="s">
+        <v>550</v>
+      </c>
+      <c r="D254" t="s">
+        <v>18</v>
+      </c>
+      <c r="E254" t="s">
+        <v>25</v>
+      </c>
+      <c r="F254" t="s">
+        <v>551</v>
+      </c>
+      <c r="G254" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B255" t="s">
+        <v>536</v>
+      </c>
+      <c r="C255" t="s">
+        <v>537</v>
+      </c>
+      <c r="D255" t="s">
+        <v>9</v>
+      </c>
+      <c r="E255" t="s">
+        <v>25</v>
+      </c>
+      <c r="F255" t="s">
+        <v>15</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B256" t="s">
+        <v>552</v>
+      </c>
+      <c r="C256" t="s">
+        <v>553</v>
+      </c>
+      <c r="D256" t="s">
+        <v>16</v>
+      </c>
+      <c r="E256" t="s">
+        <v>7</v>
+      </c>
+      <c r="F256" t="s">
+        <v>8</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B257" t="s">
+        <v>554</v>
+      </c>
+      <c r="C257" t="s">
+        <v>555</v>
+      </c>
+      <c r="D257" t="s">
+        <v>18</v>
+      </c>
+      <c r="E257" t="s">
+        <v>25</v>
+      </c>
+      <c r="F257" t="s">
+        <v>58</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B258" t="s">
+        <v>556</v>
+      </c>
+      <c r="C258" t="s">
+        <v>557</v>
+      </c>
+      <c r="D258" t="s">
+        <v>10</v>
+      </c>
+      <c r="E258" t="s">
+        <v>7</v>
+      </c>
+      <c r="F258" t="s">
+        <v>8</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B259" t="s">
+        <v>558</v>
+      </c>
+      <c r="C259" t="s">
+        <v>559</v>
+      </c>
+      <c r="D259" t="s">
+        <v>17</v>
+      </c>
+      <c r="E259" t="s">
+        <v>14</v>
+      </c>
+      <c r="F259" t="s">
+        <v>15</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B260" t="s">
+        <v>560</v>
+      </c>
+      <c r="C260" t="s">
+        <v>561</v>
+      </c>
+      <c r="D260" t="s">
+        <v>27</v>
+      </c>
+      <c r="E260" t="s">
+        <v>25</v>
+      </c>
+      <c r="F260" t="s">
+        <v>58</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B261" t="s">
+        <v>562</v>
+      </c>
+      <c r="C261" t="s">
+        <v>563</v>
+      </c>
+      <c r="D261" t="s">
+        <v>6</v>
+      </c>
+      <c r="E261" t="s">
+        <v>7</v>
+      </c>
+      <c r="F261" t="s">
+        <v>58</v>
+      </c>
+      <c r="G261">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B262" t="s">
+        <v>564</v>
+      </c>
+      <c r="C262" t="s">
+        <v>565</v>
+      </c>
+      <c r="D262" t="s">
+        <v>6</v>
+      </c>
+      <c r="E262" t="s">
+        <v>7</v>
+      </c>
+      <c r="F262" t="s">
+        <v>15</v>
+      </c>
+      <c r="G262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B263" t="s">
+        <v>566</v>
+      </c>
+      <c r="C263" t="s">
+        <v>567</v>
+      </c>
+      <c r="D263" t="s">
+        <v>23</v>
+      </c>
+      <c r="E263" t="s">
+        <v>7</v>
+      </c>
+      <c r="F263" t="s">
+        <v>15</v>
+      </c>
+      <c r="G263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B264" t="s">
+        <v>568</v>
+      </c>
+      <c r="C264" t="s">
+        <v>569</v>
+      </c>
+      <c r="D264" t="s">
+        <v>17</v>
+      </c>
+      <c r="E264" t="s">
+        <v>7</v>
+      </c>
+      <c r="F264" t="s">
+        <v>15</v>
+      </c>
+      <c r="G264">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B265" t="s">
+        <v>570</v>
+      </c>
+      <c r="C265" t="s">
+        <v>571</v>
+      </c>
+      <c r="D265" t="s">
+        <v>20</v>
+      </c>
+      <c r="E265" t="s">
+        <v>7</v>
+      </c>
+      <c r="F265" t="s">
+        <v>12</v>
+      </c>
+      <c r="G265">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B266" t="s">
+        <v>572</v>
+      </c>
+      <c r="C266" t="s">
+        <v>573</v>
+      </c>
+      <c r="D266" t="s">
+        <v>19</v>
+      </c>
+      <c r="E266" t="s">
+        <v>7</v>
+      </c>
+      <c r="F266" t="s">
+        <v>15</v>
+      </c>
+      <c r="G266">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B267" t="s">
+        <v>574</v>
+      </c>
+      <c r="C267" t="s">
+        <v>575</v>
+      </c>
+      <c r="D267" t="s">
+        <v>23</v>
+      </c>
+      <c r="E267" t="s">
+        <v>7</v>
+      </c>
+      <c r="F267" t="s">
+        <v>15</v>
+      </c>
+      <c r="G267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B268" t="s">
+        <v>576</v>
+      </c>
+      <c r="C268" t="s">
+        <v>577</v>
+      </c>
+      <c r="D268" t="s">
+        <v>13</v>
+      </c>
+      <c r="E268" t="s">
+        <v>7</v>
+      </c>
+      <c r="F268" t="s">
+        <v>15</v>
+      </c>
+      <c r="G268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B269" t="s">
+        <v>578</v>
+      </c>
+      <c r="C269" t="s">
+        <v>579</v>
+      </c>
+      <c r="D269" t="s">
+        <v>27</v>
+      </c>
+      <c r="E269" t="s">
+        <v>14</v>
+      </c>
+      <c r="F269" t="s">
+        <v>15</v>
+      </c>
+      <c r="G269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B270" t="s">
+        <v>580</v>
+      </c>
+      <c r="C270" t="s">
+        <v>581</v>
+      </c>
+      <c r="D270" t="s">
+        <v>23</v>
+      </c>
+      <c r="E270" t="s">
+        <v>7</v>
+      </c>
+      <c r="F270" t="s">
+        <v>8</v>
+      </c>
+      <c r="G270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B271" t="s">
+        <v>582</v>
+      </c>
+      <c r="C271" t="s">
+        <v>583</v>
+      </c>
+      <c r="D271" t="s">
+        <v>16</v>
+      </c>
+      <c r="E271" t="s">
+        <v>14</v>
+      </c>
+      <c r="F271" t="s">
+        <v>15</v>
+      </c>
+      <c r="G271">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B272" t="s">
+        <v>584</v>
+      </c>
+      <c r="C272" t="s">
+        <v>585</v>
+      </c>
+      <c r="D272" t="s">
+        <v>22</v>
+      </c>
+      <c r="E272" t="s">
+        <v>7</v>
+      </c>
+      <c r="F272" t="s">
+        <v>15</v>
+      </c>
+      <c r="G272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B273" t="s">
+        <v>586</v>
+      </c>
+      <c r="C273" t="s">
+        <v>587</v>
+      </c>
+      <c r="D273" t="s">
+        <v>13</v>
+      </c>
+      <c r="E273" t="s">
+        <v>7</v>
+      </c>
+      <c r="F273" t="s">
+        <v>15</v>
+      </c>
+      <c r="G273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B274" t="s">
+        <v>588</v>
+      </c>
+      <c r="C274" t="s">
+        <v>589</v>
+      </c>
+      <c r="D274" t="s">
+        <v>22</v>
+      </c>
+      <c r="E274" t="s">
+        <v>7</v>
+      </c>
+      <c r="F274" t="s">
+        <v>58</v>
+      </c>
+      <c r="G274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B275" t="s">
+        <v>590</v>
+      </c>
+      <c r="C275" t="s">
+        <v>591</v>
+      </c>
+      <c r="D275" t="s">
+        <v>23</v>
+      </c>
+      <c r="E275" t="s">
+        <v>7</v>
+      </c>
+      <c r="F275" t="s">
+        <v>15</v>
+      </c>
+      <c r="G275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B276" t="s">
+        <v>592</v>
+      </c>
+      <c r="C276" t="s">
+        <v>593</v>
+      </c>
+      <c r="D276" t="s">
+        <v>16</v>
+      </c>
+      <c r="E276" t="s">
+        <v>7</v>
+      </c>
+      <c r="F276" t="s">
+        <v>15</v>
+      </c>
+      <c r="G276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B277" t="s">
+        <v>594</v>
+      </c>
+      <c r="C277" t="s">
+        <v>595</v>
+      </c>
+      <c r="D277" t="s">
+        <v>26</v>
+      </c>
+      <c r="E277" t="s">
+        <v>7</v>
+      </c>
+      <c r="F277" t="s">
+        <v>58</v>
+      </c>
+      <c r="G277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B278" t="s">
+        <v>596</v>
+      </c>
+      <c r="C278" t="s">
+        <v>597</v>
+      </c>
+      <c r="D278" t="s">
+        <v>9</v>
+      </c>
+      <c r="E278" t="s">
+        <v>7</v>
+      </c>
+      <c r="F278" t="s">
+        <v>15</v>
+      </c>
+      <c r="G278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B279" t="s">
+        <v>598</v>
+      </c>
+      <c r="C279" t="s">
+        <v>599</v>
+      </c>
+      <c r="D279" t="s">
+        <v>19</v>
+      </c>
+      <c r="E279" t="s">
+        <v>7</v>
+      </c>
+      <c r="F279" t="s">
+        <v>15</v>
+      </c>
+      <c r="G279">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B280" t="s">
+        <v>600</v>
+      </c>
+      <c r="C280" t="s">
+        <v>601</v>
+      </c>
+      <c r="D280" t="s">
+        <v>22</v>
+      </c>
+      <c r="E280" t="s">
+        <v>14</v>
+      </c>
+      <c r="F280" t="s">
+        <v>8</v>
+      </c>
+      <c r="G280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B281" t="s">
+        <v>602</v>
+      </c>
+      <c r="C281" t="s">
+        <v>603</v>
+      </c>
+      <c r="D281" t="s">
+        <v>27</v>
+      </c>
+      <c r="E281" t="s">
+        <v>7</v>
+      </c>
+      <c r="F281" t="s">
+        <v>15</v>
+      </c>
+      <c r="G281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B282" t="s">
+        <v>604</v>
+      </c>
+      <c r="C282" t="s">
+        <v>605</v>
+      </c>
+      <c r="D282" t="s">
+        <v>18</v>
+      </c>
+      <c r="E282" t="s">
+        <v>7</v>
+      </c>
+      <c r="F282" t="s">
+        <v>15</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A283" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B283" t="s">
+        <v>606</v>
+      </c>
+      <c r="C283" t="s">
+        <v>607</v>
+      </c>
+      <c r="D283" t="s">
+        <v>13</v>
+      </c>
+      <c r="E283" t="s">
+        <v>7</v>
+      </c>
+      <c r="F283" t="s">
+        <v>15</v>
+      </c>
+      <c r="G283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B284" t="s">
+        <v>608</v>
+      </c>
+      <c r="C284" t="s">
+        <v>609</v>
+      </c>
+      <c r="D284" t="s">
+        <v>9</v>
+      </c>
+      <c r="E284" t="s">
+        <v>7</v>
+      </c>
+      <c r="F284" t="s">
+        <v>8</v>
+      </c>
+      <c r="G284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B285" t="s">
+        <v>610</v>
+      </c>
+      <c r="C285" t="s">
+        <v>611</v>
+      </c>
+      <c r="D285" t="s">
+        <v>6</v>
+      </c>
+      <c r="E285" t="s">
+        <v>7</v>
+      </c>
+      <c r="F285" t="s">
+        <v>551</v>
+      </c>
+      <c r="G285" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B286" t="s">
+        <v>612</v>
+      </c>
+      <c r="C286" t="s">
+        <v>613</v>
+      </c>
+      <c r="D286" t="s">
+        <v>614</v>
+      </c>
+      <c r="E286" t="s">
+        <v>465</v>
+      </c>
+      <c r="F286" t="s">
+        <v>15</v>
+      </c>
+      <c r="G286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B287" t="s">
+        <v>615</v>
+      </c>
+      <c r="C287" t="s">
+        <v>616</v>
+      </c>
+      <c r="D287" t="s">
+        <v>10</v>
+      </c>
+      <c r="E287" t="s">
+        <v>7</v>
+      </c>
+      <c r="F287" t="s">
+        <v>15</v>
+      </c>
+      <c r="G287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B288" t="s">
+        <v>617</v>
+      </c>
+      <c r="C288" t="s">
+        <v>618</v>
+      </c>
+      <c r="D288" t="s">
+        <v>16</v>
+      </c>
+      <c r="E288" t="s">
+        <v>7</v>
+      </c>
+      <c r="F288" t="s">
+        <v>15</v>
+      </c>
+      <c r="G288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B289" t="s">
+        <v>619</v>
+      </c>
+      <c r="C289" t="s">
+        <v>620</v>
+      </c>
+      <c r="D289" t="s">
+        <v>10</v>
+      </c>
+      <c r="E289" t="s">
+        <v>7</v>
+      </c>
+      <c r="F289" t="s">
+        <v>15</v>
+      </c>
+      <c r="G289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B290" t="s">
+        <v>621</v>
+      </c>
+      <c r="C290" t="s">
+        <v>622</v>
+      </c>
+      <c r="D290" t="s">
+        <v>10</v>
+      </c>
+      <c r="E290" t="s">
+        <v>7</v>
+      </c>
+      <c r="F290" t="s">
+        <v>15</v>
+      </c>
+      <c r="G290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B291" t="s">
+        <v>623</v>
+      </c>
+      <c r="C291" t="s">
+        <v>624</v>
+      </c>
+      <c r="D291" t="s">
+        <v>22</v>
+      </c>
+      <c r="E291" t="s">
+        <v>7</v>
+      </c>
+      <c r="F291" t="s">
+        <v>15</v>
+      </c>
+      <c r="G291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B292" t="s">
+        <v>625</v>
+      </c>
+      <c r="C292" t="s">
+        <v>626</v>
+      </c>
+      <c r="D292" t="s">
+        <v>10</v>
+      </c>
+      <c r="E292" t="s">
+        <v>7</v>
+      </c>
+      <c r="F292" t="s">
+        <v>8</v>
+      </c>
+      <c r="G292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B293" t="s">
+        <v>627</v>
+      </c>
+      <c r="C293" t="s">
+        <v>628</v>
+      </c>
+      <c r="D293" t="s">
+        <v>22</v>
+      </c>
+      <c r="E293" t="s">
+        <v>7</v>
+      </c>
+      <c r="F293" t="s">
+        <v>15</v>
+      </c>
+      <c r="G293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B294" t="s">
+        <v>629</v>
+      </c>
+      <c r="C294" t="s">
+        <v>630</v>
+      </c>
+      <c r="D294" t="s">
+        <v>18</v>
+      </c>
+      <c r="E294" t="s">
+        <v>7</v>
+      </c>
+      <c r="F294" t="s">
+        <v>58</v>
+      </c>
+      <c r="G294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B295" t="s">
+        <v>631</v>
+      </c>
+      <c r="C295" t="s">
+        <v>632</v>
+      </c>
+      <c r="D295" t="s">
+        <v>17</v>
+      </c>
+      <c r="E295" t="s">
+        <v>7</v>
+      </c>
+      <c r="F295" t="s">
+        <v>15</v>
+      </c>
+      <c r="G295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B296" t="s">
+        <v>633</v>
+      </c>
+      <c r="C296" t="s">
+        <v>634</v>
+      </c>
+      <c r="D296" t="s">
+        <v>10</v>
+      </c>
+      <c r="E296" t="s">
+        <v>7</v>
+      </c>
+      <c r="F296" t="s">
+        <v>15</v>
+      </c>
+      <c r="G296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B297" t="s">
+        <v>635</v>
+      </c>
+      <c r="C297" t="s">
+        <v>636</v>
+      </c>
+      <c r="D297" t="s">
+        <v>11</v>
+      </c>
+      <c r="E297" t="s">
+        <v>25</v>
+      </c>
+      <c r="F297" t="s">
+        <v>15</v>
+      </c>
+      <c r="G297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B298" t="s">
+        <v>637</v>
+      </c>
+      <c r="C298" t="s">
+        <v>638</v>
+      </c>
+      <c r="D298" t="s">
+        <v>20</v>
+      </c>
+      <c r="E298" t="s">
+        <v>7</v>
+      </c>
+      <c r="F298" t="s">
+        <v>15</v>
+      </c>
+      <c r="G298">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B299" t="s">
+        <v>639</v>
+      </c>
+      <c r="C299" t="s">
+        <v>640</v>
+      </c>
+      <c r="D299" t="s">
+        <v>20</v>
+      </c>
+      <c r="E299" t="s">
+        <v>7</v>
+      </c>
+      <c r="F299" t="s">
+        <v>8</v>
+      </c>
+      <c r="G299">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B300" t="s">
+        <v>641</v>
+      </c>
+      <c r="C300" t="s">
+        <v>642</v>
+      </c>
+      <c r="D300" t="s">
+        <v>6</v>
+      </c>
+      <c r="E300" t="s">
+        <v>7</v>
+      </c>
+      <c r="F300" t="s">
+        <v>15</v>
+      </c>
+      <c r="G300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B301" t="s">
+        <v>643</v>
+      </c>
+      <c r="C301" t="s">
+        <v>644</v>
+      </c>
+      <c r="D301" t="s">
+        <v>16</v>
+      </c>
+      <c r="E301" t="s">
+        <v>14</v>
+      </c>
+      <c r="F301" t="s">
+        <v>15</v>
+      </c>
+      <c r="G301">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B302" t="s">
+        <v>645</v>
+      </c>
+      <c r="C302" t="s">
+        <v>646</v>
+      </c>
+      <c r="D302" t="s">
+        <v>26</v>
+      </c>
+      <c r="E302" t="s">
+        <v>7</v>
+      </c>
+      <c r="F302" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B303" t="s">
+        <v>647</v>
+      </c>
+      <c r="C303" t="s">
+        <v>648</v>
+      </c>
+      <c r="D303" t="s">
+        <v>330</v>
+      </c>
+      <c r="E303" t="s">
+        <v>7</v>
+      </c>
+      <c r="F303" t="s">
+        <v>8</v>
+      </c>
+      <c r="G303">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B304" t="s">
+        <v>649</v>
+      </c>
+      <c r="C304" t="s">
+        <v>650</v>
+      </c>
+      <c r="D304" t="s">
+        <v>20</v>
+      </c>
+      <c r="E304" t="s">
+        <v>7</v>
+      </c>
+      <c r="F304" t="s">
+        <v>15</v>
+      </c>
+      <c r="G304">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B305" t="s">
+        <v>651</v>
+      </c>
+      <c r="C305" t="s">
+        <v>652</v>
+      </c>
+      <c r="D305" t="s">
+        <v>9</v>
+      </c>
+      <c r="E305" t="s">
+        <v>7</v>
+      </c>
+      <c r="F305" t="s">
+        <v>15</v>
+      </c>
+      <c r="G305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B306" t="s">
+        <v>653</v>
+      </c>
+      <c r="C306" t="s">
+        <v>654</v>
+      </c>
+      <c r="D306" t="s">
+        <v>655</v>
+      </c>
+      <c r="E306" t="s">
+        <v>385</v>
+      </c>
+      <c r="F306" t="s">
+        <v>15</v>
+      </c>
+      <c r="G306">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B307" t="s">
+        <v>656</v>
+      </c>
+      <c r="C307" t="s">
+        <v>657</v>
+      </c>
+      <c r="D307" t="s">
+        <v>13</v>
+      </c>
+      <c r="E307" t="s">
+        <v>7</v>
+      </c>
+      <c r="F307" t="s">
+        <v>58</v>
+      </c>
+      <c r="G307">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B308" t="s">
+        <v>658</v>
+      </c>
+      <c r="C308" t="s">
+        <v>659</v>
+      </c>
+      <c r="D308" t="s">
+        <v>17</v>
+      </c>
+      <c r="E308" t="s">
+        <v>7</v>
+      </c>
+      <c r="F308" t="s">
+        <v>58</v>
+      </c>
+      <c r="G308">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B309" t="s">
+        <v>660</v>
+      </c>
+      <c r="C309" t="s">
+        <v>661</v>
+      </c>
+      <c r="D309" t="s">
+        <v>16</v>
+      </c>
+      <c r="E309" t="s">
+        <v>7</v>
+      </c>
+      <c r="F309" t="s">
+        <v>15</v>
+      </c>
+      <c r="G309">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B310" t="s">
+        <v>662</v>
+      </c>
+      <c r="C310" t="s">
+        <v>663</v>
+      </c>
+      <c r="D310" t="s">
+        <v>20</v>
+      </c>
+      <c r="E310" t="s">
+        <v>7</v>
+      </c>
+      <c r="F310" t="s">
+        <v>15</v>
+      </c>
+      <c r="G310">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B311" t="s">
+        <v>664</v>
+      </c>
+      <c r="C311" t="s">
+        <v>665</v>
+      </c>
+      <c r="D311" t="s">
+        <v>19</v>
+      </c>
+      <c r="E311" t="s">
+        <v>7</v>
+      </c>
+      <c r="F311" t="s">
+        <v>15</v>
+      </c>
+      <c r="G311">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B312" t="s">
+        <v>666</v>
+      </c>
+      <c r="C312" t="s">
+        <v>667</v>
+      </c>
+      <c r="D312" t="s">
+        <v>23</v>
+      </c>
+      <c r="E312" t="s">
+        <v>7</v>
+      </c>
+      <c r="F312" t="s">
+        <v>15</v>
+      </c>
+      <c r="G312">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>45995</v>
+      </c>
+      <c r="B313" t="s">
+        <v>668</v>
+      </c>
+      <c r="C313" t="s">
+        <v>669</v>
+      </c>
+      <c r="D313" t="s">
+        <v>6</v>
+      </c>
+      <c r="E313" t="s">
+        <v>7</v>
+      </c>
+      <c r="F313" t="s">
+        <v>15</v>
+      </c>
+      <c r="G313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B314" t="s">
+        <v>670</v>
+      </c>
+      <c r="C314" t="s">
+        <v>671</v>
+      </c>
+      <c r="D314" t="s">
+        <v>22</v>
+      </c>
+      <c r="E314" t="s">
+        <v>7</v>
+      </c>
+      <c r="F314" t="s">
+        <v>15</v>
+      </c>
+      <c r="G314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B315" t="s">
+        <v>672</v>
+      </c>
+      <c r="C315" t="s">
+        <v>673</v>
+      </c>
+      <c r="D315" t="s">
+        <v>19</v>
+      </c>
+      <c r="E315" t="s">
+        <v>7</v>
+      </c>
+      <c r="F315" t="s">
+        <v>15</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B316" t="s">
+        <v>674</v>
+      </c>
+      <c r="C316" t="s">
+        <v>675</v>
+      </c>
+      <c r="D316" t="s">
+        <v>6</v>
+      </c>
+      <c r="E316" t="s">
+        <v>7</v>
+      </c>
+      <c r="F316" t="s">
+        <v>15</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B317" t="s">
+        <v>676</v>
+      </c>
+      <c r="C317" t="s">
+        <v>677</v>
+      </c>
+      <c r="D317" t="s">
+        <v>26</v>
+      </c>
+      <c r="E317" t="s">
+        <v>7</v>
+      </c>
+      <c r="F317" t="s">
+        <v>15</v>
+      </c>
+      <c r="G317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B318" t="s">
+        <v>678</v>
+      </c>
+      <c r="C318" t="s">
+        <v>679</v>
+      </c>
+      <c r="D318" t="s">
+        <v>23</v>
+      </c>
+      <c r="E318" t="s">
+        <v>7</v>
+      </c>
+      <c r="F318" t="s">
+        <v>15</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="1">
+        <v>45996</v>
+      </c>
+      <c r="B319" t="s">
+        <v>680</v>
+      </c>
+      <c r="C319" t="s">
+        <v>681</v>
+      </c>
+      <c r="D319" t="s">
+        <v>9</v>
+      </c>
+      <c r="E319" t="s">
+        <v>7</v>
+      </c>
+      <c r="F319" t="s">
+        <v>15</v>
+      </c>
+      <c r="G319">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizacao operacional, bd_cc e base qualificacao 08/12/2025
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2025-12.xlsx
+++ b/first-atlas/producao_2025-12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12E2794-399E-4AC2-BEEA-A0AD84F467E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834E5235-BC25-4AB4-8A49-70897F682BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$1473</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$1093</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2005" uniqueCount="845">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -2457,6 +2457,123 @@
   </si>
   <si>
     <t>C H LAVORINI ASSESSORIA E GESTAO COMERCIAL</t>
+  </si>
+  <si>
+    <t>19809970000160</t>
+  </si>
+  <si>
+    <t>CASTANHAL MATERIAIS DE CONSTRUCOES LTDA.</t>
+  </si>
+  <si>
+    <t>28167000000108</t>
+  </si>
+  <si>
+    <t>MANASSES DE SOUSA LANNES</t>
+  </si>
+  <si>
+    <t>34765882000106</t>
+  </si>
+  <si>
+    <t>THAIS DRUMOND FREITAS</t>
+  </si>
+  <si>
+    <t>31938737000183</t>
+  </si>
+  <si>
+    <t>SUELLEM NASCIMENTO MATHIAS</t>
+  </si>
+  <si>
+    <t>26107072000126</t>
+  </si>
+  <si>
+    <t>26.107.072 LEIR ANTONIO DE MOURA</t>
+  </si>
+  <si>
+    <t>33057968000103</t>
+  </si>
+  <si>
+    <t>C E DA SILVA COSTA REFRIGERACAO</t>
+  </si>
+  <si>
+    <t>34990890000148</t>
+  </si>
+  <si>
+    <t>T.R.C. TURCZIM LTDA</t>
+  </si>
+  <si>
+    <t>32913844000110</t>
+  </si>
+  <si>
+    <t>32.913.844 MARCOS DE LIMA</t>
+  </si>
+  <si>
+    <t>28120198000166</t>
+  </si>
+  <si>
+    <t>AMANDA FERREIRA SANTOS 40890551804</t>
+  </si>
+  <si>
+    <t>34454904000109</t>
+  </si>
+  <si>
+    <t>EDUARDO MARTINS SOARES</t>
+  </si>
+  <si>
+    <t>34813937000106</t>
+  </si>
+  <si>
+    <t>WAGNER ADAM BERWALDT</t>
+  </si>
+  <si>
+    <t>24876011000106</t>
+  </si>
+  <si>
+    <t>WILLYAN JOSE RODRIGUES DE SOUZA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>34827921000144</t>
+  </si>
+  <si>
+    <t>ROMUALDO MORAIS DE SOUSA</t>
+  </si>
+  <si>
+    <t>28000083000138</t>
+  </si>
+  <si>
+    <t>ADEGA DO TIGRINHO INDAIATUBA LTDA</t>
+  </si>
+  <si>
+    <t>34187938000184</t>
+  </si>
+  <si>
+    <t>SANTANA TRANSPORTES E MATERIAIS CONSTRUCAO LTDA</t>
+  </si>
+  <si>
+    <t>31970553000109</t>
+  </si>
+  <si>
+    <t>J D DE S NOLETO BASTOS CONTABILIDADE</t>
+  </si>
+  <si>
+    <t>34741698000118</t>
+  </si>
+  <si>
+    <t>MARIA ROSANE ABADE DA ROSA</t>
+  </si>
+  <si>
+    <t>34469203000143</t>
+  </si>
+  <si>
+    <t>MIRANGUINHA FESTAS  ARTIGOS PARA FESTAS LTDA</t>
+  </si>
+  <si>
+    <t>08669859000108</t>
+  </si>
+  <si>
+    <t>FELIX RECICLAGEM INDUSTRIA E COMERCIO DE PLASTICOS LTDA</t>
+  </si>
+  <si>
+    <t>Contrato social atualizado e registrado no orgao competente</t>
   </si>
 </sst>
 </file>
@@ -2828,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCD3CE2-DBA2-4F4F-B6A3-11EE884EA727}">
-  <dimension ref="A1:G381"/>
+  <dimension ref="A1:G399"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="G2" sqref="G2:G399"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,13 +3066,13 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45992</v>
       </c>
@@ -3294,7 +3411,7 @@
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>175</v>
+        <v>8</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -5617,7 +5734,7 @@
         <v>7</v>
       </c>
       <c r="F121" t="s">
-        <v>175</v>
+        <v>56</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -7779,7 +7896,7 @@
         <v>7</v>
       </c>
       <c r="F215" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="G215">
         <v>0</v>
@@ -8503,16 +8620,16 @@
         <v>45995</v>
       </c>
       <c r="B247" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="C247" t="s">
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="D247" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="E247" t="s">
-        <v>7</v>
+        <v>186</v>
       </c>
       <c r="F247" t="s">
         <v>15</v>
@@ -8526,19 +8643,19 @@
         <v>45995</v>
       </c>
       <c r="B248" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="C248" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D248" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
       <c r="E248" t="s">
-        <v>186</v>
+        <v>7</v>
       </c>
       <c r="F248" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G248">
         <v>0</v>
@@ -8549,10 +8666,10 @@
         <v>45995</v>
       </c>
       <c r="B249" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C249" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D249" t="s">
         <v>10</v>
@@ -8561,7 +8678,7 @@
         <v>7</v>
       </c>
       <c r="F249" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G249">
         <v>0</v>
@@ -8572,22 +8689,22 @@
         <v>45995</v>
       </c>
       <c r="B250" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="C250" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="D250" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E250" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F250" t="s">
-        <v>15</v>
-      </c>
-      <c r="G250">
-        <v>0</v>
+        <v>547</v>
+      </c>
+      <c r="G250" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -8595,22 +8712,22 @@
         <v>45995</v>
       </c>
       <c r="B251" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="C251" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
       <c r="D251" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E251" t="s">
         <v>24</v>
       </c>
       <c r="F251" t="s">
-        <v>547</v>
-      </c>
-      <c r="G251" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G251">
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -8618,19 +8735,19 @@
         <v>45995</v>
       </c>
       <c r="B252" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="C252" t="s">
-        <v>534</v>
+        <v>549</v>
       </c>
       <c r="D252" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E252" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F252" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G252">
         <v>0</v>
@@ -8641,19 +8758,19 @@
         <v>45995</v>
       </c>
       <c r="B253" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C253" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="D253" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E253" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F253" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="G253">
         <v>0</v>
@@ -8664,19 +8781,19 @@
         <v>45995</v>
       </c>
       <c r="B254" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="C254" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D254" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E254" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F254" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G254">
         <v>0</v>
@@ -8687,19 +8804,19 @@
         <v>45995</v>
       </c>
       <c r="B255" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="C255" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="D255" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E255" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F255" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -8710,19 +8827,19 @@
         <v>45995</v>
       </c>
       <c r="B256" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="C256" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D256" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E256" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F256" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G256">
         <v>0</v>
@@ -8733,16 +8850,16 @@
         <v>45995</v>
       </c>
       <c r="B257" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C257" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="D257" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E257" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F257" t="s">
         <v>56</v>
@@ -8756,10 +8873,10 @@
         <v>45995</v>
       </c>
       <c r="B258" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C258" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D258" t="s">
         <v>6</v>
@@ -8768,7 +8885,7 @@
         <v>7</v>
       </c>
       <c r="F258" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G258">
         <v>0</v>
@@ -8779,13 +8896,13 @@
         <v>45995</v>
       </c>
       <c r="B259" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C259" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D259" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E259" t="s">
         <v>7</v>
@@ -8802,13 +8919,13 @@
         <v>45995</v>
       </c>
       <c r="B260" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C260" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D260" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E260" t="s">
         <v>7</v>
@@ -8825,19 +8942,19 @@
         <v>45995</v>
       </c>
       <c r="B261" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C261" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D261" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E261" t="s">
         <v>7</v>
       </c>
       <c r="F261" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G261">
         <v>0</v>
@@ -8848,19 +8965,19 @@
         <v>45995</v>
       </c>
       <c r="B262" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C262" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="D262" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E262" t="s">
         <v>7</v>
       </c>
       <c r="F262" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G262">
         <v>0</v>
@@ -8871,13 +8988,13 @@
         <v>45995</v>
       </c>
       <c r="B263" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="C263" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="D263" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E263" t="s">
         <v>7</v>
@@ -8894,13 +9011,13 @@
         <v>45995</v>
       </c>
       <c r="B264" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="C264" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="D264" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E264" t="s">
         <v>7</v>
@@ -8917,16 +9034,16 @@
         <v>45995</v>
       </c>
       <c r="B265" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="C265" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="D265" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E265" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F265" t="s">
         <v>15</v>
@@ -8940,19 +9057,19 @@
         <v>45995</v>
       </c>
       <c r="B266" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C266" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="D266" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E266" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F266" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G266">
         <v>0</v>
@@ -8963,19 +9080,19 @@
         <v>45995</v>
       </c>
       <c r="B267" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C267" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
       <c r="D267" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E267" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F267" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G267">
         <v>0</v>
@@ -8986,16 +9103,16 @@
         <v>45995</v>
       </c>
       <c r="B268" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C268" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D268" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E268" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F268" t="s">
         <v>15</v>
@@ -9009,13 +9126,13 @@
         <v>45995</v>
       </c>
       <c r="B269" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C269" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="D269" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E269" t="s">
         <v>7</v>
@@ -9032,19 +9149,19 @@
         <v>45995</v>
       </c>
       <c r="B270" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C270" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="D270" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E270" t="s">
         <v>7</v>
       </c>
       <c r="F270" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G270">
         <v>0</v>
@@ -9055,19 +9172,19 @@
         <v>45995</v>
       </c>
       <c r="B271" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C271" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="D271" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E271" t="s">
         <v>7</v>
       </c>
       <c r="F271" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G271">
         <v>0</v>
@@ -9078,13 +9195,13 @@
         <v>45995</v>
       </c>
       <c r="B272" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="C272" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="D272" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E272" t="s">
         <v>7</v>
@@ -9101,19 +9218,19 @@
         <v>45995</v>
       </c>
       <c r="B273" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="C273" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="D273" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E273" t="s">
         <v>7</v>
       </c>
       <c r="F273" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G273">
         <v>0</v>
@@ -9124,19 +9241,19 @@
         <v>45995</v>
       </c>
       <c r="B274" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="C274" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="D274" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E274" t="s">
         <v>7</v>
       </c>
       <c r="F274" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G274">
         <v>0</v>
@@ -9147,13 +9264,13 @@
         <v>45995</v>
       </c>
       <c r="B275" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C275" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="D275" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E275" t="s">
         <v>7</v>
@@ -9170,19 +9287,19 @@
         <v>45995</v>
       </c>
       <c r="B276" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="C276" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="D276" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E276" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F276" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G276">
         <v>0</v>
@@ -9193,19 +9310,19 @@
         <v>45995</v>
       </c>
       <c r="B277" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C277" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D277" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E277" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F277" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G277">
         <v>0</v>
@@ -9216,13 +9333,13 @@
         <v>45995</v>
       </c>
       <c r="B278" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C278" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D278" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E278" t="s">
         <v>7</v>
@@ -9239,13 +9356,13 @@
         <v>45995</v>
       </c>
       <c r="B279" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C279" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D279" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E279" t="s">
         <v>7</v>
@@ -9262,19 +9379,19 @@
         <v>45995</v>
       </c>
       <c r="B280" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C280" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D280" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E280" t="s">
         <v>7</v>
       </c>
       <c r="F280" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G280">
         <v>0</v>
@@ -9285,22 +9402,22 @@
         <v>45995</v>
       </c>
       <c r="B281" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C281" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="D281" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E281" t="s">
         <v>7</v>
       </c>
       <c r="F281" t="s">
-        <v>8</v>
-      </c>
-      <c r="G281">
-        <v>0</v>
+        <v>547</v>
+      </c>
+      <c r="G281" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
@@ -9308,22 +9425,22 @@
         <v>45995</v>
       </c>
       <c r="B282" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="C282" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="D282" t="s">
-        <v>6</v>
+        <v>610</v>
       </c>
       <c r="E282" t="s">
-        <v>7</v>
+        <v>462</v>
       </c>
       <c r="F282" t="s">
-        <v>547</v>
-      </c>
-      <c r="G282" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G282">
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
@@ -9331,16 +9448,16 @@
         <v>45995</v>
       </c>
       <c r="B283" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="C283" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="D283" t="s">
-        <v>610</v>
+        <v>10</v>
       </c>
       <c r="E283" t="s">
-        <v>462</v>
+        <v>7</v>
       </c>
       <c r="F283" t="s">
         <v>15</v>
@@ -9354,13 +9471,13 @@
         <v>45995</v>
       </c>
       <c r="B284" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C284" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="D284" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E284" t="s">
         <v>7</v>
@@ -9377,13 +9494,13 @@
         <v>45995</v>
       </c>
       <c r="B285" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="C285" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="D285" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E285" t="s">
         <v>7</v>
@@ -9400,10 +9517,10 @@
         <v>45995</v>
       </c>
       <c r="B286" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="C286" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="D286" t="s">
         <v>10</v>
@@ -9423,13 +9540,13 @@
         <v>45995</v>
       </c>
       <c r="B287" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="C287" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="D287" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E287" t="s">
         <v>7</v>
@@ -9446,19 +9563,19 @@
         <v>45995</v>
       </c>
       <c r="B288" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C288" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="D288" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E288" t="s">
         <v>7</v>
       </c>
       <c r="F288" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G288">
         <v>0</v>
@@ -9469,19 +9586,19 @@
         <v>45995</v>
       </c>
       <c r="B289" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="C289" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="D289" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E289" t="s">
         <v>7</v>
       </c>
       <c r="F289" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G289">
         <v>0</v>
@@ -9492,19 +9609,19 @@
         <v>45995</v>
       </c>
       <c r="B290" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="C290" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="D290" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E290" t="s">
         <v>7</v>
       </c>
       <c r="F290" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G290">
         <v>0</v>
@@ -9515,19 +9632,19 @@
         <v>45995</v>
       </c>
       <c r="B291" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="C291" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="D291" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E291" t="s">
         <v>7</v>
       </c>
       <c r="F291" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G291">
         <v>0</v>
@@ -9538,13 +9655,13 @@
         <v>45995</v>
       </c>
       <c r="B292" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="C292" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D292" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E292" t="s">
         <v>7</v>
@@ -9561,16 +9678,16 @@
         <v>45995</v>
       </c>
       <c r="B293" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="C293" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D293" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E293" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F293" t="s">
         <v>15</v>
@@ -9584,16 +9701,16 @@
         <v>45995</v>
       </c>
       <c r="B294" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="C294" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="D294" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E294" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F294" t="s">
         <v>15</v>
@@ -9607,10 +9724,10 @@
         <v>45995</v>
       </c>
       <c r="B295" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="C295" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D295" t="s">
         <v>20</v>
@@ -9619,7 +9736,7 @@
         <v>7</v>
       </c>
       <c r="F295" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G295">
         <v>0</v>
@@ -9630,19 +9747,19 @@
         <v>45995</v>
       </c>
       <c r="B296" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="C296" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D296" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E296" t="s">
         <v>7</v>
       </c>
       <c r="F296" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G296">
         <v>0</v>
@@ -9653,16 +9770,16 @@
         <v>45995</v>
       </c>
       <c r="B297" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="C297" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="D297" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E297" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F297" t="s">
         <v>15</v>
@@ -9676,19 +9793,19 @@
         <v>45995</v>
       </c>
       <c r="B298" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="C298" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="D298" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E298" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F298" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G298">
         <v>0</v>
@@ -9699,19 +9816,19 @@
         <v>45995</v>
       </c>
       <c r="B299" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="C299" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
       <c r="D299" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E299" t="s">
         <v>7</v>
       </c>
       <c r="F299" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G299">
         <v>0</v>
@@ -9722,19 +9839,19 @@
         <v>45995</v>
       </c>
       <c r="B300" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
       <c r="C300" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="D300" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E300" t="s">
         <v>7</v>
       </c>
       <c r="F300" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G300">
         <v>0</v>
@@ -9745,13 +9862,13 @@
         <v>45995</v>
       </c>
       <c r="B301" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="C301" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="D301" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E301" t="s">
         <v>7</v>
@@ -9768,16 +9885,16 @@
         <v>45995</v>
       </c>
       <c r="B302" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
       <c r="C302" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
       <c r="D302" t="s">
-        <v>9</v>
+        <v>651</v>
       </c>
       <c r="E302" t="s">
-        <v>7</v>
+        <v>382</v>
       </c>
       <c r="F302" t="s">
         <v>15</v>
@@ -9791,19 +9908,19 @@
         <v>45995</v>
       </c>
       <c r="B303" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="C303" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="D303" t="s">
-        <v>651</v>
+        <v>13</v>
       </c>
       <c r="E303" t="s">
-        <v>382</v>
+        <v>7</v>
       </c>
       <c r="F303" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="G303">
         <v>0</v>
@@ -9814,13 +9931,13 @@
         <v>45995</v>
       </c>
       <c r="B304" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="C304" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
       <c r="D304" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E304" t="s">
         <v>7</v>
@@ -9837,13 +9954,13 @@
         <v>45995</v>
       </c>
       <c r="B305" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
       <c r="C305" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="D305" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E305" t="s">
         <v>7</v>
@@ -9860,19 +9977,19 @@
         <v>45995</v>
       </c>
       <c r="B306" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="C306" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="D306" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E306" t="s">
         <v>7</v>
       </c>
       <c r="F306" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G306">
         <v>0</v>
@@ -9883,13 +10000,13 @@
         <v>45995</v>
       </c>
       <c r="B307" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="C307" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
       <c r="D307" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E307" t="s">
         <v>7</v>
@@ -9906,13 +10023,13 @@
         <v>45995</v>
       </c>
       <c r="B308" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="C308" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="D308" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E308" t="s">
         <v>7</v>
@@ -9929,13 +10046,13 @@
         <v>45995</v>
       </c>
       <c r="B309" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
       <c r="C309" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
       <c r="D309" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E309" t="s">
         <v>7</v>
@@ -9949,16 +10066,16 @@
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
-        <v>45995</v>
+        <v>45996</v>
       </c>
       <c r="B310" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
       <c r="C310" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
       <c r="D310" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E310" t="s">
         <v>7</v>
@@ -9975,13 +10092,13 @@
         <v>45996</v>
       </c>
       <c r="B311" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
       <c r="C311" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="D311" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E311" t="s">
         <v>7</v>
@@ -9998,13 +10115,13 @@
         <v>45996</v>
       </c>
       <c r="B312" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
       <c r="C312" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
       <c r="D312" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E312" t="s">
         <v>7</v>
@@ -10021,13 +10138,13 @@
         <v>45996</v>
       </c>
       <c r="B313" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
       <c r="C313" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="D313" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E313" t="s">
         <v>7</v>
@@ -10044,13 +10161,13 @@
         <v>45996</v>
       </c>
       <c r="B314" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
       <c r="C314" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
       <c r="D314" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E314" t="s">
         <v>7</v>
@@ -10067,13 +10184,13 @@
         <v>45996</v>
       </c>
       <c r="B315" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="C315" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="D315" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E315" t="s">
         <v>7</v>
@@ -10090,13 +10207,13 @@
         <v>45996</v>
       </c>
       <c r="B316" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="C316" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
       <c r="D316" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E316" t="s">
         <v>7</v>
@@ -10113,13 +10230,13 @@
         <v>45996</v>
       </c>
       <c r="B317" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C317" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="D317" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E317" t="s">
         <v>7</v>
@@ -10136,16 +10253,16 @@
         <v>45996</v>
       </c>
       <c r="B318" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="C318" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="D318" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E318" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F318" t="s">
         <v>15</v>
@@ -10159,16 +10276,16 @@
         <v>45996</v>
       </c>
       <c r="B319" t="s">
-        <v>685</v>
+        <v>538</v>
       </c>
       <c r="C319" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="D319" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E319" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F319" t="s">
         <v>15</v>
@@ -10182,19 +10299,19 @@
         <v>45996</v>
       </c>
       <c r="B320" t="s">
-        <v>538</v>
+        <v>688</v>
       </c>
       <c r="C320" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="D320" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E320" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F320" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G320">
         <v>0</v>
@@ -10205,19 +10322,19 @@
         <v>45996</v>
       </c>
       <c r="B321" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="C321" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="D321" t="s">
         <v>6</v>
       </c>
       <c r="E321" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F321" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G321">
         <v>0</v>
@@ -10228,19 +10345,19 @@
         <v>45996</v>
       </c>
       <c r="B322" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="C322" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="D322" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E322" t="s">
         <v>7</v>
       </c>
       <c r="F322" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="G322">
         <v>0</v>
@@ -10251,19 +10368,19 @@
         <v>45996</v>
       </c>
       <c r="B323" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="C323" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="D323" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E323" t="s">
         <v>7</v>
       </c>
       <c r="F323" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G323">
         <v>0</v>
@@ -10274,13 +10391,13 @@
         <v>45996</v>
       </c>
       <c r="B324" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="C324" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="D324" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E324" t="s">
         <v>7</v>
@@ -10297,13 +10414,13 @@
         <v>45996</v>
       </c>
       <c r="B325" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="C325" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D325" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E325" t="s">
         <v>7</v>
@@ -10320,16 +10437,16 @@
         <v>45996</v>
       </c>
       <c r="B326" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C326" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="D326" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E326" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F326" t="s">
         <v>15</v>
@@ -10343,16 +10460,16 @@
         <v>45996</v>
       </c>
       <c r="B327" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="C327" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="D327" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E327" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F327" t="s">
         <v>15</v>
@@ -10366,16 +10483,16 @@
         <v>45996</v>
       </c>
       <c r="B328" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="C328" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="D328" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E328" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F328" t="s">
         <v>15</v>
@@ -10389,13 +10506,13 @@
         <v>45996</v>
       </c>
       <c r="B329" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C329" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="D329" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E329" t="s">
         <v>14</v>
@@ -10412,19 +10529,19 @@
         <v>45996</v>
       </c>
       <c r="B330" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="C330" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="D330" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E330" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F330" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G330">
         <v>0</v>
@@ -10435,22 +10552,22 @@
         <v>45996</v>
       </c>
       <c r="B331" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="C331" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="D331" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E331" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F331" t="s">
-        <v>15</v>
-      </c>
-      <c r="G331">
-        <v>0</v>
+        <v>537</v>
+      </c>
+      <c r="G331" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.25">
@@ -10458,19 +10575,19 @@
         <v>45996</v>
       </c>
       <c r="B332" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C332" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="D332" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E332" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F332" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G332">
         <v>0</v>
@@ -10481,19 +10598,19 @@
         <v>45996</v>
       </c>
       <c r="B333" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="C333" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="D333" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E333" t="s">
         <v>7</v>
       </c>
       <c r="F333" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G333">
         <v>0</v>
@@ -10504,16 +10621,16 @@
         <v>45996</v>
       </c>
       <c r="B334" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C334" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="D334" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E334" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F334" t="s">
         <v>15</v>
@@ -10527,19 +10644,19 @@
         <v>45996</v>
       </c>
       <c r="B335" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C335" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="D335" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E335" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F335" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G335">
         <v>0</v>
@@ -10550,16 +10667,16 @@
         <v>45996</v>
       </c>
       <c r="B336" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="C336" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D336" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="E336" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F336" t="s">
         <v>56</v>
@@ -10573,19 +10690,19 @@
         <v>45996</v>
       </c>
       <c r="B337" t="s">
-        <v>720</v>
+        <v>51</v>
       </c>
       <c r="C337" t="s">
-        <v>721</v>
+        <v>52</v>
       </c>
       <c r="D337" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E337" t="s">
         <v>7</v>
       </c>
       <c r="F337" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="G337">
         <v>0</v>
@@ -10596,19 +10713,19 @@
         <v>45996</v>
       </c>
       <c r="B338" t="s">
-        <v>51</v>
+        <v>722</v>
       </c>
       <c r="C338" t="s">
-        <v>52</v>
+        <v>723</v>
       </c>
       <c r="D338" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E338" t="s">
         <v>7</v>
       </c>
       <c r="F338" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G338">
         <v>0</v>
@@ -10619,13 +10736,13 @@
         <v>45996</v>
       </c>
       <c r="B339" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C339" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="D339" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E339" t="s">
         <v>7</v>
@@ -10642,10 +10759,10 @@
         <v>45996</v>
       </c>
       <c r="B340" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="C340" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="D340" t="s">
         <v>10</v>
@@ -10654,7 +10771,7 @@
         <v>7</v>
       </c>
       <c r="F340" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G340">
         <v>0</v>
@@ -10665,19 +10782,19 @@
         <v>45996</v>
       </c>
       <c r="B341" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C341" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D341" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E341" t="s">
         <v>7</v>
       </c>
       <c r="F341" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G341">
         <v>0</v>
@@ -10688,19 +10805,19 @@
         <v>45996</v>
       </c>
       <c r="B342" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C342" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="D342" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E342" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F342" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G342">
         <v>0</v>
@@ -10711,19 +10828,19 @@
         <v>45996</v>
       </c>
       <c r="B343" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="C343" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="D343" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E343" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F343" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G343">
         <v>0</v>
@@ -10734,19 +10851,19 @@
         <v>45996</v>
       </c>
       <c r="B344" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C344" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="D344" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E344" t="s">
         <v>7</v>
       </c>
       <c r="F344" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G344">
         <v>0</v>
@@ -10757,19 +10874,19 @@
         <v>45996</v>
       </c>
       <c r="B345" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="C345" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="D345" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E345" t="s">
         <v>7</v>
       </c>
       <c r="F345" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G345">
         <v>0</v>
@@ -10780,13 +10897,13 @@
         <v>45996</v>
       </c>
       <c r="B346" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="C346" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="D346" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E346" t="s">
         <v>7</v>
@@ -10803,13 +10920,13 @@
         <v>45996</v>
       </c>
       <c r="B347" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="C347" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="D347" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E347" t="s">
         <v>7</v>
@@ -10826,13 +10943,13 @@
         <v>45996</v>
       </c>
       <c r="B348" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C348" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D348" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E348" t="s">
         <v>7</v>
@@ -10849,22 +10966,22 @@
         <v>45996</v>
       </c>
       <c r="B349" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C349" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="D349" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="E349" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F349" t="s">
-        <v>15</v>
-      </c>
-      <c r="G349">
-        <v>0</v>
+        <v>537</v>
+      </c>
+      <c r="G349" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
@@ -10872,22 +10989,22 @@
         <v>45996</v>
       </c>
       <c r="B350" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="C350" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="D350" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E350" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F350" t="s">
-        <v>56</v>
-      </c>
-      <c r="G350" t="s">
-        <v>536</v>
+        <v>15</v>
+      </c>
+      <c r="G350">
+        <v>0</v>
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.25">
@@ -10895,13 +11012,13 @@
         <v>45996</v>
       </c>
       <c r="B351" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="C351" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="D351" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E351" t="s">
         <v>7</v>
@@ -10918,13 +11035,13 @@
         <v>45996</v>
       </c>
       <c r="B352" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="C352" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D352" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E352" t="s">
         <v>7</v>
@@ -10941,10 +11058,10 @@
         <v>45996</v>
       </c>
       <c r="B353" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="C353" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="D353" t="s">
         <v>16</v>
@@ -10964,13 +11081,13 @@
         <v>45996</v>
       </c>
       <c r="B354" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="C354" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="D354" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E354" t="s">
         <v>7</v>
@@ -10987,10 +11104,10 @@
         <v>45996</v>
       </c>
       <c r="B355" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C355" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="D355" t="s">
         <v>10</v>
@@ -10999,7 +11116,7 @@
         <v>7</v>
       </c>
       <c r="F355" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G355">
         <v>0</v>
@@ -11010,19 +11127,19 @@
         <v>45996</v>
       </c>
       <c r="B356" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="C356" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="D356" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E356" t="s">
         <v>7</v>
       </c>
       <c r="F356" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G356">
         <v>0</v>
@@ -11033,13 +11150,13 @@
         <v>45996</v>
       </c>
       <c r="B357" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C357" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="D357" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E357" t="s">
         <v>7</v>
@@ -11056,13 +11173,13 @@
         <v>45996</v>
       </c>
       <c r="B358" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C358" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="D358" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E358" t="s">
         <v>7</v>
@@ -11079,13 +11196,13 @@
         <v>45996</v>
       </c>
       <c r="B359" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="C359" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="D359" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E359" t="s">
         <v>7</v>
@@ -11102,13 +11219,13 @@
         <v>45996</v>
       </c>
       <c r="B360" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="C360" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="D360" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E360" t="s">
         <v>7</v>
@@ -11125,19 +11242,19 @@
         <v>45996</v>
       </c>
       <c r="B361" t="s">
-        <v>766</v>
+        <v>47</v>
       </c>
       <c r="C361" t="s">
-        <v>767</v>
+        <v>48</v>
       </c>
       <c r="D361" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E361" t="s">
         <v>7</v>
       </c>
       <c r="F361" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G361">
         <v>0</v>
@@ -11148,19 +11265,19 @@
         <v>45996</v>
       </c>
       <c r="B362" t="s">
-        <v>47</v>
+        <v>768</v>
       </c>
       <c r="C362" t="s">
-        <v>48</v>
+        <v>769</v>
       </c>
       <c r="D362" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E362" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F362" t="s">
-        <v>56</v>
+        <v>175</v>
       </c>
       <c r="G362">
         <v>0</v>
@@ -11171,19 +11288,19 @@
         <v>45996</v>
       </c>
       <c r="B363" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C363" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="D363" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E363" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F363" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G363">
         <v>0</v>
@@ -11194,13 +11311,13 @@
         <v>45996</v>
       </c>
       <c r="B364" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="C364" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="D364" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E364" t="s">
         <v>7</v>
@@ -11217,13 +11334,13 @@
         <v>45996</v>
       </c>
       <c r="B365" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="C365" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="D365" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E365" t="s">
         <v>7</v>
@@ -11240,13 +11357,13 @@
         <v>45996</v>
       </c>
       <c r="B366" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="C366" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="D366" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E366" t="s">
         <v>7</v>
@@ -11263,16 +11380,16 @@
         <v>45996</v>
       </c>
       <c r="B367" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="C367" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D367" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E367" t="s">
-        <v>7</v>
+        <v>455</v>
       </c>
       <c r="F367" t="s">
         <v>15</v>
@@ -11286,16 +11403,16 @@
         <v>45996</v>
       </c>
       <c r="B368" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="C368" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="D368" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E368" t="s">
-        <v>455</v>
+        <v>7</v>
       </c>
       <c r="F368" t="s">
         <v>15</v>
@@ -11309,19 +11426,19 @@
         <v>45996</v>
       </c>
       <c r="B369" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C369" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="D369" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E369" t="s">
         <v>7</v>
       </c>
       <c r="F369" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G369">
         <v>0</v>
@@ -11332,19 +11449,19 @@
         <v>45996</v>
       </c>
       <c r="B370" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C370" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D370" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E370" t="s">
         <v>7</v>
       </c>
       <c r="F370" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G370">
         <v>0</v>
@@ -11355,13 +11472,13 @@
         <v>45996</v>
       </c>
       <c r="B371" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="C371" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="D371" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E371" t="s">
         <v>7</v>
@@ -11378,13 +11495,13 @@
         <v>45996</v>
       </c>
       <c r="B372" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="C372" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="D372" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E372" t="s">
         <v>7</v>
@@ -11401,13 +11518,13 @@
         <v>45996</v>
       </c>
       <c r="B373" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="C373" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="D373" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E373" t="s">
         <v>7</v>
@@ -11424,13 +11541,13 @@
         <v>45996</v>
       </c>
       <c r="B374" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C374" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="D374" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E374" t="s">
         <v>7</v>
@@ -11447,13 +11564,13 @@
         <v>45996</v>
       </c>
       <c r="B375" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="C375" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="D375" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E375" t="s">
         <v>7</v>
@@ -11470,13 +11587,13 @@
         <v>45996</v>
       </c>
       <c r="B376" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C376" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="D376" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E376" t="s">
         <v>7</v>
@@ -11490,16 +11607,16 @@
     </row>
     <row r="377" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
-        <v>45996</v>
+        <v>45997</v>
       </c>
       <c r="B377" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C377" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="D377" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E377" t="s">
         <v>7</v>
@@ -11516,13 +11633,13 @@
         <v>45997</v>
       </c>
       <c r="B378" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C378" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="D378" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E378" t="s">
         <v>7</v>
@@ -11539,13 +11656,13 @@
         <v>45997</v>
       </c>
       <c r="B379" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C379" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="D379" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E379" t="s">
         <v>7</v>
@@ -11562,16 +11679,16 @@
         <v>45997</v>
       </c>
       <c r="B380" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="C380" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="D380" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E380" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F380" t="s">
         <v>15</v>
@@ -11585,21 +11702,435 @@
         <v>45997</v>
       </c>
       <c r="B381" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C381" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D381" t="s">
+        <v>10</v>
+      </c>
+      <c r="E381" t="s">
+        <v>7</v>
+      </c>
+      <c r="F381" t="s">
+        <v>15</v>
+      </c>
+      <c r="G381">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A382" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B382" t="s">
+        <v>808</v>
+      </c>
+      <c r="C382" t="s">
+        <v>809</v>
+      </c>
+      <c r="D382" t="s">
+        <v>19</v>
+      </c>
+      <c r="E382" t="s">
+        <v>7</v>
+      </c>
+      <c r="F382" t="s">
+        <v>15</v>
+      </c>
+      <c r="G382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A383" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B383" t="s">
+        <v>810</v>
+      </c>
+      <c r="C383" t="s">
+        <v>811</v>
+      </c>
+      <c r="D383" t="s">
+        <v>10</v>
+      </c>
+      <c r="E383" t="s">
+        <v>7</v>
+      </c>
+      <c r="F383" t="s">
+        <v>15</v>
+      </c>
+      <c r="G383">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A384" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B384" t="s">
+        <v>812</v>
+      </c>
+      <c r="C384" t="s">
+        <v>813</v>
+      </c>
+      <c r="D384" t="s">
+        <v>22</v>
+      </c>
+      <c r="E384" t="s">
+        <v>7</v>
+      </c>
+      <c r="F384" t="s">
+        <v>15</v>
+      </c>
+      <c r="G384">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A385" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B385" t="s">
+        <v>814</v>
+      </c>
+      <c r="C385" t="s">
+        <v>815</v>
+      </c>
+      <c r="D385" t="s">
+        <v>19</v>
+      </c>
+      <c r="E385" t="s">
+        <v>7</v>
+      </c>
+      <c r="F385" t="s">
+        <v>15</v>
+      </c>
+      <c r="G385">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A386" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B386" t="s">
+        <v>816</v>
+      </c>
+      <c r="C386" t="s">
+        <v>817</v>
+      </c>
+      <c r="D386" t="s">
+        <v>19</v>
+      </c>
+      <c r="E386" t="s">
+        <v>7</v>
+      </c>
+      <c r="F386" t="s">
+        <v>15</v>
+      </c>
+      <c r="G386">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A387" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B387" t="s">
+        <v>818</v>
+      </c>
+      <c r="C387" t="s">
+        <v>819</v>
+      </c>
+      <c r="D387" t="s">
+        <v>26</v>
+      </c>
+      <c r="E387" t="s">
+        <v>7</v>
+      </c>
+      <c r="F387" t="s">
+        <v>15</v>
+      </c>
+      <c r="G387">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A388" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B388" t="s">
+        <v>820</v>
+      </c>
+      <c r="C388" t="s">
+        <v>821</v>
+      </c>
+      <c r="D388" t="s">
+        <v>26</v>
+      </c>
+      <c r="E388" t="s">
+        <v>14</v>
+      </c>
+      <c r="F388" t="s">
+        <v>15</v>
+      </c>
+      <c r="G388">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A389" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B389" t="s">
+        <v>822</v>
+      </c>
+      <c r="C389" t="s">
+        <v>823</v>
+      </c>
+      <c r="D389" t="s">
+        <v>10</v>
+      </c>
+      <c r="E389" t="s">
+        <v>7</v>
+      </c>
+      <c r="F389" t="s">
+        <v>15</v>
+      </c>
+      <c r="G389">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A390" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B390" t="s">
+        <v>824</v>
+      </c>
+      <c r="C390" t="s">
+        <v>825</v>
+      </c>
+      <c r="D390" t="s">
+        <v>10</v>
+      </c>
+      <c r="E390" t="s">
+        <v>7</v>
+      </c>
+      <c r="F390" t="s">
+        <v>15</v>
+      </c>
+      <c r="G390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A391" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B391" t="s">
+        <v>826</v>
+      </c>
+      <c r="C391" t="s">
+        <v>827</v>
+      </c>
+      <c r="D391" t="s">
+        <v>22</v>
+      </c>
+      <c r="E391" t="s">
+        <v>7</v>
+      </c>
+      <c r="F391" t="s">
+        <v>8</v>
+      </c>
+      <c r="G391">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A392" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B392" t="s">
+        <v>828</v>
+      </c>
+      <c r="C392" t="s">
+        <v>829</v>
+      </c>
+      <c r="D392" t="s">
+        <v>10</v>
+      </c>
+      <c r="E392" t="s">
+        <v>7</v>
+      </c>
+      <c r="F392" t="s">
+        <v>56</v>
+      </c>
+      <c r="G392">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A393" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B393" t="s">
+        <v>830</v>
+      </c>
+      <c r="C393" t="s">
+        <v>831</v>
+      </c>
+      <c r="D393" t="s">
+        <v>22</v>
+      </c>
+      <c r="E393" t="s">
+        <v>7</v>
+      </c>
+      <c r="F393" t="s">
+        <v>15</v>
+      </c>
+      <c r="G393">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A394" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B394" t="s">
+        <v>832</v>
+      </c>
+      <c r="C394" t="s">
+        <v>833</v>
+      </c>
+      <c r="D394" t="s">
         <v>11</v>
       </c>
-      <c r="E381" t="s">
-        <v>24</v>
-      </c>
-      <c r="F381" t="s">
-        <v>15</v>
-      </c>
-      <c r="G381">
+      <c r="E394" t="s">
+        <v>7</v>
+      </c>
+      <c r="F394" t="s">
+        <v>15</v>
+      </c>
+      <c r="G394">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A395" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B395" t="s">
+        <v>834</v>
+      </c>
+      <c r="C395" t="s">
+        <v>835</v>
+      </c>
+      <c r="D395" t="s">
+        <v>19</v>
+      </c>
+      <c r="E395" t="s">
+        <v>7</v>
+      </c>
+      <c r="F395" t="s">
+        <v>15</v>
+      </c>
+      <c r="G395">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A396" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B396" t="s">
+        <v>836</v>
+      </c>
+      <c r="C396" t="s">
+        <v>837</v>
+      </c>
+      <c r="D396" t="s">
+        <v>22</v>
+      </c>
+      <c r="E396" t="s">
+        <v>7</v>
+      </c>
+      <c r="F396" t="s">
+        <v>8</v>
+      </c>
+      <c r="G396">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A397" s="1">
+        <v>45997</v>
+      </c>
+      <c r="B397" t="s">
+        <v>838</v>
+      </c>
+      <c r="C397" t="s">
+        <v>839</v>
+      </c>
+      <c r="D397" t="s">
+        <v>22</v>
+      </c>
+      <c r="E397" t="s">
+        <v>7</v>
+      </c>
+      <c r="F397" t="s">
+        <v>15</v>
+      </c>
+      <c r="G397">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A398" s="1">
+        <v>45999</v>
+      </c>
+      <c r="B398" t="s">
+        <v>840</v>
+      </c>
+      <c r="C398" t="s">
+        <v>841</v>
+      </c>
+      <c r="D398" t="s">
+        <v>9</v>
+      </c>
+      <c r="E398" t="s">
+        <v>7</v>
+      </c>
+      <c r="F398" t="s">
+        <v>15</v>
+      </c>
+      <c r="G398">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A399" s="1">
+        <v>45999</v>
+      </c>
+      <c r="B399" t="s">
+        <v>842</v>
+      </c>
+      <c r="C399" t="s">
+        <v>843</v>
+      </c>
+      <c r="D399" t="s">
+        <v>20</v>
+      </c>
+      <c r="E399" t="s">
+        <v>7</v>
+      </c>
+      <c r="F399" t="s">
+        <v>15</v>
+      </c>
+      <c r="G399">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated balde and producao - base 09/12/2025
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2025-12.xlsx
+++ b/first-atlas/producao_2025-12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612E7695-4F3B-4133-A324-6721F0834C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D815761-0ACE-4FF0-934D-22BAD2945986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="992">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -1646,9 +1646,6 @@
     <t>JACG CONSULTORIA E ASSESSORIA LTDA</t>
   </si>
   <si>
-    <t>Procuracao com poderes para abrir e movimentar contas, pois identificamos que a representacao da sua empresa deve ser em conjunto pelos socios. O documento deve ser assinado pelos representantes legais nomeados no contrato social, assinada digitalmente GOV.BR, o documento deve ser enviado PDF.</t>
-  </si>
-  <si>
     <t>Procuracao com poderes de abrir e movimentar conta corrente junto a instituicoes financeiras com mandato vigente e devidamente assinada&lt;br&gt;&lt;br&gt;Contrato social atualizado e registrado no orgao competente</t>
   </si>
   <si>
@@ -2573,9 +2570,6 @@
     <t>FELIX RECICLAGEM INDUSTRIA E COMERCIO DE PLASTICOS LTDA</t>
   </si>
   <si>
-    <t>Contrato social atualizado e registrado no orgao competente</t>
-  </si>
-  <si>
     <t>33954917000184</t>
   </si>
   <si>
@@ -2955,6 +2949,72 @@
   </si>
   <si>
     <t>FLAVIO HENRIQUE DE MORAES ARMENTANO</t>
+  </si>
+  <si>
+    <t>38359693000186</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> JOAO CARLOS FERREIRA DA SILVA</t>
+  </si>
+  <si>
+    <t>28760672000114</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CAROLINE SILVA PATRICIO</t>
+  </si>
+  <si>
+    <t>37972985000127</t>
+  </si>
+  <si>
+    <t>ANDREZA TEIXEIRA REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>39763720000144</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FRANCISCO KENNEDY TORRES CONCEICAO</t>
+  </si>
+  <si>
+    <t>63621688000147</t>
+  </si>
+  <si>
+    <t>R RIGO AGRONEGOCIO LTDA</t>
+  </si>
+  <si>
+    <t>26931676000192</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EDSON PAULO SCHMITZ</t>
+  </si>
+  <si>
+    <t>34313082000146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VITORIA NUNES LIMAS </t>
+  </si>
+  <si>
+    <t>63915929000160</t>
+  </si>
+  <si>
+    <t>CARINE HEERDT PSICOLOGIA LTDA</t>
+  </si>
+  <si>
+    <t>45264616000108</t>
+  </si>
+  <si>
+    <t>M A CAVALCANTE BOX KIDS</t>
+  </si>
+  <si>
+    <t>45466375000180</t>
+  </si>
+  <si>
+    <t>J FERNANDES PINTO FILHO</t>
+  </si>
+  <si>
+    <t>A procuracao precisara ser assinada digitalmente GOV.br ou procuracao publica. Em caso de assinatura digital, devera ser encaminhado o documento em formato PDF.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procuracao com poderes para abrir e movimentar contas, pois identificamos que a representacao da sua empresa deve ser em conjunto pelos socios,  A procuracao deve ser assinada digitalmente pelos socios pela plataforma "GOV." e estar em formato PDF.&lt;br&gt;&lt;br&gt;Para garantir a seguranca e a validade do processo, Pedimos gentilmente que envie uma nova selfie, conforme as orientacoes </t>
   </si>
 </sst>
 </file>
@@ -3326,10 +3386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCD3CE2-DBA2-4F4F-B6A3-11EE884EA727}">
-  <dimension ref="A1:G463"/>
+  <dimension ref="A1:G473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A443" workbookViewId="0">
-      <selection activeCell="A463" sqref="A463"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3401,7 +3461,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G3" t="s">
         <v>55</v>
@@ -3487,7 +3547,7 @@
         <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -4666,10 +4726,10 @@
         <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>56</v>
+        <v>536</v>
       </c>
       <c r="G58" t="s">
-        <v>535</v>
+        <v>990</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -4827,7 +4887,7 @@
         <v>24</v>
       </c>
       <c r="F65" t="s">
-        <v>175</v>
+        <v>8</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -6069,10 +6129,10 @@
         <v>7</v>
       </c>
       <c r="F119" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G119" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -8234,7 +8294,7 @@
         <v>56</v>
       </c>
       <c r="G213" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -8277,7 +8337,7 @@
         <v>7</v>
       </c>
       <c r="F215" t="s">
-        <v>175</v>
+        <v>56</v>
       </c>
       <c r="G215">
         <v>0</v>
@@ -8530,7 +8590,7 @@
         <v>382</v>
       </c>
       <c r="F226" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="G226">
         <v>0</v>
@@ -8760,10 +8820,10 @@
         <v>14</v>
       </c>
       <c r="F236" t="s">
-        <v>537</v>
+        <v>56</v>
       </c>
       <c r="G236" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -8875,7 +8935,7 @@
         <v>7</v>
       </c>
       <c r="F241" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G241">
         <v>0</v>
@@ -9001,10 +9061,10 @@
         <v>45995</v>
       </c>
       <c r="B247" t="s">
+        <v>538</v>
+      </c>
+      <c r="C247" t="s">
         <v>539</v>
-      </c>
-      <c r="C247" t="s">
-        <v>540</v>
       </c>
       <c r="D247" t="s">
         <v>185</v>
@@ -9024,10 +9084,10 @@
         <v>45995</v>
       </c>
       <c r="B248" t="s">
+        <v>540</v>
+      </c>
+      <c r="C248" t="s">
         <v>541</v>
-      </c>
-      <c r="C248" t="s">
-        <v>542</v>
       </c>
       <c r="D248" t="s">
         <v>10</v>
@@ -9047,10 +9107,10 @@
         <v>45995</v>
       </c>
       <c r="B249" t="s">
+        <v>542</v>
+      </c>
+      <c r="C249" t="s">
         <v>543</v>
-      </c>
-      <c r="C249" t="s">
-        <v>544</v>
       </c>
       <c r="D249" t="s">
         <v>10</v>
@@ -9070,10 +9130,10 @@
         <v>45995</v>
       </c>
       <c r="B250" t="s">
+        <v>544</v>
+      </c>
+      <c r="C250" t="s">
         <v>545</v>
-      </c>
-      <c r="C250" t="s">
-        <v>546</v>
       </c>
       <c r="D250" t="s">
         <v>18</v>
@@ -9082,7 +9142,7 @@
         <v>24</v>
       </c>
       <c r="F250" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G250" t="e">
         <v>#N/A</v>
@@ -9116,10 +9176,10 @@
         <v>45995</v>
       </c>
       <c r="B252" t="s">
+        <v>547</v>
+      </c>
+      <c r="C252" t="s">
         <v>548</v>
-      </c>
-      <c r="C252" t="s">
-        <v>549</v>
       </c>
       <c r="D252" t="s">
         <v>16</v>
@@ -9139,10 +9199,10 @@
         <v>45995</v>
       </c>
       <c r="B253" t="s">
+        <v>549</v>
+      </c>
+      <c r="C253" t="s">
         <v>550</v>
-      </c>
-      <c r="C253" t="s">
-        <v>551</v>
       </c>
       <c r="D253" t="s">
         <v>18</v>
@@ -9162,10 +9222,10 @@
         <v>45995</v>
       </c>
       <c r="B254" t="s">
+        <v>551</v>
+      </c>
+      <c r="C254" t="s">
         <v>552</v>
-      </c>
-      <c r="C254" t="s">
-        <v>553</v>
       </c>
       <c r="D254" t="s">
         <v>10</v>
@@ -9185,10 +9245,10 @@
         <v>45995</v>
       </c>
       <c r="B255" t="s">
+        <v>553</v>
+      </c>
+      <c r="C255" t="s">
         <v>554</v>
-      </c>
-      <c r="C255" t="s">
-        <v>555</v>
       </c>
       <c r="D255" t="s">
         <v>17</v>
@@ -9208,10 +9268,10 @@
         <v>45995</v>
       </c>
       <c r="B256" t="s">
+        <v>555</v>
+      </c>
+      <c r="C256" t="s">
         <v>556</v>
-      </c>
-      <c r="C256" t="s">
-        <v>557</v>
       </c>
       <c r="D256" t="s">
         <v>26</v>
@@ -9231,10 +9291,10 @@
         <v>45995</v>
       </c>
       <c r="B257" t="s">
+        <v>557</v>
+      </c>
+      <c r="C257" t="s">
         <v>558</v>
-      </c>
-      <c r="C257" t="s">
-        <v>559</v>
       </c>
       <c r="D257" t="s">
         <v>6</v>
@@ -9254,10 +9314,10 @@
         <v>45995</v>
       </c>
       <c r="B258" t="s">
+        <v>559</v>
+      </c>
+      <c r="C258" t="s">
         <v>560</v>
-      </c>
-      <c r="C258" t="s">
-        <v>561</v>
       </c>
       <c r="D258" t="s">
         <v>6</v>
@@ -9277,10 +9337,10 @@
         <v>45995</v>
       </c>
       <c r="B259" t="s">
+        <v>561</v>
+      </c>
+      <c r="C259" t="s">
         <v>562</v>
-      </c>
-      <c r="C259" t="s">
-        <v>563</v>
       </c>
       <c r="D259" t="s">
         <v>22</v>
@@ -9300,10 +9360,10 @@
         <v>45995</v>
       </c>
       <c r="B260" t="s">
+        <v>563</v>
+      </c>
+      <c r="C260" t="s">
         <v>564</v>
-      </c>
-      <c r="C260" t="s">
-        <v>565</v>
       </c>
       <c r="D260" t="s">
         <v>17</v>
@@ -9323,10 +9383,10 @@
         <v>45995</v>
       </c>
       <c r="B261" t="s">
+        <v>565</v>
+      </c>
+      <c r="C261" t="s">
         <v>566</v>
-      </c>
-      <c r="C261" t="s">
-        <v>567</v>
       </c>
       <c r="D261" t="s">
         <v>20</v>
@@ -9346,10 +9406,10 @@
         <v>45995</v>
       </c>
       <c r="B262" t="s">
+        <v>567</v>
+      </c>
+      <c r="C262" t="s">
         <v>568</v>
-      </c>
-      <c r="C262" t="s">
-        <v>569</v>
       </c>
       <c r="D262" t="s">
         <v>19</v>
@@ -9369,10 +9429,10 @@
         <v>45995</v>
       </c>
       <c r="B263" t="s">
+        <v>569</v>
+      </c>
+      <c r="C263" t="s">
         <v>570</v>
-      </c>
-      <c r="C263" t="s">
-        <v>571</v>
       </c>
       <c r="D263" t="s">
         <v>22</v>
@@ -9392,10 +9452,10 @@
         <v>45995</v>
       </c>
       <c r="B264" t="s">
+        <v>571</v>
+      </c>
+      <c r="C264" t="s">
         <v>572</v>
-      </c>
-      <c r="C264" t="s">
-        <v>573</v>
       </c>
       <c r="D264" t="s">
         <v>13</v>
@@ -9415,10 +9475,10 @@
         <v>45995</v>
       </c>
       <c r="B265" t="s">
+        <v>573</v>
+      </c>
+      <c r="C265" t="s">
         <v>574</v>
-      </c>
-      <c r="C265" t="s">
-        <v>575</v>
       </c>
       <c r="D265" t="s">
         <v>26</v>
@@ -9438,10 +9498,10 @@
         <v>45995</v>
       </c>
       <c r="B266" t="s">
+        <v>575</v>
+      </c>
+      <c r="C266" t="s">
         <v>576</v>
-      </c>
-      <c r="C266" t="s">
-        <v>577</v>
       </c>
       <c r="D266" t="s">
         <v>22</v>
@@ -9461,10 +9521,10 @@
         <v>45995</v>
       </c>
       <c r="B267" t="s">
+        <v>577</v>
+      </c>
+      <c r="C267" t="s">
         <v>578</v>
-      </c>
-      <c r="C267" t="s">
-        <v>579</v>
       </c>
       <c r="D267" t="s">
         <v>16</v>
@@ -9484,10 +9544,10 @@
         <v>45995</v>
       </c>
       <c r="B268" t="s">
+        <v>579</v>
+      </c>
+      <c r="C268" t="s">
         <v>580</v>
-      </c>
-      <c r="C268" t="s">
-        <v>581</v>
       </c>
       <c r="D268" t="s">
         <v>21</v>
@@ -9507,10 +9567,10 @@
         <v>45995</v>
       </c>
       <c r="B269" t="s">
+        <v>581</v>
+      </c>
+      <c r="C269" t="s">
         <v>582</v>
-      </c>
-      <c r="C269" t="s">
-        <v>583</v>
       </c>
       <c r="D269" t="s">
         <v>13</v>
@@ -9530,10 +9590,10 @@
         <v>45995</v>
       </c>
       <c r="B270" t="s">
+        <v>583</v>
+      </c>
+      <c r="C270" t="s">
         <v>584</v>
-      </c>
-      <c r="C270" t="s">
-        <v>585</v>
       </c>
       <c r="D270" t="s">
         <v>21</v>
@@ -9553,10 +9613,10 @@
         <v>45995</v>
       </c>
       <c r="B271" t="s">
+        <v>585</v>
+      </c>
+      <c r="C271" t="s">
         <v>586</v>
-      </c>
-      <c r="C271" t="s">
-        <v>587</v>
       </c>
       <c r="D271" t="s">
         <v>22</v>
@@ -9576,10 +9636,10 @@
         <v>45995</v>
       </c>
       <c r="B272" t="s">
+        <v>587</v>
+      </c>
+      <c r="C272" t="s">
         <v>588</v>
-      </c>
-      <c r="C272" t="s">
-        <v>589</v>
       </c>
       <c r="D272" t="s">
         <v>16</v>
@@ -9599,10 +9659,10 @@
         <v>45995</v>
       </c>
       <c r="B273" t="s">
+        <v>589</v>
+      </c>
+      <c r="C273" t="s">
         <v>590</v>
-      </c>
-      <c r="C273" t="s">
-        <v>591</v>
       </c>
       <c r="D273" t="s">
         <v>25</v>
@@ -9622,10 +9682,10 @@
         <v>45995</v>
       </c>
       <c r="B274" t="s">
+        <v>591</v>
+      </c>
+      <c r="C274" t="s">
         <v>592</v>
-      </c>
-      <c r="C274" t="s">
-        <v>593</v>
       </c>
       <c r="D274" t="s">
         <v>9</v>
@@ -9645,10 +9705,10 @@
         <v>45995</v>
       </c>
       <c r="B275" t="s">
+        <v>593</v>
+      </c>
+      <c r="C275" t="s">
         <v>594</v>
-      </c>
-      <c r="C275" t="s">
-        <v>595</v>
       </c>
       <c r="D275" t="s">
         <v>19</v>
@@ -9668,10 +9728,10 @@
         <v>45995</v>
       </c>
       <c r="B276" t="s">
+        <v>595</v>
+      </c>
+      <c r="C276" t="s">
         <v>596</v>
-      </c>
-      <c r="C276" t="s">
-        <v>597</v>
       </c>
       <c r="D276" t="s">
         <v>21</v>
@@ -9691,10 +9751,10 @@
         <v>45995</v>
       </c>
       <c r="B277" t="s">
+        <v>597</v>
+      </c>
+      <c r="C277" t="s">
         <v>598</v>
-      </c>
-      <c r="C277" t="s">
-        <v>599</v>
       </c>
       <c r="D277" t="s">
         <v>26</v>
@@ -9714,10 +9774,10 @@
         <v>45995</v>
       </c>
       <c r="B278" t="s">
+        <v>599</v>
+      </c>
+      <c r="C278" t="s">
         <v>600</v>
-      </c>
-      <c r="C278" t="s">
-        <v>601</v>
       </c>
       <c r="D278" t="s">
         <v>18</v>
@@ -9737,10 +9797,10 @@
         <v>45995</v>
       </c>
       <c r="B279" t="s">
+        <v>601</v>
+      </c>
+      <c r="C279" t="s">
         <v>602</v>
-      </c>
-      <c r="C279" t="s">
-        <v>603</v>
       </c>
       <c r="D279" t="s">
         <v>13</v>
@@ -9760,10 +9820,10 @@
         <v>45995</v>
       </c>
       <c r="B280" t="s">
+        <v>603</v>
+      </c>
+      <c r="C280" t="s">
         <v>604</v>
-      </c>
-      <c r="C280" t="s">
-        <v>605</v>
       </c>
       <c r="D280" t="s">
         <v>9</v>
@@ -9783,10 +9843,10 @@
         <v>45995</v>
       </c>
       <c r="B281" t="s">
+        <v>605</v>
+      </c>
+      <c r="C281" t="s">
         <v>606</v>
-      </c>
-      <c r="C281" t="s">
-        <v>607</v>
       </c>
       <c r="D281" t="s">
         <v>6</v>
@@ -9795,7 +9855,7 @@
         <v>7</v>
       </c>
       <c r="F281" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G281" t="e">
         <v>#N/A</v>
@@ -9806,13 +9866,13 @@
         <v>45995</v>
       </c>
       <c r="B282" t="s">
+        <v>607</v>
+      </c>
+      <c r="C282" t="s">
         <v>608</v>
       </c>
-      <c r="C282" t="s">
+      <c r="D282" t="s">
         <v>609</v>
-      </c>
-      <c r="D282" t="s">
-        <v>610</v>
       </c>
       <c r="E282" t="s">
         <v>462</v>
@@ -9829,10 +9889,10 @@
         <v>45995</v>
       </c>
       <c r="B283" t="s">
+        <v>610</v>
+      </c>
+      <c r="C283" t="s">
         <v>611</v>
-      </c>
-      <c r="C283" t="s">
-        <v>612</v>
       </c>
       <c r="D283" t="s">
         <v>10</v>
@@ -9852,10 +9912,10 @@
         <v>45995</v>
       </c>
       <c r="B284" t="s">
+        <v>612</v>
+      </c>
+      <c r="C284" t="s">
         <v>613</v>
-      </c>
-      <c r="C284" t="s">
-        <v>614</v>
       </c>
       <c r="D284" t="s">
         <v>16</v>
@@ -9875,10 +9935,10 @@
         <v>45995</v>
       </c>
       <c r="B285" t="s">
+        <v>614</v>
+      </c>
+      <c r="C285" t="s">
         <v>615</v>
-      </c>
-      <c r="C285" t="s">
-        <v>616</v>
       </c>
       <c r="D285" t="s">
         <v>10</v>
@@ -9898,10 +9958,10 @@
         <v>45995</v>
       </c>
       <c r="B286" t="s">
+        <v>616</v>
+      </c>
+      <c r="C286" t="s">
         <v>617</v>
-      </c>
-      <c r="C286" t="s">
-        <v>618</v>
       </c>
       <c r="D286" t="s">
         <v>10</v>
@@ -9921,10 +9981,10 @@
         <v>45995</v>
       </c>
       <c r="B287" t="s">
+        <v>618</v>
+      </c>
+      <c r="C287" t="s">
         <v>619</v>
-      </c>
-      <c r="C287" t="s">
-        <v>620</v>
       </c>
       <c r="D287" t="s">
         <v>21</v>
@@ -9944,10 +10004,10 @@
         <v>45995</v>
       </c>
       <c r="B288" t="s">
+        <v>620</v>
+      </c>
+      <c r="C288" t="s">
         <v>621</v>
-      </c>
-      <c r="C288" t="s">
-        <v>622</v>
       </c>
       <c r="D288" t="s">
         <v>10</v>
@@ -9967,10 +10027,10 @@
         <v>45995</v>
       </c>
       <c r="B289" t="s">
+        <v>622</v>
+      </c>
+      <c r="C289" t="s">
         <v>623</v>
-      </c>
-      <c r="C289" t="s">
-        <v>624</v>
       </c>
       <c r="D289" t="s">
         <v>21</v>
@@ -9990,10 +10050,10 @@
         <v>45995</v>
       </c>
       <c r="B290" t="s">
+        <v>624</v>
+      </c>
+      <c r="C290" t="s">
         <v>625</v>
-      </c>
-      <c r="C290" t="s">
-        <v>626</v>
       </c>
       <c r="D290" t="s">
         <v>18</v>
@@ -10013,10 +10073,10 @@
         <v>45995</v>
       </c>
       <c r="B291" t="s">
+        <v>626</v>
+      </c>
+      <c r="C291" t="s">
         <v>627</v>
-      </c>
-      <c r="C291" t="s">
-        <v>628</v>
       </c>
       <c r="D291" t="s">
         <v>17</v>
@@ -10036,10 +10096,10 @@
         <v>45995</v>
       </c>
       <c r="B292" t="s">
+        <v>628</v>
+      </c>
+      <c r="C292" t="s">
         <v>629</v>
-      </c>
-      <c r="C292" t="s">
-        <v>630</v>
       </c>
       <c r="D292" t="s">
         <v>10</v>
@@ -10059,10 +10119,10 @@
         <v>45995</v>
       </c>
       <c r="B293" t="s">
+        <v>630</v>
+      </c>
+      <c r="C293" t="s">
         <v>631</v>
-      </c>
-      <c r="C293" t="s">
-        <v>632</v>
       </c>
       <c r="D293" t="s">
         <v>11</v>
@@ -10082,10 +10142,10 @@
         <v>45995</v>
       </c>
       <c r="B294" t="s">
+        <v>632</v>
+      </c>
+      <c r="C294" t="s">
         <v>633</v>
-      </c>
-      <c r="C294" t="s">
-        <v>634</v>
       </c>
       <c r="D294" t="s">
         <v>20</v>
@@ -10105,10 +10165,10 @@
         <v>45995</v>
       </c>
       <c r="B295" t="s">
+        <v>634</v>
+      </c>
+      <c r="C295" t="s">
         <v>635</v>
-      </c>
-      <c r="C295" t="s">
-        <v>636</v>
       </c>
       <c r="D295" t="s">
         <v>20</v>
@@ -10128,10 +10188,10 @@
         <v>45995</v>
       </c>
       <c r="B296" t="s">
+        <v>636</v>
+      </c>
+      <c r="C296" t="s">
         <v>637</v>
-      </c>
-      <c r="C296" t="s">
-        <v>638</v>
       </c>
       <c r="D296" t="s">
         <v>6</v>
@@ -10151,10 +10211,10 @@
         <v>45995</v>
       </c>
       <c r="B297" t="s">
+        <v>638</v>
+      </c>
+      <c r="C297" t="s">
         <v>639</v>
-      </c>
-      <c r="C297" t="s">
-        <v>640</v>
       </c>
       <c r="D297" t="s">
         <v>16</v>
@@ -10174,10 +10234,10 @@
         <v>45995</v>
       </c>
       <c r="B298" t="s">
+        <v>640</v>
+      </c>
+      <c r="C298" t="s">
         <v>641</v>
-      </c>
-      <c r="C298" t="s">
-        <v>642</v>
       </c>
       <c r="D298" t="s">
         <v>25</v>
@@ -10197,10 +10257,10 @@
         <v>45995</v>
       </c>
       <c r="B299" t="s">
+        <v>642</v>
+      </c>
+      <c r="C299" t="s">
         <v>643</v>
-      </c>
-      <c r="C299" t="s">
-        <v>644</v>
       </c>
       <c r="D299" t="s">
         <v>10</v>
@@ -10220,10 +10280,10 @@
         <v>45995</v>
       </c>
       <c r="B300" t="s">
+        <v>644</v>
+      </c>
+      <c r="C300" t="s">
         <v>645</v>
-      </c>
-      <c r="C300" t="s">
-        <v>646</v>
       </c>
       <c r="D300" t="s">
         <v>20</v>
@@ -10243,10 +10303,10 @@
         <v>45995</v>
       </c>
       <c r="B301" t="s">
+        <v>646</v>
+      </c>
+      <c r="C301" t="s">
         <v>647</v>
-      </c>
-      <c r="C301" t="s">
-        <v>648</v>
       </c>
       <c r="D301" t="s">
         <v>9</v>
@@ -10266,13 +10326,13 @@
         <v>45995</v>
       </c>
       <c r="B302" t="s">
+        <v>648</v>
+      </c>
+      <c r="C302" t="s">
         <v>649</v>
       </c>
-      <c r="C302" t="s">
+      <c r="D302" t="s">
         <v>650</v>
-      </c>
-      <c r="D302" t="s">
-        <v>651</v>
       </c>
       <c r="E302" t="s">
         <v>382</v>
@@ -10289,10 +10349,10 @@
         <v>45995</v>
       </c>
       <c r="B303" t="s">
+        <v>651</v>
+      </c>
+      <c r="C303" t="s">
         <v>652</v>
-      </c>
-      <c r="C303" t="s">
-        <v>653</v>
       </c>
       <c r="D303" t="s">
         <v>13</v>
@@ -10312,10 +10372,10 @@
         <v>45995</v>
       </c>
       <c r="B304" t="s">
+        <v>653</v>
+      </c>
+      <c r="C304" t="s">
         <v>654</v>
-      </c>
-      <c r="C304" t="s">
-        <v>655</v>
       </c>
       <c r="D304" t="s">
         <v>17</v>
@@ -10335,10 +10395,10 @@
         <v>45995</v>
       </c>
       <c r="B305" t="s">
+        <v>655</v>
+      </c>
+      <c r="C305" t="s">
         <v>656</v>
-      </c>
-      <c r="C305" t="s">
-        <v>657</v>
       </c>
       <c r="D305" t="s">
         <v>16</v>
@@ -10358,10 +10418,10 @@
         <v>45995</v>
       </c>
       <c r="B306" t="s">
+        <v>657</v>
+      </c>
+      <c r="C306" t="s">
         <v>658</v>
-      </c>
-      <c r="C306" t="s">
-        <v>659</v>
       </c>
       <c r="D306" t="s">
         <v>20</v>
@@ -10381,10 +10441,10 @@
         <v>45995</v>
       </c>
       <c r="B307" t="s">
+        <v>659</v>
+      </c>
+      <c r="C307" t="s">
         <v>660</v>
-      </c>
-      <c r="C307" t="s">
-        <v>661</v>
       </c>
       <c r="D307" t="s">
         <v>19</v>
@@ -10404,10 +10464,10 @@
         <v>45995</v>
       </c>
       <c r="B308" t="s">
+        <v>661</v>
+      </c>
+      <c r="C308" t="s">
         <v>662</v>
-      </c>
-      <c r="C308" t="s">
-        <v>663</v>
       </c>
       <c r="D308" t="s">
         <v>22</v>
@@ -10427,10 +10487,10 @@
         <v>45995</v>
       </c>
       <c r="B309" t="s">
+        <v>663</v>
+      </c>
+      <c r="C309" t="s">
         <v>664</v>
-      </c>
-      <c r="C309" t="s">
-        <v>665</v>
       </c>
       <c r="D309" t="s">
         <v>6</v>
@@ -10450,10 +10510,10 @@
         <v>45996</v>
       </c>
       <c r="B310" t="s">
+        <v>665</v>
+      </c>
+      <c r="C310" t="s">
         <v>666</v>
-      </c>
-      <c r="C310" t="s">
-        <v>667</v>
       </c>
       <c r="D310" t="s">
         <v>21</v>
@@ -10473,10 +10533,10 @@
         <v>45996</v>
       </c>
       <c r="B311" t="s">
+        <v>667</v>
+      </c>
+      <c r="C311" t="s">
         <v>668</v>
-      </c>
-      <c r="C311" t="s">
-        <v>669</v>
       </c>
       <c r="D311" t="s">
         <v>19</v>
@@ -10496,10 +10556,10 @@
         <v>45996</v>
       </c>
       <c r="B312" t="s">
+        <v>669</v>
+      </c>
+      <c r="C312" t="s">
         <v>670</v>
-      </c>
-      <c r="C312" t="s">
-        <v>671</v>
       </c>
       <c r="D312" t="s">
         <v>6</v>
@@ -10519,10 +10579,10 @@
         <v>45996</v>
       </c>
       <c r="B313" t="s">
+        <v>671</v>
+      </c>
+      <c r="C313" t="s">
         <v>672</v>
-      </c>
-      <c r="C313" t="s">
-        <v>673</v>
       </c>
       <c r="D313" t="s">
         <v>25</v>
@@ -10542,10 +10602,10 @@
         <v>45996</v>
       </c>
       <c r="B314" t="s">
+        <v>673</v>
+      </c>
+      <c r="C314" t="s">
         <v>674</v>
-      </c>
-      <c r="C314" t="s">
-        <v>675</v>
       </c>
       <c r="D314" t="s">
         <v>22</v>
@@ -10565,10 +10625,10 @@
         <v>45996</v>
       </c>
       <c r="B315" t="s">
+        <v>675</v>
+      </c>
+      <c r="C315" t="s">
         <v>676</v>
-      </c>
-      <c r="C315" t="s">
-        <v>677</v>
       </c>
       <c r="D315" t="s">
         <v>9</v>
@@ -10588,10 +10648,10 @@
         <v>45996</v>
       </c>
       <c r="B316" t="s">
+        <v>680</v>
+      </c>
+      <c r="C316" t="s">
         <v>681</v>
-      </c>
-      <c r="C316" t="s">
-        <v>682</v>
       </c>
       <c r="D316" t="s">
         <v>19</v>
@@ -10611,10 +10671,10 @@
         <v>45996</v>
       </c>
       <c r="B317" t="s">
+        <v>682</v>
+      </c>
+      <c r="C317" t="s">
         <v>683</v>
-      </c>
-      <c r="C317" t="s">
-        <v>684</v>
       </c>
       <c r="D317" t="s">
         <v>22</v>
@@ -10634,10 +10694,10 @@
         <v>45996</v>
       </c>
       <c r="B318" t="s">
+        <v>684</v>
+      </c>
+      <c r="C318" t="s">
         <v>685</v>
-      </c>
-      <c r="C318" t="s">
-        <v>686</v>
       </c>
       <c r="D318" t="s">
         <v>26</v>
@@ -10657,10 +10717,10 @@
         <v>45996</v>
       </c>
       <c r="B319" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C319" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D319" t="s">
         <v>18</v>
@@ -10680,10 +10740,10 @@
         <v>45996</v>
       </c>
       <c r="B320" t="s">
+        <v>687</v>
+      </c>
+      <c r="C320" t="s">
         <v>688</v>
-      </c>
-      <c r="C320" t="s">
-        <v>689</v>
       </c>
       <c r="D320" t="s">
         <v>6</v>
@@ -10703,10 +10763,10 @@
         <v>45996</v>
       </c>
       <c r="B321" t="s">
+        <v>689</v>
+      </c>
+      <c r="C321" t="s">
         <v>690</v>
-      </c>
-      <c r="C321" t="s">
-        <v>691</v>
       </c>
       <c r="D321" t="s">
         <v>6</v>
@@ -10726,10 +10786,10 @@
         <v>45996</v>
       </c>
       <c r="B322" t="s">
+        <v>691</v>
+      </c>
+      <c r="C322" t="s">
         <v>692</v>
-      </c>
-      <c r="C322" t="s">
-        <v>693</v>
       </c>
       <c r="D322" t="s">
         <v>21</v>
@@ -10749,10 +10809,10 @@
         <v>45996</v>
       </c>
       <c r="B323" t="s">
+        <v>693</v>
+      </c>
+      <c r="C323" t="s">
         <v>694</v>
-      </c>
-      <c r="C323" t="s">
-        <v>695</v>
       </c>
       <c r="D323" t="s">
         <v>13</v>
@@ -10772,10 +10832,10 @@
         <v>45996</v>
       </c>
       <c r="B324" t="s">
+        <v>695</v>
+      </c>
+      <c r="C324" t="s">
         <v>696</v>
-      </c>
-      <c r="C324" t="s">
-        <v>697</v>
       </c>
       <c r="D324" t="s">
         <v>10</v>
@@ -10795,10 +10855,10 @@
         <v>45996</v>
       </c>
       <c r="B325" t="s">
+        <v>697</v>
+      </c>
+      <c r="C325" t="s">
         <v>698</v>
-      </c>
-      <c r="C325" t="s">
-        <v>699</v>
       </c>
       <c r="D325" t="s">
         <v>17</v>
@@ -10818,10 +10878,10 @@
         <v>45996</v>
       </c>
       <c r="B326" t="s">
+        <v>699</v>
+      </c>
+      <c r="C326" t="s">
         <v>700</v>
-      </c>
-      <c r="C326" t="s">
-        <v>701</v>
       </c>
       <c r="D326" t="s">
         <v>26</v>
@@ -10841,10 +10901,10 @@
         <v>45996</v>
       </c>
       <c r="B327" t="s">
+        <v>701</v>
+      </c>
+      <c r="C327" t="s">
         <v>702</v>
-      </c>
-      <c r="C327" t="s">
-        <v>703</v>
       </c>
       <c r="D327" t="s">
         <v>13</v>
@@ -10864,10 +10924,10 @@
         <v>45996</v>
       </c>
       <c r="B328" t="s">
+        <v>703</v>
+      </c>
+      <c r="C328" t="s">
         <v>704</v>
-      </c>
-      <c r="C328" t="s">
-        <v>705</v>
       </c>
       <c r="D328" t="s">
         <v>10</v>
@@ -10887,10 +10947,10 @@
         <v>45996</v>
       </c>
       <c r="B329" t="s">
+        <v>705</v>
+      </c>
+      <c r="C329" t="s">
         <v>706</v>
-      </c>
-      <c r="C329" t="s">
-        <v>707</v>
       </c>
       <c r="D329" t="s">
         <v>6</v>
@@ -10910,10 +10970,10 @@
         <v>45996</v>
       </c>
       <c r="B330" t="s">
+        <v>707</v>
+      </c>
+      <c r="C330" t="s">
         <v>708</v>
-      </c>
-      <c r="C330" t="s">
-        <v>709</v>
       </c>
       <c r="D330" t="s">
         <v>16</v>
@@ -10933,10 +10993,10 @@
         <v>45996</v>
       </c>
       <c r="B331" t="s">
+        <v>709</v>
+      </c>
+      <c r="C331" t="s">
         <v>710</v>
-      </c>
-      <c r="C331" t="s">
-        <v>711</v>
       </c>
       <c r="D331" t="s">
         <v>26</v>
@@ -10945,10 +11005,10 @@
         <v>14</v>
       </c>
       <c r="F331" t="s">
-        <v>537</v>
-      </c>
-      <c r="G331" t="s">
-        <v>844</v>
+        <v>175</v>
+      </c>
+      <c r="G331">
+        <v>0</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.25">
@@ -10956,10 +11016,10 @@
         <v>45996</v>
       </c>
       <c r="B332" t="s">
+        <v>711</v>
+      </c>
+      <c r="C332" t="s">
         <v>712</v>
-      </c>
-      <c r="C332" t="s">
-        <v>713</v>
       </c>
       <c r="D332" t="s">
         <v>10</v>
@@ -10979,10 +11039,10 @@
         <v>45996</v>
       </c>
       <c r="B333" t="s">
+        <v>713</v>
+      </c>
+      <c r="C333" t="s">
         <v>714</v>
-      </c>
-      <c r="C333" t="s">
-        <v>715</v>
       </c>
       <c r="D333" t="s">
         <v>9</v>
@@ -11002,10 +11062,10 @@
         <v>45996</v>
       </c>
       <c r="B334" t="s">
+        <v>715</v>
+      </c>
+      <c r="C334" t="s">
         <v>716</v>
-      </c>
-      <c r="C334" t="s">
-        <v>717</v>
       </c>
       <c r="D334" t="s">
         <v>11</v>
@@ -11025,10 +11085,10 @@
         <v>45996</v>
       </c>
       <c r="B335" t="s">
+        <v>717</v>
+      </c>
+      <c r="C335" t="s">
         <v>718</v>
-      </c>
-      <c r="C335" t="s">
-        <v>719</v>
       </c>
       <c r="D335" t="s">
         <v>26</v>
@@ -11048,10 +11108,10 @@
         <v>45996</v>
       </c>
       <c r="B336" t="s">
+        <v>719</v>
+      </c>
+      <c r="C336" t="s">
         <v>720</v>
-      </c>
-      <c r="C336" t="s">
-        <v>721</v>
       </c>
       <c r="D336" t="s">
         <v>6</v>
@@ -11083,10 +11143,10 @@
         <v>7</v>
       </c>
       <c r="F337" t="s">
-        <v>175</v>
-      </c>
-      <c r="G337">
-        <v>0</v>
+        <v>536</v>
+      </c>
+      <c r="G337" t="s">
+        <v>991</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.25">
@@ -11094,10 +11154,10 @@
         <v>45996</v>
       </c>
       <c r="B338" t="s">
+        <v>721</v>
+      </c>
+      <c r="C338" t="s">
         <v>722</v>
-      </c>
-      <c r="C338" t="s">
-        <v>723</v>
       </c>
       <c r="D338" t="s">
         <v>9</v>
@@ -11117,10 +11177,10 @@
         <v>45996</v>
       </c>
       <c r="B339" t="s">
+        <v>723</v>
+      </c>
+      <c r="C339" t="s">
         <v>724</v>
-      </c>
-      <c r="C339" t="s">
-        <v>725</v>
       </c>
       <c r="D339" t="s">
         <v>10</v>
@@ -11140,10 +11200,10 @@
         <v>45996</v>
       </c>
       <c r="B340" t="s">
+        <v>725</v>
+      </c>
+      <c r="C340" t="s">
         <v>726</v>
-      </c>
-      <c r="C340" t="s">
-        <v>727</v>
       </c>
       <c r="D340" t="s">
         <v>10</v>
@@ -11163,10 +11223,10 @@
         <v>45996</v>
       </c>
       <c r="B341" t="s">
+        <v>727</v>
+      </c>
+      <c r="C341" t="s">
         <v>728</v>
-      </c>
-      <c r="C341" t="s">
-        <v>729</v>
       </c>
       <c r="D341" t="s">
         <v>22</v>
@@ -11186,10 +11246,10 @@
         <v>45996</v>
       </c>
       <c r="B342" t="s">
+        <v>729</v>
+      </c>
+      <c r="C342" t="s">
         <v>730</v>
-      </c>
-      <c r="C342" t="s">
-        <v>731</v>
       </c>
       <c r="D342" t="s">
         <v>9</v>
@@ -11209,10 +11269,10 @@
         <v>45996</v>
       </c>
       <c r="B343" t="s">
+        <v>731</v>
+      </c>
+      <c r="C343" t="s">
         <v>732</v>
-      </c>
-      <c r="C343" t="s">
-        <v>733</v>
       </c>
       <c r="D343" t="s">
         <v>17</v>
@@ -11232,10 +11292,10 @@
         <v>45996</v>
       </c>
       <c r="B344" t="s">
+        <v>733</v>
+      </c>
+      <c r="C344" t="s">
         <v>734</v>
-      </c>
-      <c r="C344" t="s">
-        <v>735</v>
       </c>
       <c r="D344" t="s">
         <v>10</v>
@@ -11255,10 +11315,10 @@
         <v>45996</v>
       </c>
       <c r="B345" t="s">
+        <v>735</v>
+      </c>
+      <c r="C345" t="s">
         <v>736</v>
-      </c>
-      <c r="C345" t="s">
-        <v>737</v>
       </c>
       <c r="D345" t="s">
         <v>9</v>
@@ -11278,10 +11338,10 @@
         <v>45996</v>
       </c>
       <c r="B346" t="s">
+        <v>737</v>
+      </c>
+      <c r="C346" t="s">
         <v>738</v>
-      </c>
-      <c r="C346" t="s">
-        <v>739</v>
       </c>
       <c r="D346" t="s">
         <v>21</v>
@@ -11301,10 +11361,10 @@
         <v>45996</v>
       </c>
       <c r="B347" t="s">
+        <v>739</v>
+      </c>
+      <c r="C347" t="s">
         <v>740</v>
-      </c>
-      <c r="C347" t="s">
-        <v>741</v>
       </c>
       <c r="D347" t="s">
         <v>19</v>
@@ -11324,10 +11384,10 @@
         <v>45996</v>
       </c>
       <c r="B348" t="s">
+        <v>741</v>
+      </c>
+      <c r="C348" t="s">
         <v>742</v>
-      </c>
-      <c r="C348" t="s">
-        <v>743</v>
       </c>
       <c r="D348" t="s">
         <v>9</v>
@@ -11347,10 +11407,10 @@
         <v>45996</v>
       </c>
       <c r="B349" t="s">
+        <v>743</v>
+      </c>
+      <c r="C349" t="s">
         <v>744</v>
-      </c>
-      <c r="C349" t="s">
-        <v>745</v>
       </c>
       <c r="D349" t="s">
         <v>26</v>
@@ -11359,10 +11419,10 @@
         <v>14</v>
       </c>
       <c r="F349" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G349" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="350" spans="1:7" x14ac:dyDescent="0.25">
@@ -11370,10 +11430,10 @@
         <v>45996</v>
       </c>
       <c r="B350" t="s">
+        <v>745</v>
+      </c>
+      <c r="C350" t="s">
         <v>746</v>
-      </c>
-      <c r="C350" t="s">
-        <v>747</v>
       </c>
       <c r="D350" t="s">
         <v>13</v>
@@ -11393,10 +11453,10 @@
         <v>45996</v>
       </c>
       <c r="B351" t="s">
+        <v>747</v>
+      </c>
+      <c r="C351" t="s">
         <v>748</v>
-      </c>
-      <c r="C351" t="s">
-        <v>749</v>
       </c>
       <c r="D351" t="s">
         <v>10</v>
@@ -11416,10 +11476,10 @@
         <v>45996</v>
       </c>
       <c r="B352" t="s">
+        <v>749</v>
+      </c>
+      <c r="C352" t="s">
         <v>750</v>
-      </c>
-      <c r="C352" t="s">
-        <v>751</v>
       </c>
       <c r="D352" t="s">
         <v>16</v>
@@ -11439,10 +11499,10 @@
         <v>45996</v>
       </c>
       <c r="B353" t="s">
+        <v>751</v>
+      </c>
+      <c r="C353" t="s">
         <v>752</v>
-      </c>
-      <c r="C353" t="s">
-        <v>753</v>
       </c>
       <c r="D353" t="s">
         <v>16</v>
@@ -11462,10 +11522,10 @@
         <v>45996</v>
       </c>
       <c r="B354" t="s">
+        <v>753</v>
+      </c>
+      <c r="C354" t="s">
         <v>754</v>
-      </c>
-      <c r="C354" t="s">
-        <v>755</v>
       </c>
       <c r="D354" t="s">
         <v>10</v>
@@ -11485,10 +11545,10 @@
         <v>45996</v>
       </c>
       <c r="B355" t="s">
+        <v>755</v>
+      </c>
+      <c r="C355" t="s">
         <v>756</v>
-      </c>
-      <c r="C355" t="s">
-        <v>757</v>
       </c>
       <c r="D355" t="s">
         <v>10</v>
@@ -11508,10 +11568,10 @@
         <v>45996</v>
       </c>
       <c r="B356" t="s">
+        <v>757</v>
+      </c>
+      <c r="C356" t="s">
         <v>758</v>
-      </c>
-      <c r="C356" t="s">
-        <v>759</v>
       </c>
       <c r="D356" t="s">
         <v>6</v>
@@ -11531,10 +11591,10 @@
         <v>45996</v>
       </c>
       <c r="B357" t="s">
+        <v>759</v>
+      </c>
+      <c r="C357" t="s">
         <v>760</v>
-      </c>
-      <c r="C357" t="s">
-        <v>761</v>
       </c>
       <c r="D357" t="s">
         <v>21</v>
@@ -11554,10 +11614,10 @@
         <v>45996</v>
       </c>
       <c r="B358" t="s">
+        <v>761</v>
+      </c>
+      <c r="C358" t="s">
         <v>762</v>
-      </c>
-      <c r="C358" t="s">
-        <v>763</v>
       </c>
       <c r="D358" t="s">
         <v>17</v>
@@ -11577,10 +11637,10 @@
         <v>45996</v>
       </c>
       <c r="B359" t="s">
+        <v>763</v>
+      </c>
+      <c r="C359" t="s">
         <v>764</v>
-      </c>
-      <c r="C359" t="s">
-        <v>765</v>
       </c>
       <c r="D359" t="s">
         <v>6</v>
@@ -11600,10 +11660,10 @@
         <v>45996</v>
       </c>
       <c r="B360" t="s">
+        <v>765</v>
+      </c>
+      <c r="C360" t="s">
         <v>766</v>
-      </c>
-      <c r="C360" t="s">
-        <v>767</v>
       </c>
       <c r="D360" t="s">
         <v>19</v>
@@ -11646,10 +11706,10 @@
         <v>45996</v>
       </c>
       <c r="B362" t="s">
+        <v>767</v>
+      </c>
+      <c r="C362" t="s">
         <v>768</v>
-      </c>
-      <c r="C362" t="s">
-        <v>769</v>
       </c>
       <c r="D362" t="s">
         <v>11</v>
@@ -11669,10 +11729,10 @@
         <v>45996</v>
       </c>
       <c r="B363" t="s">
+        <v>769</v>
+      </c>
+      <c r="C363" t="s">
         <v>770</v>
-      </c>
-      <c r="C363" t="s">
-        <v>771</v>
       </c>
       <c r="D363" t="s">
         <v>22</v>
@@ -11692,10 +11752,10 @@
         <v>45996</v>
       </c>
       <c r="B364" t="s">
+        <v>771</v>
+      </c>
+      <c r="C364" t="s">
         <v>772</v>
-      </c>
-      <c r="C364" t="s">
-        <v>773</v>
       </c>
       <c r="D364" t="s">
         <v>10</v>
@@ -11715,10 +11775,10 @@
         <v>45996</v>
       </c>
       <c r="B365" t="s">
+        <v>773</v>
+      </c>
+      <c r="C365" t="s">
         <v>774</v>
-      </c>
-      <c r="C365" t="s">
-        <v>775</v>
       </c>
       <c r="D365" t="s">
         <v>16</v>
@@ -11738,10 +11798,10 @@
         <v>45996</v>
       </c>
       <c r="B366" t="s">
+        <v>775</v>
+      </c>
+      <c r="C366" t="s">
         <v>776</v>
-      </c>
-      <c r="C366" t="s">
-        <v>777</v>
       </c>
       <c r="D366" t="s">
         <v>22</v>
@@ -11761,10 +11821,10 @@
         <v>45996</v>
       </c>
       <c r="B367" t="s">
+        <v>777</v>
+      </c>
+      <c r="C367" t="s">
         <v>778</v>
-      </c>
-      <c r="C367" t="s">
-        <v>779</v>
       </c>
       <c r="D367" t="s">
         <v>6</v>
@@ -11784,10 +11844,10 @@
         <v>45996</v>
       </c>
       <c r="B368" t="s">
+        <v>779</v>
+      </c>
+      <c r="C368" t="s">
         <v>780</v>
-      </c>
-      <c r="C368" t="s">
-        <v>781</v>
       </c>
       <c r="D368" t="s">
         <v>13</v>
@@ -11807,10 +11867,10 @@
         <v>45996</v>
       </c>
       <c r="B369" t="s">
+        <v>781</v>
+      </c>
+      <c r="C369" t="s">
         <v>782</v>
-      </c>
-      <c r="C369" t="s">
-        <v>783</v>
       </c>
       <c r="D369" t="s">
         <v>20</v>
@@ -11830,10 +11890,10 @@
         <v>45996</v>
       </c>
       <c r="B370" t="s">
+        <v>783</v>
+      </c>
+      <c r="C370" t="s">
         <v>784</v>
-      </c>
-      <c r="C370" t="s">
-        <v>785</v>
       </c>
       <c r="D370" t="s">
         <v>9</v>
@@ -11853,10 +11913,10 @@
         <v>45996</v>
       </c>
       <c r="B371" t="s">
+        <v>785</v>
+      </c>
+      <c r="C371" t="s">
         <v>786</v>
-      </c>
-      <c r="C371" t="s">
-        <v>787</v>
       </c>
       <c r="D371" t="s">
         <v>6</v>
@@ -11876,10 +11936,10 @@
         <v>45996</v>
       </c>
       <c r="B372" t="s">
+        <v>787</v>
+      </c>
+      <c r="C372" t="s">
         <v>788</v>
-      </c>
-      <c r="C372" t="s">
-        <v>789</v>
       </c>
       <c r="D372" t="s">
         <v>16</v>
@@ -11899,10 +11959,10 @@
         <v>45996</v>
       </c>
       <c r="B373" t="s">
+        <v>789</v>
+      </c>
+      <c r="C373" t="s">
         <v>790</v>
-      </c>
-      <c r="C373" t="s">
-        <v>791</v>
       </c>
       <c r="D373" t="s">
         <v>9</v>
@@ -11922,10 +11982,10 @@
         <v>45996</v>
       </c>
       <c r="B374" t="s">
+        <v>791</v>
+      </c>
+      <c r="C374" t="s">
         <v>792</v>
-      </c>
-      <c r="C374" t="s">
-        <v>793</v>
       </c>
       <c r="D374" t="s">
         <v>19</v>
@@ -11945,10 +12005,10 @@
         <v>45996</v>
       </c>
       <c r="B375" t="s">
+        <v>793</v>
+      </c>
+      <c r="C375" t="s">
         <v>794</v>
-      </c>
-      <c r="C375" t="s">
-        <v>795</v>
       </c>
       <c r="D375" t="s">
         <v>22</v>
@@ -11968,10 +12028,10 @@
         <v>45996</v>
       </c>
       <c r="B376" t="s">
+        <v>795</v>
+      </c>
+      <c r="C376" t="s">
         <v>796</v>
-      </c>
-      <c r="C376" t="s">
-        <v>797</v>
       </c>
       <c r="D376" t="s">
         <v>9</v>
@@ -11991,10 +12051,10 @@
         <v>45997</v>
       </c>
       <c r="B377" t="s">
+        <v>797</v>
+      </c>
+      <c r="C377" t="s">
         <v>798</v>
-      </c>
-      <c r="C377" t="s">
-        <v>799</v>
       </c>
       <c r="D377" t="s">
         <v>19</v>
@@ -12014,10 +12074,10 @@
         <v>45997</v>
       </c>
       <c r="B378" t="s">
+        <v>799</v>
+      </c>
+      <c r="C378" t="s">
         <v>800</v>
-      </c>
-      <c r="C378" t="s">
-        <v>801</v>
       </c>
       <c r="D378" t="s">
         <v>22</v>
@@ -12037,10 +12097,10 @@
         <v>45997</v>
       </c>
       <c r="B379" t="s">
+        <v>801</v>
+      </c>
+      <c r="C379" t="s">
         <v>802</v>
-      </c>
-      <c r="C379" t="s">
-        <v>803</v>
       </c>
       <c r="D379" t="s">
         <v>6</v>
@@ -12060,10 +12120,10 @@
         <v>45997</v>
       </c>
       <c r="B380" t="s">
+        <v>803</v>
+      </c>
+      <c r="C380" t="s">
         <v>804</v>
-      </c>
-      <c r="C380" t="s">
-        <v>805</v>
       </c>
       <c r="D380" t="s">
         <v>11</v>
@@ -12083,10 +12143,10 @@
         <v>45997</v>
       </c>
       <c r="B381" t="s">
+        <v>805</v>
+      </c>
+      <c r="C381" t="s">
         <v>806</v>
-      </c>
-      <c r="C381" t="s">
-        <v>807</v>
       </c>
       <c r="D381" t="s">
         <v>10</v>
@@ -12106,10 +12166,10 @@
         <v>45997</v>
       </c>
       <c r="B382" t="s">
+        <v>807</v>
+      </c>
+      <c r="C382" t="s">
         <v>808</v>
-      </c>
-      <c r="C382" t="s">
-        <v>809</v>
       </c>
       <c r="D382" t="s">
         <v>19</v>
@@ -12129,10 +12189,10 @@
         <v>45997</v>
       </c>
       <c r="B383" t="s">
+        <v>809</v>
+      </c>
+      <c r="C383" t="s">
         <v>810</v>
-      </c>
-      <c r="C383" t="s">
-        <v>811</v>
       </c>
       <c r="D383" t="s">
         <v>10</v>
@@ -12152,10 +12212,10 @@
         <v>45997</v>
       </c>
       <c r="B384" t="s">
+        <v>811</v>
+      </c>
+      <c r="C384" t="s">
         <v>812</v>
-      </c>
-      <c r="C384" t="s">
-        <v>813</v>
       </c>
       <c r="D384" t="s">
         <v>22</v>
@@ -12175,10 +12235,10 @@
         <v>45997</v>
       </c>
       <c r="B385" t="s">
+        <v>813</v>
+      </c>
+      <c r="C385" t="s">
         <v>814</v>
-      </c>
-      <c r="C385" t="s">
-        <v>815</v>
       </c>
       <c r="D385" t="s">
         <v>19</v>
@@ -12198,10 +12258,10 @@
         <v>45997</v>
       </c>
       <c r="B386" t="s">
+        <v>815</v>
+      </c>
+      <c r="C386" t="s">
         <v>816</v>
-      </c>
-      <c r="C386" t="s">
-        <v>817</v>
       </c>
       <c r="D386" t="s">
         <v>19</v>
@@ -12221,10 +12281,10 @@
         <v>45997</v>
       </c>
       <c r="B387" t="s">
+        <v>817</v>
+      </c>
+      <c r="C387" t="s">
         <v>818</v>
-      </c>
-      <c r="C387" t="s">
-        <v>819</v>
       </c>
       <c r="D387" t="s">
         <v>26</v>
@@ -12244,10 +12304,10 @@
         <v>45997</v>
       </c>
       <c r="B388" t="s">
+        <v>819</v>
+      </c>
+      <c r="C388" t="s">
         <v>820</v>
-      </c>
-      <c r="C388" t="s">
-        <v>821</v>
       </c>
       <c r="D388" t="s">
         <v>26</v>
@@ -12267,10 +12327,10 @@
         <v>45997</v>
       </c>
       <c r="B389" t="s">
+        <v>821</v>
+      </c>
+      <c r="C389" t="s">
         <v>822</v>
-      </c>
-      <c r="C389" t="s">
-        <v>823</v>
       </c>
       <c r="D389" t="s">
         <v>10</v>
@@ -12290,10 +12350,10 @@
         <v>45997</v>
       </c>
       <c r="B390" t="s">
+        <v>823</v>
+      </c>
+      <c r="C390" t="s">
         <v>824</v>
-      </c>
-      <c r="C390" t="s">
-        <v>825</v>
       </c>
       <c r="D390" t="s">
         <v>10</v>
@@ -12313,10 +12373,10 @@
         <v>45997</v>
       </c>
       <c r="B391" t="s">
+        <v>825</v>
+      </c>
+      <c r="C391" t="s">
         <v>826</v>
-      </c>
-      <c r="C391" t="s">
-        <v>827</v>
       </c>
       <c r="D391" t="s">
         <v>22</v>
@@ -12336,10 +12396,10 @@
         <v>45997</v>
       </c>
       <c r="B392" t="s">
+        <v>827</v>
+      </c>
+      <c r="C392" t="s">
         <v>828</v>
-      </c>
-      <c r="C392" t="s">
-        <v>829</v>
       </c>
       <c r="D392" t="s">
         <v>10</v>
@@ -12359,10 +12419,10 @@
         <v>45997</v>
       </c>
       <c r="B393" t="s">
+        <v>829</v>
+      </c>
+      <c r="C393" t="s">
         <v>830</v>
-      </c>
-      <c r="C393" t="s">
-        <v>831</v>
       </c>
       <c r="D393" t="s">
         <v>22</v>
@@ -12382,10 +12442,10 @@
         <v>45997</v>
       </c>
       <c r="B394" t="s">
+        <v>831</v>
+      </c>
+      <c r="C394" t="s">
         <v>832</v>
-      </c>
-      <c r="C394" t="s">
-        <v>833</v>
       </c>
       <c r="D394" t="s">
         <v>11</v>
@@ -12405,10 +12465,10 @@
         <v>45997</v>
       </c>
       <c r="B395" t="s">
+        <v>833</v>
+      </c>
+      <c r="C395" t="s">
         <v>834</v>
-      </c>
-      <c r="C395" t="s">
-        <v>835</v>
       </c>
       <c r="D395" t="s">
         <v>19</v>
@@ -12428,10 +12488,10 @@
         <v>45997</v>
       </c>
       <c r="B396" t="s">
+        <v>835</v>
+      </c>
+      <c r="C396" t="s">
         <v>836</v>
-      </c>
-      <c r="C396" t="s">
-        <v>837</v>
       </c>
       <c r="D396" t="s">
         <v>22</v>
@@ -12451,10 +12511,10 @@
         <v>45997</v>
       </c>
       <c r="B397" t="s">
+        <v>837</v>
+      </c>
+      <c r="C397" t="s">
         <v>838</v>
-      </c>
-      <c r="C397" t="s">
-        <v>839</v>
       </c>
       <c r="D397" t="s">
         <v>22</v>
@@ -12474,10 +12534,10 @@
         <v>45999</v>
       </c>
       <c r="B398" t="s">
+        <v>839</v>
+      </c>
+      <c r="C398" t="s">
         <v>840</v>
-      </c>
-      <c r="C398" t="s">
-        <v>841</v>
       </c>
       <c r="D398" t="s">
         <v>9</v>
@@ -12497,10 +12557,10 @@
         <v>45999</v>
       </c>
       <c r="B399" t="s">
+        <v>841</v>
+      </c>
+      <c r="C399" t="s">
         <v>842</v>
-      </c>
-      <c r="C399" t="s">
-        <v>843</v>
       </c>
       <c r="D399" t="s">
         <v>20</v>
@@ -12520,10 +12580,10 @@
         <v>45999</v>
       </c>
       <c r="B400" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="C400" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D400" t="s">
         <v>17</v>
@@ -12534,16 +12594,19 @@
       <c r="F400" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>45999</v>
       </c>
       <c r="B401" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="C401" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D401" t="s">
         <v>17</v>
@@ -12554,16 +12617,19 @@
       <c r="F401" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G401">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>45999</v>
       </c>
       <c r="B402" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="C402" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D402" t="s">
         <v>17</v>
@@ -12574,16 +12640,19 @@
       <c r="F402" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G402">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>45999</v>
       </c>
       <c r="B403" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="C403" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D403" t="s">
         <v>18</v>
@@ -12592,18 +12661,21 @@
         <v>24</v>
       </c>
       <c r="F403" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G403">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>45999</v>
       </c>
       <c r="B404" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C404" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D404" t="s">
         <v>10</v>
@@ -12614,16 +12686,19 @@
       <c r="F404" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>45999</v>
       </c>
       <c r="B405" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C405" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D405" t="s">
         <v>22</v>
@@ -12634,16 +12709,19 @@
       <c r="F405" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G405">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>45999</v>
       </c>
       <c r="B406" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="C406" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D406" t="s">
         <v>18</v>
@@ -12654,16 +12732,19 @@
       <c r="F406" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G406">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>45999</v>
       </c>
       <c r="B407" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C407" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D407" t="s">
         <v>22</v>
@@ -12674,16 +12755,19 @@
       <c r="F407" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G407">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>45999</v>
       </c>
       <c r="B408" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="C408" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D408" t="s">
         <v>16</v>
@@ -12694,16 +12778,19 @@
       <c r="F408" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G408">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>45999</v>
       </c>
       <c r="B409" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C409" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D409" t="s">
         <v>20</v>
@@ -12712,18 +12799,21 @@
         <v>7</v>
       </c>
       <c r="F409" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G409">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>45999</v>
       </c>
       <c r="B410" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="C410" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D410" t="s">
         <v>9</v>
@@ -12734,16 +12824,19 @@
       <c r="F410" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G410">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>45999</v>
       </c>
       <c r="B411" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C411" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="D411" t="s">
         <v>10</v>
@@ -12754,16 +12847,19 @@
       <c r="F411" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G411">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>45999</v>
       </c>
       <c r="B412" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C412" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D412" t="s">
         <v>10</v>
@@ -12774,16 +12870,19 @@
       <c r="F412" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>45999</v>
       </c>
       <c r="B413" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C413" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D413" t="s">
         <v>20</v>
@@ -12794,16 +12893,19 @@
       <c r="F413" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G413">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>45999</v>
       </c>
       <c r="B414" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C414" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D414" t="s">
         <v>17</v>
@@ -12814,16 +12916,19 @@
       <c r="F414" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G414">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>45999</v>
       </c>
       <c r="B415" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C415" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="D415" t="s">
         <v>6</v>
@@ -12834,16 +12939,19 @@
       <c r="F415" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G415">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>45999</v>
       </c>
       <c r="B416" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C416" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="D416" t="s">
         <v>16</v>
@@ -12854,16 +12962,19 @@
       <c r="F416" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G416">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>45999</v>
       </c>
       <c r="B417" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C417" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D417" t="s">
         <v>22</v>
@@ -12874,16 +12985,19 @@
       <c r="F417" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G417">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>45999</v>
       </c>
       <c r="B418" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C418" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="D418" t="s">
         <v>17</v>
@@ -12894,16 +13008,19 @@
       <c r="F418" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G418">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>45999</v>
       </c>
       <c r="B419" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C419" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="D419" t="s">
         <v>13</v>
@@ -12914,16 +13031,19 @@
       <c r="F419" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G419">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>45999</v>
       </c>
       <c r="B420" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="C420" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="D420" t="s">
         <v>19</v>
@@ -12934,16 +13054,19 @@
       <c r="F420" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G420">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>45999</v>
       </c>
       <c r="B421" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="C421" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D421" t="s">
         <v>9</v>
@@ -12954,16 +13077,19 @@
       <c r="F421" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G421">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>45999</v>
       </c>
       <c r="B422" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C422" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D422" t="s">
         <v>17</v>
@@ -12974,16 +13100,19 @@
       <c r="F422" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G422">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>45999</v>
       </c>
       <c r="B423" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C423" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D423" t="s">
         <v>16</v>
@@ -12994,16 +13123,19 @@
       <c r="F423" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G423">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>45999</v>
       </c>
       <c r="B424" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C424" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D424" t="s">
         <v>10</v>
@@ -13012,18 +13144,21 @@
         <v>7</v>
       </c>
       <c r="F424" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G424">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>45999</v>
       </c>
       <c r="B425" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C425" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D425" t="s">
         <v>22</v>
@@ -13034,16 +13169,19 @@
       <c r="F425" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G425">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>45999</v>
       </c>
       <c r="B426" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C426" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="D426" t="s">
         <v>10</v>
@@ -13054,16 +13192,19 @@
       <c r="F426" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G426">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>45999</v>
       </c>
       <c r="B427" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="C427" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D427" t="s">
         <v>17</v>
@@ -13074,16 +13215,19 @@
       <c r="F427" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G427">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>45999</v>
       </c>
       <c r="B428" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C428" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="D428" t="s">
         <v>6</v>
@@ -13094,16 +13238,19 @@
       <c r="F428" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G428">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>45999</v>
       </c>
       <c r="B429" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C429" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D429" t="s">
         <v>16</v>
@@ -13114,16 +13261,19 @@
       <c r="F429" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G429">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>45999</v>
       </c>
       <c r="B430" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C430" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D430" t="s">
         <v>18</v>
@@ -13134,16 +13284,19 @@
       <c r="F430" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G430">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>45999</v>
       </c>
       <c r="B431" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C431" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D431" t="s">
         <v>9</v>
@@ -13154,16 +13307,19 @@
       <c r="F431" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G431">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>45999</v>
       </c>
       <c r="B432" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C432" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D432" t="s">
         <v>25</v>
@@ -13174,16 +13330,19 @@
       <c r="F432" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G432">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>45999</v>
       </c>
       <c r="B433" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C433" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D433" t="s">
         <v>17</v>
@@ -13194,16 +13353,19 @@
       <c r="F433" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G433">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>45999</v>
       </c>
       <c r="B434" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C434" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D434" t="s">
         <v>19</v>
@@ -13214,16 +13376,19 @@
       <c r="F434" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>45999</v>
       </c>
       <c r="B435" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C435" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="D435" t="s">
         <v>10</v>
@@ -13234,16 +13399,19 @@
       <c r="F435" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>45999</v>
       </c>
       <c r="B436" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C436" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D436" t="s">
         <v>11</v>
@@ -13254,16 +13422,19 @@
       <c r="F436" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G436">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="437" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>45999</v>
       </c>
       <c r="B437" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C437" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D437" t="s">
         <v>17</v>
@@ -13274,16 +13445,19 @@
       <c r="F437" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G437">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="438" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>45999</v>
       </c>
       <c r="B438" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="C438" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D438" t="s">
         <v>10</v>
@@ -13294,16 +13468,19 @@
       <c r="F438" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G438">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="439" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>45999</v>
       </c>
       <c r="B439" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C439" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D439" t="s">
         <v>9</v>
@@ -13314,16 +13491,19 @@
       <c r="F439" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G439">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>45999</v>
       </c>
       <c r="B440" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C440" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D440" t="s">
         <v>22</v>
@@ -13332,18 +13512,21 @@
         <v>7</v>
       </c>
       <c r="F440" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G440">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>45999</v>
       </c>
       <c r="B441" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="C441" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D441" t="s">
         <v>6</v>
@@ -13354,16 +13537,19 @@
       <c r="F441" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G441">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>45999</v>
       </c>
       <c r="B442" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="C442" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D442" t="s">
         <v>22</v>
@@ -13374,16 +13560,19 @@
       <c r="F442" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G442">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>45999</v>
       </c>
       <c r="B443" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="C443" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D443" t="s">
         <v>19</v>
@@ -13394,16 +13583,19 @@
       <c r="F443" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <v>45999</v>
       </c>
       <c r="B444" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C444" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D444" t="s">
         <v>22</v>
@@ -13414,16 +13606,19 @@
       <c r="F444" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G444">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>45999</v>
       </c>
       <c r="B445" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="C445" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D445" t="s">
         <v>10</v>
@@ -13434,16 +13629,19 @@
       <c r="F445" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G445">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>45999</v>
       </c>
       <c r="B446" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="C446" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="D446" t="s">
         <v>17</v>
@@ -13454,16 +13652,19 @@
       <c r="F446" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G446">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <v>45999</v>
       </c>
       <c r="B447" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="C447" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D447" t="s">
         <v>25</v>
@@ -13474,16 +13675,19 @@
       <c r="F447" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G447">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="448" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <v>45999</v>
       </c>
       <c r="B448" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C448" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D448" t="s">
         <v>16</v>
@@ -13494,16 +13698,19 @@
       <c r="F448" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G448">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="449" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>45999</v>
       </c>
       <c r="B449" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C449" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D449" t="s">
         <v>10</v>
@@ -13512,18 +13719,21 @@
         <v>382</v>
       </c>
       <c r="F449" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G449">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>45999</v>
       </c>
       <c r="B450" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="C450" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D450" t="s">
         <v>18</v>
@@ -13534,16 +13744,19 @@
       <c r="F450" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G450">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <v>45999</v>
       </c>
       <c r="B451" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C451" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D451" t="s">
         <v>26</v>
@@ -13554,16 +13767,19 @@
       <c r="F451" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G451">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <v>45999</v>
       </c>
       <c r="B452" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="C452" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D452" t="s">
         <v>17</v>
@@ -13574,16 +13790,19 @@
       <c r="F452" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G452">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>45999</v>
       </c>
       <c r="B453" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="C453" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D453" t="s">
         <v>26</v>
@@ -13594,16 +13813,19 @@
       <c r="F453" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G453">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>45999</v>
       </c>
       <c r="B454" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C454" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="D454" t="s">
         <v>11</v>
@@ -13614,16 +13836,19 @@
       <c r="F454" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>45999</v>
       </c>
       <c r="B455" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C455" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D455" t="s">
         <v>19</v>
@@ -13634,16 +13859,19 @@
       <c r="F455" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G455">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>45999</v>
       </c>
       <c r="B456" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C456" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="D456" t="s">
         <v>10</v>
@@ -13654,16 +13882,19 @@
       <c r="F456" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G456">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>45999</v>
       </c>
       <c r="B457" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C457" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="D457" t="s">
         <v>26</v>
@@ -13674,16 +13905,19 @@
       <c r="F457" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>45999</v>
       </c>
       <c r="B458" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C458" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D458" t="s">
         <v>25</v>
@@ -13694,16 +13928,19 @@
       <c r="F458" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G458">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>45999</v>
       </c>
       <c r="B459" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="C459" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="D459" t="s">
         <v>13</v>
@@ -13712,18 +13949,21 @@
         <v>7</v>
       </c>
       <c r="F459" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G459">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="460" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>45999</v>
       </c>
       <c r="B460" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C460" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="D460" t="s">
         <v>22</v>
@@ -13734,16 +13974,19 @@
       <c r="F460" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>45999</v>
       </c>
       <c r="B461" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C461" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="D461" t="s">
         <v>6</v>
@@ -13754,16 +13997,19 @@
       <c r="F461" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G461">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>45999</v>
       </c>
       <c r="B462" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C462" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D462" t="s">
         <v>6</v>
@@ -13774,16 +14020,19 @@
       <c r="F462" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G462">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>45999</v>
       </c>
       <c r="B463" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="C463" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D463" t="s">
         <v>6</v>
@@ -13793,6 +14042,239 @@
       </c>
       <c r="F463" t="s">
         <v>56</v>
+      </c>
+      <c r="G463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A464" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B464" t="s">
+        <v>970</v>
+      </c>
+      <c r="C464" t="s">
+        <v>971</v>
+      </c>
+      <c r="D464" t="s">
+        <v>6</v>
+      </c>
+      <c r="E464" t="s">
+        <v>7</v>
+      </c>
+      <c r="F464" t="s">
+        <v>15</v>
+      </c>
+      <c r="G464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A465" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B465" t="s">
+        <v>972</v>
+      </c>
+      <c r="C465" t="s">
+        <v>973</v>
+      </c>
+      <c r="D465" t="s">
+        <v>16</v>
+      </c>
+      <c r="E465" t="s">
+        <v>7</v>
+      </c>
+      <c r="F465" t="s">
+        <v>15</v>
+      </c>
+      <c r="G465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A466" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B466" t="s">
+        <v>974</v>
+      </c>
+      <c r="C466" t="s">
+        <v>975</v>
+      </c>
+      <c r="D466" t="s">
+        <v>9</v>
+      </c>
+      <c r="E466" t="s">
+        <v>7</v>
+      </c>
+      <c r="F466" t="s">
+        <v>15</v>
+      </c>
+      <c r="G466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A467" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B467" t="s">
+        <v>976</v>
+      </c>
+      <c r="C467" t="s">
+        <v>977</v>
+      </c>
+      <c r="D467" t="s">
+        <v>13</v>
+      </c>
+      <c r="E467" t="s">
+        <v>7</v>
+      </c>
+      <c r="F467" t="s">
+        <v>15</v>
+      </c>
+      <c r="G467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A468" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B468" t="s">
+        <v>978</v>
+      </c>
+      <c r="C468" t="s">
+        <v>979</v>
+      </c>
+      <c r="D468" t="s">
+        <v>287</v>
+      </c>
+      <c r="E468" t="s">
+        <v>24</v>
+      </c>
+      <c r="F468" t="s">
+        <v>15</v>
+      </c>
+      <c r="G468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A469" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B469" t="s">
+        <v>980</v>
+      </c>
+      <c r="C469" t="s">
+        <v>981</v>
+      </c>
+      <c r="D469" t="s">
+        <v>13</v>
+      </c>
+      <c r="E469" t="s">
+        <v>7</v>
+      </c>
+      <c r="F469" t="s">
+        <v>15</v>
+      </c>
+      <c r="G469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A470" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B470" t="s">
+        <v>982</v>
+      </c>
+      <c r="C470" t="s">
+        <v>983</v>
+      </c>
+      <c r="D470" t="s">
+        <v>22</v>
+      </c>
+      <c r="E470" t="s">
+        <v>7</v>
+      </c>
+      <c r="F470" t="s">
+        <v>15</v>
+      </c>
+      <c r="G470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A471" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B471" t="s">
+        <v>984</v>
+      </c>
+      <c r="C471" t="s">
+        <v>985</v>
+      </c>
+      <c r="D471" t="s">
+        <v>20</v>
+      </c>
+      <c r="E471" t="s">
+        <v>7</v>
+      </c>
+      <c r="F471" t="s">
+        <v>15</v>
+      </c>
+      <c r="G471">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A472" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B472" t="s">
+        <v>986</v>
+      </c>
+      <c r="C472" t="s">
+        <v>987</v>
+      </c>
+      <c r="D472" t="s">
+        <v>178</v>
+      </c>
+      <c r="E472" t="s">
+        <v>24</v>
+      </c>
+      <c r="F472" t="s">
+        <v>15</v>
+      </c>
+      <c r="G472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A473" s="1">
+        <v>46000</v>
+      </c>
+      <c r="B473" t="s">
+        <v>988</v>
+      </c>
+      <c r="C473" t="s">
+        <v>989</v>
+      </c>
+      <c r="D473" t="s">
+        <v>178</v>
+      </c>
+      <c r="E473" t="s">
+        <v>24</v>
+      </c>
+      <c r="F473" t="s">
+        <v>15</v>
+      </c>
+      <c r="G473">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated balde and producao - base 12/12/2025
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2025-12.xlsx
+++ b/first-atlas/producao_2025-12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE76DF2B-4B6A-40D5-A8A2-EFD0A953EE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FEF277-1EE4-4682-982F-21FFF01B112E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="1830" windowWidth="20730" windowHeight="11160" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="1336">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -3629,9 +3629,6 @@
     <t>60739590000109</t>
   </si>
   <si>
-    <t>D S</t>
-  </si>
-  <si>
     <t>Documento de identificacao pois o apresentado estava ilegivel</t>
   </si>
   <si>
@@ -3642,6 +3639,414 @@
   </si>
   <si>
     <t>Requerimento de Empresario, atualizado e registrado no orgao competente</t>
+  </si>
+  <si>
+    <t>LEIDY RUBENS DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>DEJANIRA SILVA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>24844228000126</t>
+  </si>
+  <si>
+    <t>HLG TEC LIMA CLIMATIZACAO LTDA</t>
+  </si>
+  <si>
+    <t>42400338000180</t>
+  </si>
+  <si>
+    <t>FISH MAR PESCADOS LTDA</t>
+  </si>
+  <si>
+    <t>63988850000160</t>
+  </si>
+  <si>
+    <t>AMARANTE CORRESPONDENTE BANCARIO E SEGUROS LTDA</t>
+  </si>
+  <si>
+    <t>12262621000122</t>
+  </si>
+  <si>
+    <t>ELETROTERM AUTOMACAO INDUSTRIAL LTDA</t>
+  </si>
+  <si>
+    <t>29589177000157</t>
+  </si>
+  <si>
+    <t>COMERCIAL SERVE BEM LTDA</t>
+  </si>
+  <si>
+    <t>26493579000165</t>
+  </si>
+  <si>
+    <t>ZELI FERNANDES DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>63983851000111</t>
+  </si>
+  <si>
+    <t>BRAGA SILVA &amp; CAYRES SERVICOS E COMERCIO LTDA</t>
+  </si>
+  <si>
+    <t>38031801000197</t>
+  </si>
+  <si>
+    <t>DANIELLY LIMA PESSOA SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>05243832000152</t>
+  </si>
+  <si>
+    <t>SANTOS &amp; AMORIM LTDA</t>
+  </si>
+  <si>
+    <t>22452930000119</t>
+  </si>
+  <si>
+    <t>ALVO PROJETOS E TOPOGRAFIA LTDA</t>
+  </si>
+  <si>
+    <t>22282295000179</t>
+  </si>
+  <si>
+    <t>CLEYTON APARECIDO BATISTA DE REZENDE LTDA</t>
+  </si>
+  <si>
+    <t>45814224000175</t>
+  </si>
+  <si>
+    <t>IZABEL CRISTINA DOMINGOS DOS SANTOS LTDA</t>
+  </si>
+  <si>
+    <t>13638240000168</t>
+  </si>
+  <si>
+    <t>ESSENCIAL HIGIENIZACAO LIMPEZA DE ESTOFADOS LTDA</t>
+  </si>
+  <si>
+    <t>33697390000150</t>
+  </si>
+  <si>
+    <t>DAVID MELO DOS SANTOS</t>
+  </si>
+  <si>
+    <t>26751053000138</t>
+  </si>
+  <si>
+    <t>CASA BELLA EVENTOS</t>
+  </si>
+  <si>
+    <t>27907865000192</t>
+  </si>
+  <si>
+    <t>MARCOS SIDNEI GONCALVES DOURADO</t>
+  </si>
+  <si>
+    <t>26194207000138</t>
+  </si>
+  <si>
+    <t>26.194.207 FERNANDO RODRIGUES FARIA DA SILVA</t>
+  </si>
+  <si>
+    <t>33238405000111</t>
+  </si>
+  <si>
+    <t>BELLA PIZZA DA CIENE LTDA</t>
+  </si>
+  <si>
+    <t>14503382000180</t>
+  </si>
+  <si>
+    <t>BALBINO &amp; BALBINO LTDA</t>
+  </si>
+  <si>
+    <t>24574454000134</t>
+  </si>
+  <si>
+    <t>PRANTE LOCACOES E TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>32063316000119</t>
+  </si>
+  <si>
+    <t>ROMILDA MARGRAF KAPP</t>
+  </si>
+  <si>
+    <t>63618198000191</t>
+  </si>
+  <si>
+    <t>OZ BURGER &amp; STEAKE HOUSE LTDA</t>
+  </si>
+  <si>
+    <t>13877533000106</t>
+  </si>
+  <si>
+    <t>TRINO OFFSHORE RECURSOS HUMANOS</t>
+  </si>
+  <si>
+    <t>63482238000110</t>
+  </si>
+  <si>
+    <t>R. THIESEN DE OLIVEIRA JUNIOR E CIA LTDA</t>
+  </si>
+  <si>
+    <t>29223324000170</t>
+  </si>
+  <si>
+    <t>29.223.324 BIANCA PAGANO PEREIRA</t>
+  </si>
+  <si>
+    <t>63974503000188</t>
+  </si>
+  <si>
+    <t>BRIDIS COMUNICACAO VISUAL LTDA</t>
+  </si>
+  <si>
+    <t>63078610000128</t>
+  </si>
+  <si>
+    <t>PASTELOUCOS LTDA</t>
+  </si>
+  <si>
+    <t>63511005000107</t>
+  </si>
+  <si>
+    <t>LODN COMERCIO DE ALIMENTOS LTDA</t>
+  </si>
+  <si>
+    <t>17015024000117</t>
+  </si>
+  <si>
+    <t>17.015.024 EDUARDO FERDINANDO GALESSO</t>
+  </si>
+  <si>
+    <t>59908990000103</t>
+  </si>
+  <si>
+    <t>DIMENSONAL ENGENHARIA LTDA</t>
+  </si>
+  <si>
+    <t>60025588000160</t>
+  </si>
+  <si>
+    <t>ADONAI TOPOGRAFIA LTDA</t>
+  </si>
+  <si>
+    <t>20318084000113</t>
+  </si>
+  <si>
+    <t>NSM GOMES COMERCIO DE BEBIDAS LTDA</t>
+  </si>
+  <si>
+    <t>24445756000102</t>
+  </si>
+  <si>
+    <t>CENTRO DIGITAL TECNOLOGIA LTDA</t>
+  </si>
+  <si>
+    <t>21260665000104</t>
+  </si>
+  <si>
+    <t>RPH TRANSPORTES LTDA</t>
+  </si>
+  <si>
+    <t>21099487000181</t>
+  </si>
+  <si>
+    <t>FABIO ROMULO MORAIS MODESTO</t>
+  </si>
+  <si>
+    <t>21437326000150</t>
+  </si>
+  <si>
+    <t>RAFAEL HENRIQUE MARTARELLO DE ALMEIDA</t>
+  </si>
+  <si>
+    <t>14540239000169</t>
+  </si>
+  <si>
+    <t>I L P VIEIRA NUTRICAO</t>
+  </si>
+  <si>
+    <t>20925658000111</t>
+  </si>
+  <si>
+    <t>JUNIO DA SILVA CARDOSO</t>
+  </si>
+  <si>
+    <t>28058339000168</t>
+  </si>
+  <si>
+    <t>RIBABOM SERVICOS COMBINADOS DE NEGOCIOS LTDA</t>
+  </si>
+  <si>
+    <t>28993151000107</t>
+  </si>
+  <si>
+    <t>A C DE OLIVEIRA HENRIQUES COMERCIO VAREJISTA DE DOCES</t>
+  </si>
+  <si>
+    <t>33967805000168</t>
+  </si>
+  <si>
+    <t>MMR TRANSPORTE LTDA</t>
+  </si>
+  <si>
+    <t>34418174000190</t>
+  </si>
+  <si>
+    <t>ESTEVIN PECAS E MOTORES LTDA</t>
+  </si>
+  <si>
+    <t>54212751000109</t>
+  </si>
+  <si>
+    <t>WESLEY HUMBERTO GAMA SANTOS SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>34726304000152</t>
+  </si>
+  <si>
+    <t>D. F DE STEFANO LTDA</t>
+  </si>
+  <si>
+    <t>25289963000188</t>
+  </si>
+  <si>
+    <t>25.289.963 JOSE CLISSON CAVALCANTI SILVA</t>
+  </si>
+  <si>
+    <t>53179648000133</t>
+  </si>
+  <si>
+    <t>INDUSTRIA E COMERCIO DE CONFECCOES CASA BELLA LTDA</t>
+  </si>
+  <si>
+    <t>63520874000190</t>
+  </si>
+  <si>
+    <t>J.E SISTEMAS DE SEGURANCA LTDA</t>
+  </si>
+  <si>
+    <t>13248854000133</t>
+  </si>
+  <si>
+    <t>TERENCE FRANCA FERREIRA</t>
+  </si>
+  <si>
+    <t>34899572000176</t>
+  </si>
+  <si>
+    <t>ALYSON RUBENS DE FRANCA</t>
+  </si>
+  <si>
+    <t>63635978000140</t>
+  </si>
+  <si>
+    <t>JONATAS RIBEIRO LEITE</t>
+  </si>
+  <si>
+    <t>64006043000167</t>
+  </si>
+  <si>
+    <t>NEXION SISTEMAS LTDA</t>
+  </si>
+  <si>
+    <t>15179622000104</t>
+  </si>
+  <si>
+    <t>NORTAO ENERGIA LTDA</t>
+  </si>
+  <si>
+    <t>24385993000125</t>
+  </si>
+  <si>
+    <t>I M CAVALCANTE</t>
+  </si>
+  <si>
+    <t>63400813000199</t>
+  </si>
+  <si>
+    <t>AGRO JME LTDA</t>
+  </si>
+  <si>
+    <t>14752944000120</t>
+  </si>
+  <si>
+    <t>SAOLO PEREIRA LIMA</t>
+  </si>
+  <si>
+    <t>49064344000153</t>
+  </si>
+  <si>
+    <t>ARISTON A DOS SANTOS COMERCIO</t>
+  </si>
+  <si>
+    <t>13214749000183</t>
+  </si>
+  <si>
+    <t>SAULO BARBOSA RAMOS</t>
+  </si>
+  <si>
+    <t>29238155000142</t>
+  </si>
+  <si>
+    <t>CARLOS GOMES DA SILVA</t>
+  </si>
+  <si>
+    <t>12577280000184</t>
+  </si>
+  <si>
+    <t>LUXO INDUSTRIA DO VESTUARIO LTDA</t>
+  </si>
+  <si>
+    <t>Ricardo Cirino Mendes Caetano</t>
+  </si>
+  <si>
+    <t>61471222000187</t>
+  </si>
+  <si>
+    <t>FRANCISCO ELENVALDO DE SOUZA</t>
+  </si>
+  <si>
+    <t>30119450000169</t>
+  </si>
+  <si>
+    <t>28541062000120</t>
+  </si>
+  <si>
+    <t>DENISE DANIELI MARTINS DA ROCHA DOS REIS</t>
+  </si>
+  <si>
+    <t>26984726000108</t>
+  </si>
+  <si>
+    <t>A DINIZ DOS SANTOS TRANSPORTES</t>
+  </si>
+  <si>
+    <t>33440642000160</t>
+  </si>
+  <si>
+    <t>ALIVALDO GUIMARAES DE SOUZA</t>
+  </si>
+  <si>
+    <t>45251403000141</t>
+  </si>
+  <si>
+    <t>M SOUZA REPRESENTACOES LTDA</t>
+  </si>
+  <si>
+    <t>63817059000197</t>
+  </si>
+  <si>
+    <t>RAFAEL HENRIQUE PETTERSEN CONSULTORIA  GESTAO</t>
+  </si>
+  <si>
+    <t>Procuracao com poderes de abrir e movimentar conta corrente junto a instituicoes financeiras com mandato vigente e devidamente assinada&lt;br&gt;&lt;br&gt;Contrato Social atualizado e registrado no orgao competente</t>
+  </si>
+  <si>
+    <t>Procuracao com poderes de representacao junto a instituicoes financeiras podendo abrir e movimentar conta corrente com mandato vigente, assinada digitalmente GOV.br ou procuracao publica. Em caso de assinatura digital, devera ser encaminhado o documento em formato PDF.</t>
   </si>
 </sst>
 </file>
@@ -3683,7 +4088,218 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4013,10 +4629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCD3CE2-DBA2-4F4F-B6A3-11EE884EA727}">
-  <dimension ref="A1:G576"/>
+  <dimension ref="A1:G643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A553" workbookViewId="0">
-      <selection activeCell="F575" sqref="F575"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4318,7 +4934,7 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -9910,7 +10526,7 @@
         <v>536</v>
       </c>
       <c r="G256" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -11405,7 +12021,7 @@
         <v>536</v>
       </c>
       <c r="G321" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.25">
@@ -11724,7 +12340,7 @@
         <v>7</v>
       </c>
       <c r="F335" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="G335">
         <v>0</v>
@@ -15821,7 +16437,7 @@
         <v>536</v>
       </c>
       <c r="G513" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.25">
@@ -16140,10 +16756,10 @@
         <v>14</v>
       </c>
       <c r="F527" t="s">
-        <v>536</v>
-      </c>
-      <c r="G527" t="s">
-        <v>1200</v>
+        <v>15</v>
+      </c>
+      <c r="G527">
+        <v>0</v>
       </c>
     </row>
     <row r="528" spans="1:7" x14ac:dyDescent="0.25">
@@ -16163,10 +16779,10 @@
         <v>7</v>
       </c>
       <c r="F528" t="s">
-        <v>536</v>
-      </c>
-      <c r="G528" t="s">
-        <v>1200</v>
+        <v>15</v>
+      </c>
+      <c r="G528">
+        <v>0</v>
       </c>
     </row>
     <row r="529" spans="1:7" x14ac:dyDescent="0.25">
@@ -16332,25 +16948,25 @@
     </row>
     <row r="536" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A536" s="1">
-        <v>46001</v>
-      </c>
-      <c r="B536" t="s">
-        <v>1116</v>
+        <v>46000</v>
+      </c>
+      <c r="B536">
+        <v>30119450000169</v>
       </c>
       <c r="C536" t="s">
-        <v>1117</v>
+        <v>1200</v>
       </c>
       <c r="D536" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E536" t="s">
         <v>7</v>
       </c>
       <c r="F536" t="s">
-        <v>15</v>
-      </c>
-      <c r="G536">
-        <v>0</v>
+        <v>536</v>
+      </c>
+      <c r="G536" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="537" spans="1:7" x14ac:dyDescent="0.25">
@@ -16358,10 +16974,10 @@
         <v>46001</v>
       </c>
       <c r="B537" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C537" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D537" t="s">
         <v>17</v>
@@ -16381,13 +16997,13 @@
         <v>46001</v>
       </c>
       <c r="B538" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C538" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="D538" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E538" t="s">
         <v>7</v>
@@ -16404,10 +17020,10 @@
         <v>46001</v>
       </c>
       <c r="B539" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="C539" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D539" t="s">
         <v>10</v>
@@ -16427,13 +17043,13 @@
         <v>46001</v>
       </c>
       <c r="B540" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="C540" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D540" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E540" t="s">
         <v>7</v>
@@ -16450,16 +17066,16 @@
         <v>46001</v>
       </c>
       <c r="B541" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="C541" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="D541" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E541" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F541" t="s">
         <v>15</v>
@@ -16473,13 +17089,13 @@
         <v>46001</v>
       </c>
       <c r="B542" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="C542" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="D542" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E542" t="s">
         <v>24</v>
@@ -16496,19 +17112,19 @@
         <v>46001</v>
       </c>
       <c r="B543" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="C543" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D543" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E543" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F543" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G543">
         <v>0</v>
@@ -16519,19 +17135,19 @@
         <v>46001</v>
       </c>
       <c r="B544" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="C544" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="D544" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E544" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F544" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G544">
         <v>0</v>
@@ -16542,13 +17158,13 @@
         <v>46001</v>
       </c>
       <c r="B545" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="C545" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="D545" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E545" t="s">
         <v>7</v>
@@ -16565,16 +17181,16 @@
         <v>46001</v>
       </c>
       <c r="B546" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="C546" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="D546" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="E546" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F546" t="s">
         <v>15</v>
@@ -16588,16 +17204,16 @@
         <v>46001</v>
       </c>
       <c r="B547" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="C547" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="D547" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E547" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F547" t="s">
         <v>15</v>
@@ -16611,19 +17227,19 @@
         <v>46001</v>
       </c>
       <c r="B548" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="C548" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="D548" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E548" t="s">
         <v>7</v>
       </c>
       <c r="F548" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G548">
         <v>0</v>
@@ -16634,22 +17250,22 @@
         <v>46001</v>
       </c>
       <c r="B549" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="C549" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="D549" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E549" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F549" t="s">
-        <v>536</v>
-      </c>
-      <c r="G549" t="s">
-        <v>1200</v>
+        <v>8</v>
+      </c>
+      <c r="G549">
+        <v>0</v>
       </c>
     </row>
     <row r="550" spans="1:7" x14ac:dyDescent="0.25">
@@ -16657,22 +17273,22 @@
         <v>46001</v>
       </c>
       <c r="B550" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="C550" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="D550" t="s">
-        <v>1005</v>
+        <v>26</v>
       </c>
       <c r="E550" t="s">
         <v>14</v>
       </c>
       <c r="F550" t="s">
-        <v>536</v>
-      </c>
-      <c r="G550" t="s">
-        <v>1200</v>
+        <v>15</v>
+      </c>
+      <c r="G550">
+        <v>0</v>
       </c>
     </row>
     <row r="551" spans="1:7" x14ac:dyDescent="0.25">
@@ -16680,16 +17296,16 @@
         <v>46001</v>
       </c>
       <c r="B551" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="C551" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="D551" t="s">
-        <v>287</v>
+        <v>1005</v>
       </c>
       <c r="E551" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F551" t="s">
         <v>15</v>
@@ -16703,16 +17319,16 @@
         <v>46001</v>
       </c>
       <c r="B552" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="C552" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="D552" t="s">
-        <v>25</v>
+        <v>287</v>
       </c>
       <c r="E552" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F552" t="s">
         <v>15</v>
@@ -16726,16 +17342,16 @@
         <v>46001</v>
       </c>
       <c r="B553" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="C553" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="D553" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E553" t="s">
-        <v>462</v>
+        <v>7</v>
       </c>
       <c r="F553" t="s">
         <v>15</v>
@@ -16749,16 +17365,16 @@
         <v>46001</v>
       </c>
       <c r="B554" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C554" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="D554" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E554" t="s">
-        <v>7</v>
+        <v>462</v>
       </c>
       <c r="F554" t="s">
         <v>15</v>
@@ -16772,10 +17388,10 @@
         <v>46001</v>
       </c>
       <c r="B555" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="C555" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="D555" t="s">
         <v>16</v>
@@ -16795,22 +17411,22 @@
         <v>46001</v>
       </c>
       <c r="B556" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="C556" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="D556" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E556" t="s">
-        <v>382</v>
+        <v>7</v>
       </c>
       <c r="F556" t="s">
-        <v>546</v>
-      </c>
-      <c r="G556" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G556">
+        <v>0</v>
       </c>
     </row>
     <row r="557" spans="1:7" x14ac:dyDescent="0.25">
@@ -16818,22 +17434,22 @@
         <v>46001</v>
       </c>
       <c r="B557" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="C557" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="D557" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E557" t="s">
-        <v>7</v>
+        <v>382</v>
       </c>
       <c r="F557" t="s">
-        <v>15</v>
-      </c>
-      <c r="G557">
-        <v>0</v>
+        <v>546</v>
+      </c>
+      <c r="G557" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="558" spans="1:7" x14ac:dyDescent="0.25">
@@ -16841,16 +17457,16 @@
         <v>46001</v>
       </c>
       <c r="B558" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="C558" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="D558" t="s">
         <v>19</v>
       </c>
       <c r="E558" t="s">
-        <v>462</v>
+        <v>7</v>
       </c>
       <c r="F558" t="s">
         <v>15</v>
@@ -16864,19 +17480,19 @@
         <v>46001</v>
       </c>
       <c r="B559" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="C559" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="D559" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E559" t="s">
-        <v>382</v>
+        <v>462</v>
       </c>
       <c r="F559" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G559">
         <v>0</v>
@@ -16887,16 +17503,16 @@
         <v>46001</v>
       </c>
       <c r="B560" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="C560" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="D560" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E560" t="s">
-        <v>7</v>
+        <v>382</v>
       </c>
       <c r="F560" t="s">
         <v>15</v>
@@ -16910,13 +17526,13 @@
         <v>46001</v>
       </c>
       <c r="B561" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="C561" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="D561" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E561" t="s">
         <v>7</v>
@@ -16933,10 +17549,10 @@
         <v>46001</v>
       </c>
       <c r="B562" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="C562" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="D562" t="s">
         <v>17</v>
@@ -16945,7 +17561,7 @@
         <v>7</v>
       </c>
       <c r="F562" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="G562">
         <v>0</v>
@@ -16956,19 +17572,19 @@
         <v>46001</v>
       </c>
       <c r="B563" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="C563" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="D563" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E563" t="s">
         <v>7</v>
       </c>
       <c r="F563" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="G563">
         <v>0</v>
@@ -16976,16 +17592,16 @@
     </row>
     <row r="564" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A564" s="1">
-        <v>46002</v>
+        <v>46001</v>
       </c>
       <c r="B564" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="C564" t="s">
-        <v>1002</v>
+        <v>1171</v>
       </c>
       <c r="D564" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E564" t="s">
         <v>7</v>
@@ -17002,13 +17618,13 @@
         <v>46002</v>
       </c>
       <c r="B565" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C565" t="s">
-        <v>1174</v>
+        <v>1002</v>
       </c>
       <c r="D565" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E565" t="s">
         <v>7</v>
@@ -17025,16 +17641,16 @@
         <v>46002</v>
       </c>
       <c r="B566" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="C566" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="D566" t="s">
-        <v>178</v>
+        <v>6</v>
       </c>
       <c r="E566" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F566" t="s">
         <v>15</v>
@@ -17048,10 +17664,10 @@
         <v>46002</v>
       </c>
       <c r="B567" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="C567" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="D567" t="s">
         <v>178</v>
@@ -17071,16 +17687,16 @@
         <v>46002</v>
       </c>
       <c r="B568" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="C568" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="D568" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="E568" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F568" t="s">
         <v>15</v>
@@ -17094,19 +17710,22 @@
         <v>46002</v>
       </c>
       <c r="B569" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="C569" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="D569" t="s">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="E569" t="s">
-        <v>186</v>
+        <v>7</v>
       </c>
       <c r="F569" t="s">
         <v>15</v>
+      </c>
+      <c r="G569">
+        <v>0</v>
       </c>
     </row>
     <row r="570" spans="1:7" x14ac:dyDescent="0.25">
@@ -17114,10 +17733,10 @@
         <v>46002</v>
       </c>
       <c r="B570" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="C570" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="D570" t="s">
         <v>185</v>
@@ -17127,6 +17746,9 @@
       </c>
       <c r="F570" t="s">
         <v>15</v>
+      </c>
+      <c r="G570">
+        <v>0</v>
       </c>
     </row>
     <row r="571" spans="1:7" x14ac:dyDescent="0.25">
@@ -17134,10 +17756,10 @@
         <v>46002</v>
       </c>
       <c r="B571" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="C571" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="D571" t="s">
         <v>185</v>
@@ -17147,6 +17769,9 @@
       </c>
       <c r="F571" t="s">
         <v>15</v>
+      </c>
+      <c r="G571">
+        <v>0</v>
       </c>
     </row>
     <row r="572" spans="1:7" x14ac:dyDescent="0.25">
@@ -17154,10 +17779,10 @@
         <v>46002</v>
       </c>
       <c r="B572" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="C572" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="D572" t="s">
         <v>185</v>
@@ -17167,6 +17792,9 @@
       </c>
       <c r="F572" t="s">
         <v>15</v>
+      </c>
+      <c r="G572">
+        <v>0</v>
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.25">
@@ -17174,10 +17802,10 @@
         <v>46002</v>
       </c>
       <c r="B573" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="C573" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="D573" t="s">
         <v>185</v>
@@ -17187,6 +17815,9 @@
       </c>
       <c r="F573" t="s">
         <v>15</v>
+      </c>
+      <c r="G573">
+        <v>0</v>
       </c>
     </row>
     <row r="574" spans="1:7" x14ac:dyDescent="0.25">
@@ -17194,10 +17825,10 @@
         <v>46002</v>
       </c>
       <c r="B574" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C574" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="D574" t="s">
         <v>185</v>
@@ -17207,6 +17838,9 @@
       </c>
       <c r="F574" t="s">
         <v>15</v>
+      </c>
+      <c r="G574">
+        <v>0</v>
       </c>
     </row>
     <row r="575" spans="1:7" x14ac:dyDescent="0.25">
@@ -17214,10 +17848,10 @@
         <v>46002</v>
       </c>
       <c r="B575" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C575" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="D575" t="s">
         <v>185</v>
@@ -17227,6 +17861,9 @@
       </c>
       <c r="F575" t="s">
         <v>15</v>
+      </c>
+      <c r="G575">
+        <v>0</v>
       </c>
     </row>
     <row r="576" spans="1:7" x14ac:dyDescent="0.25">
@@ -17234,10 +17871,10 @@
         <v>46002</v>
       </c>
       <c r="B576" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C576" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="D576" t="s">
         <v>185</v>
@@ -17247,6 +17884,1550 @@
       </c>
       <c r="F576" t="s">
         <v>15</v>
+      </c>
+      <c r="G576">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="577" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A577" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B577" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C577" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D577" t="s">
+        <v>185</v>
+      </c>
+      <c r="E577" t="s">
+        <v>186</v>
+      </c>
+      <c r="F577" t="s">
+        <v>15</v>
+      </c>
+      <c r="G577">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="578" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A578" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B578" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C578" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D578" t="s">
+        <v>9</v>
+      </c>
+      <c r="E578" t="s">
+        <v>7</v>
+      </c>
+      <c r="F578" t="s">
+        <v>8</v>
+      </c>
+      <c r="G578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A579" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B579" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C579" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D579" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E579" t="s">
+        <v>14</v>
+      </c>
+      <c r="F579" t="s">
+        <v>536</v>
+      </c>
+      <c r="G579" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A580" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B580" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C580" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D580" t="s">
+        <v>11</v>
+      </c>
+      <c r="E580" t="s">
+        <v>24</v>
+      </c>
+      <c r="F580" t="s">
+        <v>56</v>
+      </c>
+      <c r="G580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A581" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B581" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C581" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D581" t="s">
+        <v>10</v>
+      </c>
+      <c r="E581" t="s">
+        <v>7</v>
+      </c>
+      <c r="F581" t="s">
+        <v>15</v>
+      </c>
+      <c r="G581">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A582" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B582" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C582" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D582" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E582" t="s">
+        <v>14</v>
+      </c>
+      <c r="F582" t="s">
+        <v>8</v>
+      </c>
+      <c r="G582">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="583" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A583" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B583" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C583" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D583" t="s">
+        <v>26</v>
+      </c>
+      <c r="E583" t="s">
+        <v>14</v>
+      </c>
+      <c r="F583" t="s">
+        <v>15</v>
+      </c>
+      <c r="G583">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="584" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A584" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B584" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C584" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D584" t="s">
+        <v>16</v>
+      </c>
+      <c r="E584" t="s">
+        <v>24</v>
+      </c>
+      <c r="F584" t="s">
+        <v>56</v>
+      </c>
+      <c r="G584" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="585" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A585" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B585" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C585" t="s">
+        <v>1217</v>
+      </c>
+      <c r="D585" t="s">
+        <v>19</v>
+      </c>
+      <c r="E585" t="s">
+        <v>7</v>
+      </c>
+      <c r="F585" t="s">
+        <v>15</v>
+      </c>
+      <c r="G585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="586" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A586" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B586" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C586" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D586" t="s">
+        <v>16</v>
+      </c>
+      <c r="E586" t="s">
+        <v>7</v>
+      </c>
+      <c r="F586" t="s">
+        <v>56</v>
+      </c>
+      <c r="G586">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="587" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A587" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B587" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C587" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D587" t="s">
+        <v>13</v>
+      </c>
+      <c r="E587" t="s">
+        <v>7</v>
+      </c>
+      <c r="F587" t="s">
+        <v>15</v>
+      </c>
+      <c r="G587">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="588" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A588" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B588" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C588" t="s">
+        <v>1223</v>
+      </c>
+      <c r="D588" t="s">
+        <v>20</v>
+      </c>
+      <c r="E588" t="s">
+        <v>7</v>
+      </c>
+      <c r="F588" t="s">
+        <v>15</v>
+      </c>
+      <c r="G588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="589" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A589" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B589" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C589" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D589" t="s">
+        <v>26</v>
+      </c>
+      <c r="E589" t="s">
+        <v>14</v>
+      </c>
+      <c r="F589" t="s">
+        <v>15</v>
+      </c>
+      <c r="G589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A590" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B590" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C590" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D590" t="s">
+        <v>6</v>
+      </c>
+      <c r="E590" t="s">
+        <v>7</v>
+      </c>
+      <c r="F590" t="s">
+        <v>15</v>
+      </c>
+      <c r="G590">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="591" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A591" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B591" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C591" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D591" t="s">
+        <v>17</v>
+      </c>
+      <c r="E591" t="s">
+        <v>14</v>
+      </c>
+      <c r="F591" t="s">
+        <v>56</v>
+      </c>
+      <c r="G591">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="592" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A592" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B592" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C592" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D592" t="s">
+        <v>9</v>
+      </c>
+      <c r="E592" t="s">
+        <v>7</v>
+      </c>
+      <c r="F592" t="s">
+        <v>56</v>
+      </c>
+      <c r="G592" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="593" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A593" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B593" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C593" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D593" t="s">
+        <v>22</v>
+      </c>
+      <c r="E593" t="s">
+        <v>7</v>
+      </c>
+      <c r="F593" t="s">
+        <v>8</v>
+      </c>
+      <c r="G593">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="594" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A594" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B594" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C594" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D594" t="s">
+        <v>10</v>
+      </c>
+      <c r="E594" t="s">
+        <v>14</v>
+      </c>
+      <c r="F594" t="s">
+        <v>15</v>
+      </c>
+      <c r="G594">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="595" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A595" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B595" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C595" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D595" t="s">
+        <v>13</v>
+      </c>
+      <c r="E595" t="s">
+        <v>14</v>
+      </c>
+      <c r="F595" t="s">
+        <v>15</v>
+      </c>
+      <c r="G595">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="596" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A596" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B596" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C596" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D596" t="s">
+        <v>10</v>
+      </c>
+      <c r="E596" t="s">
+        <v>7</v>
+      </c>
+      <c r="F596" t="s">
+        <v>15</v>
+      </c>
+      <c r="G596">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="597" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A597" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B597" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C597" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D597" t="s">
+        <v>21</v>
+      </c>
+      <c r="E597" t="s">
+        <v>7</v>
+      </c>
+      <c r="F597" t="s">
+        <v>15</v>
+      </c>
+      <c r="G597">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="598" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A598" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B598" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C598" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D598" t="s">
+        <v>17</v>
+      </c>
+      <c r="E598" t="s">
+        <v>14</v>
+      </c>
+      <c r="F598" t="s">
+        <v>15</v>
+      </c>
+      <c r="G598">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="599" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A599" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B599" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C599" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D599" t="s">
+        <v>19</v>
+      </c>
+      <c r="E599" t="s">
+        <v>7</v>
+      </c>
+      <c r="F599" t="s">
+        <v>15</v>
+      </c>
+      <c r="G599">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A600" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B600" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C600" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D600" t="s">
+        <v>9</v>
+      </c>
+      <c r="E600" t="s">
+        <v>23</v>
+      </c>
+      <c r="F600" t="s">
+        <v>8</v>
+      </c>
+      <c r="G600">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A601" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B601" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C601" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D601" t="s">
+        <v>11</v>
+      </c>
+      <c r="E601" t="s">
+        <v>382</v>
+      </c>
+      <c r="F601" t="s">
+        <v>15</v>
+      </c>
+      <c r="G601">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A602" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B602" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C602" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D602" t="s">
+        <v>6</v>
+      </c>
+      <c r="E602" t="s">
+        <v>7</v>
+      </c>
+      <c r="F602" t="s">
+        <v>15</v>
+      </c>
+      <c r="G602">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="603" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A603" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B603" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C603" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D603" t="s">
+        <v>18</v>
+      </c>
+      <c r="E603" t="s">
+        <v>24</v>
+      </c>
+      <c r="F603" t="s">
+        <v>15</v>
+      </c>
+      <c r="G603">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A604" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B604" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C604" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D604" t="s">
+        <v>22</v>
+      </c>
+      <c r="E604" t="s">
+        <v>7</v>
+      </c>
+      <c r="F604" t="s">
+        <v>15</v>
+      </c>
+      <c r="G604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A605" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B605" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C605" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D605" t="s">
+        <v>609</v>
+      </c>
+      <c r="E605" t="s">
+        <v>462</v>
+      </c>
+      <c r="F605" t="s">
+        <v>15</v>
+      </c>
+      <c r="G605">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A606" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B606" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C606" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D606" t="s">
+        <v>26</v>
+      </c>
+      <c r="E606" t="s">
+        <v>14</v>
+      </c>
+      <c r="F606" t="s">
+        <v>15</v>
+      </c>
+      <c r="G606">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A607" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B607" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C607" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D607" t="s">
+        <v>10</v>
+      </c>
+      <c r="E607" t="s">
+        <v>7</v>
+      </c>
+      <c r="F607" t="s">
+        <v>15</v>
+      </c>
+      <c r="G607">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A608" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B608" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C608" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D608" t="s">
+        <v>16</v>
+      </c>
+      <c r="E608" t="s">
+        <v>462</v>
+      </c>
+      <c r="F608" t="s">
+        <v>15</v>
+      </c>
+      <c r="G608">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A609" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B609" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C609" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D609" t="s">
+        <v>6</v>
+      </c>
+      <c r="E609" t="s">
+        <v>7</v>
+      </c>
+      <c r="F609" t="s">
+        <v>15</v>
+      </c>
+      <c r="G609">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A610" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B610" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C610" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D610" t="s">
+        <v>26</v>
+      </c>
+      <c r="E610" t="s">
+        <v>14</v>
+      </c>
+      <c r="F610" t="s">
+        <v>15</v>
+      </c>
+      <c r="G610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A611" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B611" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C611" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D611" t="s">
+        <v>22</v>
+      </c>
+      <c r="E611" t="s">
+        <v>23</v>
+      </c>
+      <c r="F611" t="s">
+        <v>56</v>
+      </c>
+      <c r="G611">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="612" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A612" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B612" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C612" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D612" t="s">
+        <v>16</v>
+      </c>
+      <c r="E612" t="s">
+        <v>7</v>
+      </c>
+      <c r="F612" t="s">
+        <v>56</v>
+      </c>
+      <c r="G612">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A613" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B613" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C613" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D613" t="s">
+        <v>19</v>
+      </c>
+      <c r="E613" t="s">
+        <v>7</v>
+      </c>
+      <c r="F613" t="s">
+        <v>15</v>
+      </c>
+      <c r="G613">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="614" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A614" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B614" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C614" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D614" t="s">
+        <v>20</v>
+      </c>
+      <c r="E614" t="s">
+        <v>7</v>
+      </c>
+      <c r="F614" t="s">
+        <v>15</v>
+      </c>
+      <c r="G614">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A615" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B615" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C615" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D615" t="s">
+        <v>22</v>
+      </c>
+      <c r="E615" t="s">
+        <v>7</v>
+      </c>
+      <c r="F615" t="s">
+        <v>15</v>
+      </c>
+      <c r="G615">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="616" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A616" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B616" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C616" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D616" t="s">
+        <v>21</v>
+      </c>
+      <c r="E616" t="s">
+        <v>7</v>
+      </c>
+      <c r="F616" t="s">
+        <v>15</v>
+      </c>
+      <c r="G616">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="617" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A617" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B617" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C617" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D617" t="s">
+        <v>26</v>
+      </c>
+      <c r="E617" t="s">
+        <v>14</v>
+      </c>
+      <c r="F617" t="s">
+        <v>15</v>
+      </c>
+      <c r="G617">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="618" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A618" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B618" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C618" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D618" t="s">
+        <v>21</v>
+      </c>
+      <c r="E618" t="s">
+        <v>7</v>
+      </c>
+      <c r="F618" t="s">
+        <v>8</v>
+      </c>
+      <c r="G618">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A619" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B619" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C619" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D619" t="s">
+        <v>25</v>
+      </c>
+      <c r="E619" t="s">
+        <v>14</v>
+      </c>
+      <c r="F619" t="s">
+        <v>15</v>
+      </c>
+      <c r="G619">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A620" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B620" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C620" t="s">
+        <v>1287</v>
+      </c>
+      <c r="D620" t="s">
+        <v>21</v>
+      </c>
+      <c r="E620" t="s">
+        <v>7</v>
+      </c>
+      <c r="F620" t="s">
+        <v>15</v>
+      </c>
+      <c r="G620">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A621" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B621" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C621" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D621" t="s">
+        <v>22</v>
+      </c>
+      <c r="E621" t="s">
+        <v>23</v>
+      </c>
+      <c r="F621" t="s">
+        <v>15</v>
+      </c>
+      <c r="G621">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A622" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B622" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C622" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D622" t="s">
+        <v>13</v>
+      </c>
+      <c r="E622" t="s">
+        <v>7</v>
+      </c>
+      <c r="F622" t="s">
+        <v>536</v>
+      </c>
+      <c r="G622" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="623" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A623" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B623" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C623" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D623" t="s">
+        <v>6</v>
+      </c>
+      <c r="E623" t="s">
+        <v>7</v>
+      </c>
+      <c r="F623" t="s">
+        <v>536</v>
+      </c>
+      <c r="G623">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A624" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B624" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C624" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D624" t="s">
+        <v>287</v>
+      </c>
+      <c r="E624" t="s">
+        <v>24</v>
+      </c>
+      <c r="F624" t="s">
+        <v>15</v>
+      </c>
+      <c r="G624">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A625" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B625" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C625" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D625" t="s">
+        <v>22</v>
+      </c>
+      <c r="E625" t="s">
+        <v>7</v>
+      </c>
+      <c r="F625" t="s">
+        <v>536</v>
+      </c>
+      <c r="G625" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="626" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A626" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B626" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C626" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D626" t="s">
+        <v>22</v>
+      </c>
+      <c r="E626" t="s">
+        <v>7</v>
+      </c>
+      <c r="F626" t="s">
+        <v>15</v>
+      </c>
+      <c r="G626">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A627" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B627" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C627" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D627" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E627" t="s">
+        <v>7</v>
+      </c>
+      <c r="F627" t="s">
+        <v>536</v>
+      </c>
+      <c r="G627" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="628" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A628" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B628" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C628" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D628" t="s">
+        <v>11</v>
+      </c>
+      <c r="E628" t="s">
+        <v>24</v>
+      </c>
+      <c r="F628" t="s">
+        <v>15</v>
+      </c>
+      <c r="G628">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="629" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A629" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B629" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C629" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D629" t="s">
+        <v>22</v>
+      </c>
+      <c r="E629" t="s">
+        <v>7</v>
+      </c>
+      <c r="F629" t="s">
+        <v>15</v>
+      </c>
+      <c r="G629">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="630" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A630" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B630" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C630" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D630" t="s">
+        <v>6</v>
+      </c>
+      <c r="E630" t="s">
+        <v>7</v>
+      </c>
+      <c r="F630" t="s">
+        <v>15</v>
+      </c>
+      <c r="G630">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="631" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A631" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B631" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C631" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D631" t="s">
+        <v>19</v>
+      </c>
+      <c r="E631" t="s">
+        <v>7</v>
+      </c>
+      <c r="F631" t="s">
+        <v>15</v>
+      </c>
+      <c r="G631">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A632" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B632" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C632" t="s">
+        <v>1311</v>
+      </c>
+      <c r="D632" t="s">
+        <v>20</v>
+      </c>
+      <c r="E632" t="s">
+        <v>7</v>
+      </c>
+      <c r="F632" t="s">
+        <v>15</v>
+      </c>
+      <c r="G632">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A633" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B633" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C633" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D633" t="s">
+        <v>19</v>
+      </c>
+      <c r="E633" t="s">
+        <v>7</v>
+      </c>
+      <c r="F633" t="s">
+        <v>15</v>
+      </c>
+      <c r="G633">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A634" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B634" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C634" t="s">
+        <v>1315</v>
+      </c>
+      <c r="D634" t="s">
+        <v>21</v>
+      </c>
+      <c r="E634" t="s">
+        <v>7</v>
+      </c>
+      <c r="F634" t="s">
+        <v>15</v>
+      </c>
+      <c r="G634">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A635" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B635" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C635" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D635" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E635" t="s">
+        <v>14</v>
+      </c>
+      <c r="F635" t="s">
+        <v>15</v>
+      </c>
+      <c r="G635">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="636" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A636" s="1">
+        <v>46002</v>
+      </c>
+      <c r="B636" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C636" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D636" t="s">
+        <v>1320</v>
+      </c>
+      <c r="E636" t="s">
+        <v>462</v>
+      </c>
+      <c r="F636" t="s">
+        <v>15</v>
+      </c>
+      <c r="G636">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A637" s="1">
+        <v>46003</v>
+      </c>
+      <c r="B637" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C637" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D637" t="s">
+        <v>17</v>
+      </c>
+      <c r="E637" t="s">
+        <v>7</v>
+      </c>
+      <c r="F637" t="s">
+        <v>15</v>
+      </c>
+      <c r="G637">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A638" s="1">
+        <v>46003</v>
+      </c>
+      <c r="B638" t="s">
+        <v>1323</v>
+      </c>
+      <c r="C638" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D638" t="s">
+        <v>13</v>
+      </c>
+      <c r="E638" t="s">
+        <v>7</v>
+      </c>
+      <c r="F638" t="s">
+        <v>15</v>
+      </c>
+      <c r="G638">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A639" s="1">
+        <v>46003</v>
+      </c>
+      <c r="B639" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C639" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D639" t="s">
+        <v>19</v>
+      </c>
+      <c r="E639" t="s">
+        <v>7</v>
+      </c>
+      <c r="F639" t="s">
+        <v>15</v>
+      </c>
+      <c r="G639">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A640" s="1">
+        <v>46003</v>
+      </c>
+      <c r="B640" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C640" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D640" t="s">
+        <v>6</v>
+      </c>
+      <c r="E640" t="s">
+        <v>7</v>
+      </c>
+      <c r="F640" t="s">
+        <v>15</v>
+      </c>
+      <c r="G640">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A641" s="1">
+        <v>46003</v>
+      </c>
+      <c r="B641" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C641" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D641" t="s">
+        <v>10</v>
+      </c>
+      <c r="E641" t="s">
+        <v>7</v>
+      </c>
+      <c r="F641" t="s">
+        <v>15</v>
+      </c>
+      <c r="G641">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A642" s="1">
+        <v>46003</v>
+      </c>
+      <c r="B642" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C642" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D642" t="s">
+        <v>178</v>
+      </c>
+      <c r="E642" t="s">
+        <v>24</v>
+      </c>
+      <c r="F642" t="s">
+        <v>15</v>
+      </c>
+      <c r="G642">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="643" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A643" s="1">
+        <v>46003</v>
+      </c>
+      <c r="B643" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C643" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D643" t="s">
+        <v>11</v>
+      </c>
+      <c r="E643" t="s">
+        <v>24</v>
+      </c>
+      <c r="F643" t="s">
+        <v>15</v>
+      </c>
+      <c r="G643">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated balde and producao - base 22/12/2025
</commit_message>
<xml_diff>
--- a/first-atlas/producao_2025-12.xlsx
+++ b/first-atlas/producao_2025-12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augustoalmeida\Augusto\bots_comissionamento\bot_atlas\first-atlas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FD41D1-7EB7-4495-98C0-475E7850009B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E31A4F-F26A-4741-A2DA-711E87688F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{3FA0812B-7F53-402D-BAE5-61E81C02CB4E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5780" uniqueCount="2361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5887" uniqueCount="2405">
   <si>
     <t>DATA_BASE</t>
   </si>
@@ -7122,6 +7122,138 @@
   </si>
   <si>
     <t>Procuracao com poderes para abrir e movimentar contas, pois identificamos que a representacao da sua empresa deve ser em conjunto pelos representantes. O documento deve ser assinado pelos representantes legais nomeados no contrato social, assinada digitalmente GOV.br ou procuracao publica. Em caso de assinatura digital, devera ser encaminhado o documento em formato PDF, para validacao das assinaturas e protocolo de autenticidade.</t>
+  </si>
+  <si>
+    <t>10301287000143</t>
+  </si>
+  <si>
+    <t>MARCELO CHRISTIAN MARQUES</t>
+  </si>
+  <si>
+    <t>07759241000168</t>
+  </si>
+  <si>
+    <t>B&amp;B PRODUCOES LTDA</t>
+  </si>
+  <si>
+    <t>33263558000119</t>
+  </si>
+  <si>
+    <t>R M GONCALVES REPRESENTACAO COMERCIAL</t>
+  </si>
+  <si>
+    <t>08414679000177</t>
+  </si>
+  <si>
+    <t>FREDERICO SILVEIRA LEMOS</t>
+  </si>
+  <si>
+    <t>35900852000110</t>
+  </si>
+  <si>
+    <t>HONORATO RESTAURANTE E PESQUEIRO DO FORDAO LTDA</t>
+  </si>
+  <si>
+    <t>24584718000130</t>
+  </si>
+  <si>
+    <t>ELIS LOASSY DOS SANTOS MATUZALEM</t>
+  </si>
+  <si>
+    <t>26131125000144</t>
+  </si>
+  <si>
+    <t>26.131.125 VALCI DA SILVA</t>
+  </si>
+  <si>
+    <t>34298424000104</t>
+  </si>
+  <si>
+    <t>DANILO SILVA FERRAZ DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>60794846000172</t>
+  </si>
+  <si>
+    <t>ANDRIA ARAUJO SOCIEDADE INDIVIDUAL DE ADVOCACIA</t>
+  </si>
+  <si>
+    <t>31667040000115</t>
+  </si>
+  <si>
+    <t>ALESSANDRO SOUSA DA SILVA</t>
+  </si>
+  <si>
+    <t>24093319000177</t>
+  </si>
+  <si>
+    <t>SEBASTIANA APARECIDA DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>28505143000174</t>
+  </si>
+  <si>
+    <t>ELON FARIAS GONCALVES MECANICO DE VEICULOS AUTOMOTORES</t>
+  </si>
+  <si>
+    <t>33932076000104</t>
+  </si>
+  <si>
+    <t>FABRICIA LARA GODINHO</t>
+  </si>
+  <si>
+    <t>24728884000163</t>
+  </si>
+  <si>
+    <t>RICARDO DOS SANTOS FARIA</t>
+  </si>
+  <si>
+    <t>14428575000114</t>
+  </si>
+  <si>
+    <t>BRUNA PATRICIA DO ESPIRITO SANTO OLIVEIRA</t>
+  </si>
+  <si>
+    <t>33623254000115</t>
+  </si>
+  <si>
+    <t>J AGOSTINHO PIRES CONFECCOES</t>
+  </si>
+  <si>
+    <t>30312017000145</t>
+  </si>
+  <si>
+    <t>EDUARDO JOSE LIMA DE CARVALHO</t>
+  </si>
+  <si>
+    <t>24947011000141</t>
+  </si>
+  <si>
+    <t>CENTRO FONOAUDIOLOGICO JULIANA PETER LTDA</t>
+  </si>
+  <si>
+    <t>26202041000154</t>
+  </si>
+  <si>
+    <t>IMPERIO DA MODA LTDA</t>
+  </si>
+  <si>
+    <t>24864651000198</t>
+  </si>
+  <si>
+    <t>JOANIZIA TABOSA SOARES</t>
+  </si>
+  <si>
+    <t>30536365000104</t>
+  </si>
+  <si>
+    <t>LEONILDO AURELIANO DA SILVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procuracao com poderes para abrir e movimentar contas, pois identificamos que a representacao da sua empresa deve ser em conjunto pelos socios,  A procuracao deve ser assinada digitalmente pelos socios pela plataforma "GOV." e estar em formato PDF.&lt;br&gt;&lt;br&gt;Para garantir a seguranca e a validade do processo, Pedimos gentilmente que envie uma nova selfie, conforme as orientacoes </t>
+  </si>
+  <si>
+    <t>Procuracao com poderes de abrir e movimentar conta corrente junto a instituicoes financeiras com mandato vigente e devidamente assinada&lt;br&gt;&lt;br&gt;Requerimento de Empresario, atualizado e registrado no orgao competente</t>
   </si>
 </sst>
 </file>
@@ -7493,10 +7625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCD3CE2-DBA2-4F4F-B6A3-11EE884EA727}">
-  <dimension ref="A1:G1150"/>
+  <dimension ref="A1:G1171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8558,7 +8690,7 @@
         <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -9386,7 +9518,7 @@
         <v>14</v>
       </c>
       <c r="F82" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -11159,8 +11291,8 @@
       <c r="F159" t="s">
         <v>15</v>
       </c>
-      <c r="G159" t="e">
-        <v>#N/A</v>
+      <c r="G159">
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -13206,9 +13338,6 @@
       <c r="F248" t="s">
         <v>1935</v>
       </c>
-      <c r="G248" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
@@ -13342,7 +13471,7 @@
         <v>24</v>
       </c>
       <c r="F254" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="G254">
         <v>0</v>
@@ -13664,7 +13793,7 @@
         <v>7</v>
       </c>
       <c r="F268" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="G268">
         <v>0</v>
@@ -13919,9 +14048,6 @@
       <c r="F279" t="s">
         <v>1935</v>
       </c>
-      <c r="G279" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
@@ -15044,7 +15170,7 @@
         <v>7</v>
       </c>
       <c r="F328" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="G328">
         <v>0</v>
@@ -15205,10 +15331,10 @@
         <v>7</v>
       </c>
       <c r="F335" t="s">
-        <v>173</v>
-      </c>
-      <c r="G335">
-        <v>0</v>
+        <v>534</v>
+      </c>
+      <c r="G335" t="s">
+        <v>2403</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.25">
@@ -15320,7 +15446,7 @@
         <v>14</v>
       </c>
       <c r="F340" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="G340">
         <v>0</v>
@@ -18956,9 +19082,6 @@
       <c r="F498" t="s">
         <v>8</v>
       </c>
-      <c r="G498" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="499" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A499" s="1">
@@ -20267,9 +20390,6 @@
       <c r="F555" t="s">
         <v>1935</v>
       </c>
-      <c r="G555" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="556" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A556" s="1">
@@ -23119,9 +23239,6 @@
       <c r="F679" t="s">
         <v>1935</v>
       </c>
-      <c r="G679" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="680" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A680" s="1">
@@ -24223,9 +24340,6 @@
       <c r="F727" t="s">
         <v>8</v>
       </c>
-      <c r="G727" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A728" s="1">
@@ -27142,7 +27256,7 @@
         <v>24</v>
       </c>
       <c r="F854" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G854">
         <v>0</v>
@@ -28064,9 +28178,6 @@
       <c r="F894" t="s">
         <v>1935</v>
       </c>
-      <c r="G894" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="895" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A895" s="1">
@@ -28499,7 +28610,7 @@
         <v>7</v>
       </c>
       <c r="F913" t="s">
-        <v>534</v>
+        <v>12</v>
       </c>
       <c r="G913">
         <v>0</v>
@@ -28568,7 +28679,7 @@
         <v>7</v>
       </c>
       <c r="F916" t="s">
-        <v>173</v>
+        <v>12</v>
       </c>
       <c r="G916">
         <v>0</v>
@@ -29674,9 +29785,6 @@
       <c r="F964" t="s">
         <v>1935</v>
       </c>
-      <c r="G964" t="e">
-        <v>#N/A</v>
-      </c>
     </row>
     <row r="965" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A965" s="1">
@@ -31351,7 +31459,7 @@
         <v>23</v>
       </c>
       <c r="F1037" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G1037">
         <v>0</v>
@@ -32777,7 +32885,7 @@
         <v>7</v>
       </c>
       <c r="F1099" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="G1099">
         <v>0</v>
@@ -33099,10 +33207,7 @@
         <v>7</v>
       </c>
       <c r="F1113" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1113" t="e">
-        <v>#N/A</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="1114" spans="1:7" x14ac:dyDescent="0.25">
@@ -33191,7 +33296,7 @@
         <v>7</v>
       </c>
       <c r="F1117" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="G1117">
         <v>0</v>
@@ -33237,10 +33342,10 @@
         <v>14</v>
       </c>
       <c r="F1119" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1119" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G1119">
+        <v>0</v>
       </c>
     </row>
     <row r="1120" spans="1:7" x14ac:dyDescent="0.25">
@@ -33260,10 +33365,10 @@
         <v>14</v>
       </c>
       <c r="F1120" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1120" t="e">
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="G1120">
+        <v>0</v>
       </c>
     </row>
     <row r="1121" spans="1:7" x14ac:dyDescent="0.25">
@@ -33283,7 +33388,7 @@
         <v>7</v>
       </c>
       <c r="F1121" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="G1121">
         <v>0</v>
@@ -33559,10 +33664,7 @@
         <v>14</v>
       </c>
       <c r="F1133" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1133" t="e">
-        <v>#N/A</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="1134" spans="1:7" x14ac:dyDescent="0.25">
@@ -33743,7 +33845,7 @@
         <v>14</v>
       </c>
       <c r="F1141" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="G1141">
         <v>0</v>
@@ -33766,7 +33868,7 @@
         <v>24</v>
       </c>
       <c r="F1142" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="G1142">
         <v>0</v>
@@ -33789,7 +33891,7 @@
         <v>14</v>
       </c>
       <c r="F1143" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="G1143">
         <v>0</v>
@@ -33812,7 +33914,7 @@
         <v>14</v>
       </c>
       <c r="F1144" t="s">
-        <v>54</v>
+        <v>173</v>
       </c>
       <c r="G1144">
         <v>0</v>
@@ -33953,6 +34055,486 @@
         <v>15</v>
       </c>
       <c r="G1150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1151" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>2361</v>
+      </c>
+      <c r="C1151" t="s">
+        <v>2362</v>
+      </c>
+      <c r="D1151" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1151" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1151" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1152" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>2363</v>
+      </c>
+      <c r="C1152" t="s">
+        <v>2364</v>
+      </c>
+      <c r="D1152" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1152" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1152" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1153" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1153" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C1153" t="s">
+        <v>2366</v>
+      </c>
+      <c r="D1153" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E1153" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1153" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1154" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C1154" t="s">
+        <v>2368</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>2297</v>
+      </c>
+      <c r="E1154" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1154" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1155" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>2369</v>
+      </c>
+      <c r="C1155" t="s">
+        <v>2370</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>997</v>
+      </c>
+      <c r="E1155" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1155" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1156" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>2371</v>
+      </c>
+      <c r="C1156" t="s">
+        <v>2372</v>
+      </c>
+      <c r="D1156" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1156" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1156" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1157" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>2373</v>
+      </c>
+      <c r="C1157" t="s">
+        <v>2374</v>
+      </c>
+      <c r="D1157" t="s">
+        <v>2297</v>
+      </c>
+      <c r="E1157" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1157" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1158" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1158" t="s">
+        <v>2375</v>
+      </c>
+      <c r="C1158" t="s">
+        <v>2376</v>
+      </c>
+      <c r="D1158" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1158" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1158" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1159" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1159" t="s">
+        <v>2377</v>
+      </c>
+      <c r="C1159" t="s">
+        <v>2378</v>
+      </c>
+      <c r="D1159" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1159" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1159" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1160" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1160" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C1160" t="s">
+        <v>2380</v>
+      </c>
+      <c r="D1160" t="s">
+        <v>997</v>
+      </c>
+      <c r="E1160" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1160" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1161" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1161" t="s">
+        <v>2381</v>
+      </c>
+      <c r="C1161" t="s">
+        <v>2382</v>
+      </c>
+      <c r="D1161" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1161" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1161" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1162" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1162" t="s">
+        <v>2383</v>
+      </c>
+      <c r="C1162" t="s">
+        <v>2384</v>
+      </c>
+      <c r="D1162" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1162" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1163" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1163" t="s">
+        <v>2385</v>
+      </c>
+      <c r="C1163" t="s">
+        <v>2386</v>
+      </c>
+      <c r="D1163" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1163" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1163" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1164" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1164" t="s">
+        <v>2387</v>
+      </c>
+      <c r="C1164" t="s">
+        <v>2388</v>
+      </c>
+      <c r="D1164" t="s">
+        <v>997</v>
+      </c>
+      <c r="E1164" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1164" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1165" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1165" t="s">
+        <v>2389</v>
+      </c>
+      <c r="C1165" t="s">
+        <v>2390</v>
+      </c>
+      <c r="D1165" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E1165" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1165" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1166" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1166" t="s">
+        <v>2391</v>
+      </c>
+      <c r="C1166" t="s">
+        <v>2392</v>
+      </c>
+      <c r="D1166" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E1166" t="s">
+        <v>380</v>
+      </c>
+      <c r="F1166" t="s">
+        <v>534</v>
+      </c>
+      <c r="G1166" t="s">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1167" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1167" t="s">
+        <v>2393</v>
+      </c>
+      <c r="C1167" t="s">
+        <v>2394</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1167" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1167" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1168" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1168" t="s">
+        <v>2395</v>
+      </c>
+      <c r="C1168" t="s">
+        <v>2396</v>
+      </c>
+      <c r="D1168" t="s">
+        <v>997</v>
+      </c>
+      <c r="E1168" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1168" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1169" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1169" t="s">
+        <v>2397</v>
+      </c>
+      <c r="C1169" t="s">
+        <v>2398</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E1169" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1169" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1170" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>2399</v>
+      </c>
+      <c r="C1170" t="s">
+        <v>2400</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1170" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1171" s="1">
+        <v>46011</v>
+      </c>
+      <c r="B1171" t="s">
+        <v>2401</v>
+      </c>
+      <c r="C1171" t="s">
+        <v>2402</v>
+      </c>
+      <c r="D1171" t="s">
+        <v>997</v>
+      </c>
+      <c r="E1171" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1171" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1171">
         <v>0</v>
       </c>
     </row>

</xml_diff>